<commit_message>
Graphs for phenology and node numbers made. Cultivars TT targets adjusted.
</commit_message>
<xml_diff>
--- a/Prototypes/Mungbean/Exp3observed.xlsx
+++ b/Prototypes/Mungbean/Exp3observed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pas075\Documents\ApsimX\Prototypes\Mungbean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF76D180-08B4-4E15-AC0D-5812B2863746}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2422440E-FAA1-458C-8F3E-6C5DF929838C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3945" yWindow="1725" windowWidth="21600" windowHeight="11385" xr2:uid="{8C69385E-AA3F-4CF3-AF00-E1E4599E61EE}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8C69385E-AA3F-4CF3-AF00-E1E4599E61EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="1" r:id="rId1"/>
@@ -182,33 +182,6 @@
     <t>Soybean.Nodule.NFixed</t>
   </si>
   <si>
-    <t>exp3SowDec17Irr</t>
-  </si>
-  <si>
-    <t>exp3SowDec17RF</t>
-  </si>
-  <si>
-    <t>exp3SowDec17RO</t>
-  </si>
-  <si>
-    <t>exp3SowDec30Irr</t>
-  </si>
-  <si>
-    <t>exp3SowDec30RF</t>
-  </si>
-  <si>
-    <t>exp3SowDec30RO</t>
-  </si>
-  <si>
-    <t>exp3SowDec3Irr</t>
-  </si>
-  <si>
-    <t>exp3SowDec3RF</t>
-  </si>
-  <si>
-    <t>exp3SowDec3RO</t>
-  </si>
-  <si>
     <t>Soybean.Phenology.CurrentStageName</t>
   </si>
   <si>
@@ -216,6 +189,33 @@
   </si>
   <si>
     <t>Yield</t>
+  </si>
+  <si>
+    <t>exp3SowDec17IrrCultivarEmerald</t>
+  </si>
+  <si>
+    <t>exp3SowDec30IrrCultivarEmerald</t>
+  </si>
+  <si>
+    <t>exp3SowDec3IrrCultivarEmerald</t>
+  </si>
+  <si>
+    <t>exp3SowDec17RFCultivarEmerald</t>
+  </si>
+  <si>
+    <t>exp3SowDec30RFCultivarEmerald</t>
+  </si>
+  <si>
+    <t>exp3SowDec3RFCultivarEmerald</t>
+  </si>
+  <si>
+    <t>exp3SowDec17ROCultivarEmerald</t>
+  </si>
+  <si>
+    <t>exp3SowDec30ROCultivarEmerald</t>
+  </si>
+  <si>
+    <t>exp3SowDec3ROCultivarEmerald</t>
   </si>
 </sst>
 </file>
@@ -601,8 +601,8 @@
   <dimension ref="A1:AX499"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F502" sqref="F502"/>
+      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -619,7 +619,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -628,7 +628,7 @@
         <v>36</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>3</v>
@@ -765,7 +765,7 @@
     </row>
     <row r="2" spans="1:50">
       <c r="A2" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B2" s="5">
         <v>35782</v>
@@ -813,7 +813,7 @@
     </row>
     <row r="3" spans="1:50">
       <c r="A3" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B3" s="5">
         <v>35804</v>
@@ -846,7 +846,7 @@
     </row>
     <row r="4" spans="1:50">
       <c r="A4" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B4" s="5">
         <v>35809</v>
@@ -879,7 +879,7 @@
     </row>
     <row r="5" spans="1:50">
       <c r="A5" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B5" s="5">
         <v>35811</v>
@@ -912,7 +912,7 @@
     </row>
     <row r="6" spans="1:50">
       <c r="A6" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B6" s="5">
         <v>35814</v>
@@ -945,7 +945,7 @@
     </row>
     <row r="7" spans="1:50">
       <c r="A7" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B7" s="5">
         <v>35817</v>
@@ -978,7 +978,7 @@
     </row>
     <row r="8" spans="1:50">
       <c r="A8" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B8" s="5">
         <v>35821</v>
@@ -1011,7 +1011,7 @@
     </row>
     <row r="9" spans="1:50">
       <c r="A9" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B9" s="5">
         <v>35826</v>
@@ -1048,7 +1048,7 @@
     </row>
     <row r="10" spans="1:50">
       <c r="A10" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B10" s="5">
         <v>35827</v>
@@ -1081,7 +1081,7 @@
     </row>
     <row r="11" spans="1:50">
       <c r="A11" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B11" s="5">
         <v>35829</v>
@@ -1114,7 +1114,7 @@
     </row>
     <row r="12" spans="1:50">
       <c r="A12" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B12" s="5">
         <v>35830</v>
@@ -1150,7 +1150,7 @@
     </row>
     <row r="13" spans="1:50">
       <c r="A13" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B13" s="5">
         <v>35831</v>
@@ -1183,7 +1183,7 @@
     </row>
     <row r="14" spans="1:50">
       <c r="A14" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B14" s="5">
         <v>35832</v>
@@ -1216,7 +1216,7 @@
     </row>
     <row r="15" spans="1:50">
       <c r="A15" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B15" s="5">
         <v>35834</v>
@@ -1249,7 +1249,7 @@
     </row>
     <row r="16" spans="1:50">
       <c r="A16" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B16" s="5">
         <v>35838</v>
@@ -1282,7 +1282,7 @@
     </row>
     <row r="17" spans="1:50">
       <c r="A17" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B17" s="5">
         <v>35842</v>
@@ -1315,7 +1315,7 @@
     </row>
     <row r="18" spans="1:50">
       <c r="A18" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B18" s="5">
         <v>35844</v>
@@ -1354,7 +1354,7 @@
     </row>
     <row r="19" spans="1:50">
       <c r="A19" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B19" s="5">
         <v>35845</v>
@@ -1384,7 +1384,7 @@
     </row>
     <row r="20" spans="1:50">
       <c r="A20" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B20" s="5">
         <v>35847</v>
@@ -1420,7 +1420,7 @@
     </row>
     <row r="21" spans="1:50">
       <c r="A21" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B21" s="5">
         <v>35848</v>
@@ -1453,7 +1453,7 @@
     </row>
     <row r="22" spans="1:50">
       <c r="A22" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B22" s="5">
         <v>35850</v>
@@ -1486,7 +1486,7 @@
     </row>
     <row r="23" spans="1:50">
       <c r="A23" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B23" s="5">
         <v>35851</v>
@@ -1525,7 +1525,7 @@
     </row>
     <row r="24" spans="1:50">
       <c r="A24" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B24" s="5">
         <v>35853</v>
@@ -1558,7 +1558,7 @@
     </row>
     <row r="25" spans="1:50">
       <c r="A25" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B25" s="5">
         <v>35854</v>
@@ -1594,7 +1594,7 @@
     </row>
     <row r="26" spans="1:50">
       <c r="A26" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B26" s="5">
         <v>35856</v>
@@ -1636,7 +1636,7 @@
     </row>
     <row r="27" spans="1:50">
       <c r="A27" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B27" s="5">
         <v>35857</v>
@@ -1675,7 +1675,7 @@
     </row>
     <row r="28" spans="1:50">
       <c r="A28" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B28" s="5">
         <v>35858</v>
@@ -1720,7 +1720,7 @@
     </row>
     <row r="29" spans="1:50">
       <c r="A29" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B29" s="5">
         <v>35859</v>
@@ -1756,7 +1756,7 @@
     </row>
     <row r="30" spans="1:50">
       <c r="A30" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B30" s="5">
         <v>35862</v>
@@ -1789,7 +1789,7 @@
     </row>
     <row r="31" spans="1:50">
       <c r="A31" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B31" s="5">
         <v>35864</v>
@@ -1825,7 +1825,7 @@
     </row>
     <row r="32" spans="1:50">
       <c r="A32" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B32" s="5">
         <v>35865</v>
@@ -1858,7 +1858,7 @@
     </row>
     <row r="33" spans="1:48">
       <c r="A33" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B33" s="5">
         <v>35866</v>
@@ -1894,7 +1894,7 @@
     </row>
     <row r="34" spans="1:48">
       <c r="A34" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B34" s="5">
         <v>35867</v>
@@ -1927,7 +1927,7 @@
     </row>
     <row r="35" spans="1:48">
       <c r="A35" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B35" s="5">
         <v>35868</v>
@@ -1963,7 +1963,7 @@
     </row>
     <row r="36" spans="1:48">
       <c r="A36" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B36" s="5">
         <v>35869</v>
@@ -1996,7 +1996,7 @@
     </row>
     <row r="37" spans="1:48">
       <c r="A37" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B37" s="5">
         <v>35870</v>
@@ -2032,7 +2032,7 @@
     </row>
     <row r="38" spans="1:48">
       <c r="A38" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B38" s="5">
         <v>35871</v>
@@ -2092,7 +2092,7 @@
     </row>
     <row r="39" spans="1:48">
       <c r="A39" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B39" s="5">
         <v>35872</v>
@@ -2128,7 +2128,7 @@
     </row>
     <row r="40" spans="1:48">
       <c r="A40" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B40" s="5">
         <v>35873</v>
@@ -2161,7 +2161,7 @@
     </row>
     <row r="41" spans="1:48">
       <c r="A41" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B41" s="5">
         <v>35874</v>
@@ -2194,7 +2194,7 @@
     </row>
     <row r="42" spans="1:48">
       <c r="A42" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B42" s="5">
         <v>35875</v>
@@ -2227,7 +2227,7 @@
     </row>
     <row r="43" spans="1:48">
       <c r="A43" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B43" s="5">
         <v>35876</v>
@@ -2260,7 +2260,7 @@
     </row>
     <row r="44" spans="1:48">
       <c r="A44" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B44" s="5">
         <v>35877</v>
@@ -2293,7 +2293,7 @@
     </row>
     <row r="45" spans="1:48">
       <c r="A45" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B45" s="5">
         <v>35878</v>
@@ -2329,7 +2329,7 @@
     </row>
     <row r="46" spans="1:48">
       <c r="A46" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B46" s="5">
         <v>35879</v>
@@ -2362,7 +2362,7 @@
     </row>
     <row r="47" spans="1:48">
       <c r="A47" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B47" s="5">
         <v>35880</v>
@@ -2395,7 +2395,7 @@
     </row>
     <row r="48" spans="1:48">
       <c r="A48" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B48" s="5">
         <v>35882</v>
@@ -2425,7 +2425,7 @@
     </row>
     <row r="49" spans="1:49" ht="15.75" customHeight="1">
       <c r="A49" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B49" s="5">
         <v>35883</v>
@@ -2458,7 +2458,7 @@
     </row>
     <row r="50" spans="1:49">
       <c r="A50" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B50" s="5">
         <v>35884</v>
@@ -2497,13 +2497,13 @@
     </row>
     <row r="51" spans="1:49">
       <c r="A51" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B51" s="5">
         <v>35885</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D51" s="6">
         <v>104.081291759465</v>
@@ -2575,7 +2575,7 @@
     </row>
     <row r="52" spans="1:49">
       <c r="A52" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B52" s="5">
         <v>35886</v>
@@ -2608,7 +2608,7 @@
     </row>
     <row r="53" spans="1:49">
       <c r="A53" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B53" s="5">
         <v>35887</v>
@@ -2641,7 +2641,7 @@
     </row>
     <row r="54" spans="1:49">
       <c r="A54" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B54" s="5">
         <v>35890</v>
@@ -2674,7 +2674,7 @@
     </row>
     <row r="55" spans="1:49">
       <c r="A55" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B55" s="5">
         <v>35891</v>
@@ -2707,7 +2707,7 @@
     </row>
     <row r="56" spans="1:49">
       <c r="A56" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B56" s="5">
         <v>35892</v>
@@ -2740,7 +2740,7 @@
     </row>
     <row r="57" spans="1:49">
       <c r="A57" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B57" s="5">
         <v>35893</v>
@@ -2776,7 +2776,7 @@
     </row>
     <row r="58" spans="1:49">
       <c r="A58" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B58" s="5">
         <v>35895</v>
@@ -2812,7 +2812,7 @@
     </row>
     <row r="59" spans="1:49">
       <c r="A59" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B59" s="5">
         <v>35896</v>
@@ -2869,7 +2869,7 @@
     </row>
     <row r="60" spans="1:49">
       <c r="A60" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B60" s="5">
         <v>35898</v>
@@ -2902,7 +2902,7 @@
     </row>
     <row r="61" spans="1:49">
       <c r="A61" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B61" s="5">
         <v>35899</v>
@@ -2941,7 +2941,7 @@
     </row>
     <row r="62" spans="1:49">
       <c r="A62" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B62" s="5">
         <v>35900</v>
@@ -2977,7 +2977,7 @@
     </row>
     <row r="63" spans="1:49">
       <c r="A63" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B63" s="5">
         <v>35782</v>
@@ -3010,7 +3010,7 @@
     </row>
     <row r="64" spans="1:49">
       <c r="A64" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B64" s="5">
         <v>35804</v>
@@ -3043,7 +3043,7 @@
     </row>
     <row r="65" spans="1:36">
       <c r="A65" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B65" s="5">
         <v>35809</v>
@@ -3076,7 +3076,7 @@
     </row>
     <row r="66" spans="1:36">
       <c r="A66" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B66" s="5">
         <v>35811</v>
@@ -3109,7 +3109,7 @@
     </row>
     <row r="67" spans="1:36">
       <c r="A67" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B67" s="5">
         <v>35815</v>
@@ -3142,7 +3142,7 @@
     </row>
     <row r="68" spans="1:36">
       <c r="A68" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B68" s="5">
         <v>35817</v>
@@ -3175,7 +3175,7 @@
     </row>
     <row r="69" spans="1:36">
       <c r="A69" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B69" s="5">
         <v>35821</v>
@@ -3208,7 +3208,7 @@
     </row>
     <row r="70" spans="1:36">
       <c r="A70" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B70" s="5">
         <v>35827</v>
@@ -3241,7 +3241,7 @@
     </row>
     <row r="71" spans="1:36">
       <c r="A71" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B71" s="5">
         <v>35829</v>
@@ -3298,7 +3298,7 @@
     </row>
     <row r="72" spans="1:36">
       <c r="A72" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B72" s="5">
         <v>35830</v>
@@ -3334,7 +3334,7 @@
     </row>
     <row r="73" spans="1:36">
       <c r="A73" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B73" s="5">
         <v>35831</v>
@@ -3370,7 +3370,7 @@
     </row>
     <row r="74" spans="1:36">
       <c r="A74" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B74" s="5">
         <v>35832</v>
@@ -3403,7 +3403,7 @@
     </row>
     <row r="75" spans="1:36">
       <c r="A75" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B75" s="5">
         <v>35834</v>
@@ -3436,7 +3436,7 @@
     </row>
     <row r="76" spans="1:36">
       <c r="A76" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B76" s="5">
         <v>35838</v>
@@ -3469,7 +3469,7 @@
     </row>
     <row r="77" spans="1:36">
       <c r="A77" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B77" s="5">
         <v>35843</v>
@@ -3508,7 +3508,7 @@
     </row>
     <row r="78" spans="1:36">
       <c r="A78" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B78" s="5">
         <v>35844</v>
@@ -3544,7 +3544,7 @@
     </row>
     <row r="79" spans="1:36">
       <c r="A79" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B79" s="5">
         <v>35845</v>
@@ -3580,7 +3580,7 @@
     </row>
     <row r="80" spans="1:36">
       <c r="A80" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B80" s="5">
         <v>35846</v>
@@ -3613,7 +3613,7 @@
     </row>
     <row r="81" spans="1:42">
       <c r="A81" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B81" s="5">
         <v>35847</v>
@@ -3649,7 +3649,7 @@
     </row>
     <row r="82" spans="1:42">
       <c r="A82" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B82" s="5">
         <v>35849</v>
@@ -3685,7 +3685,7 @@
     </row>
     <row r="83" spans="1:42">
       <c r="A83" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B83" s="5">
         <v>35850</v>
@@ -3721,7 +3721,7 @@
     </row>
     <row r="84" spans="1:42">
       <c r="A84" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B84" s="5">
         <v>35852</v>
@@ -3754,7 +3754,7 @@
     </row>
     <row r="85" spans="1:42">
       <c r="A85" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B85" s="5">
         <v>35853</v>
@@ -3787,7 +3787,7 @@
     </row>
     <row r="86" spans="1:42">
       <c r="A86" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B86" s="5">
         <v>35854</v>
@@ -3823,7 +3823,7 @@
     </row>
     <row r="87" spans="1:42">
       <c r="A87" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B87" s="5">
         <v>35855</v>
@@ -3856,7 +3856,7 @@
     </row>
     <row r="88" spans="1:42">
       <c r="A88" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B88" s="5">
         <v>35856</v>
@@ -3895,7 +3895,7 @@
     </row>
     <row r="89" spans="1:42">
       <c r="A89" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B89" s="5">
         <v>35857</v>
@@ -3967,7 +3967,7 @@
     </row>
     <row r="90" spans="1:42">
       <c r="A90" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B90" s="5">
         <v>35858</v>
@@ -4012,7 +4012,7 @@
     </row>
     <row r="91" spans="1:42">
       <c r="A91" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B91" s="5">
         <v>35860</v>
@@ -4045,7 +4045,7 @@
     </row>
     <row r="92" spans="1:42">
       <c r="A92" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B92" s="5">
         <v>35862</v>
@@ -4081,7 +4081,7 @@
     </row>
     <row r="93" spans="1:42">
       <c r="A93" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B93" s="5">
         <v>35863</v>
@@ -4117,7 +4117,7 @@
     </row>
     <row r="94" spans="1:42">
       <c r="A94" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B94" s="5">
         <v>35865</v>
@@ -4150,7 +4150,7 @@
     </row>
     <row r="95" spans="1:42">
       <c r="A95" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B95" s="5">
         <v>35866</v>
@@ -4186,7 +4186,7 @@
     </row>
     <row r="96" spans="1:42">
       <c r="A96" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B96" s="5">
         <v>35867</v>
@@ -4219,7 +4219,7 @@
     </row>
     <row r="97" spans="1:48">
       <c r="A97" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B97" s="5">
         <v>35868</v>
@@ -4252,7 +4252,7 @@
     </row>
     <row r="98" spans="1:48">
       <c r="A98" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B98" s="5">
         <v>35869</v>
@@ -4294,7 +4294,7 @@
     </row>
     <row r="99" spans="1:48">
       <c r="A99" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B99" s="5">
         <v>35870</v>
@@ -4330,7 +4330,7 @@
     </row>
     <row r="100" spans="1:48">
       <c r="A100" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B100" s="5">
         <v>35871</v>
@@ -4375,7 +4375,7 @@
     </row>
     <row r="101" spans="1:48">
       <c r="A101" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B101" s="5">
         <v>35872</v>
@@ -4414,7 +4414,7 @@
     </row>
     <row r="102" spans="1:48">
       <c r="A102" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B102" s="5">
         <v>35873</v>
@@ -4450,7 +4450,7 @@
     </row>
     <row r="103" spans="1:48">
       <c r="A103" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B103" s="5">
         <v>35874</v>
@@ -4486,7 +4486,7 @@
     </row>
     <row r="104" spans="1:48">
       <c r="A104" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B104" s="5">
         <v>35875</v>
@@ -4540,13 +4540,13 @@
     </row>
     <row r="105" spans="1:48">
       <c r="A105" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B105" s="5">
         <v>35877</v>
       </c>
       <c r="C105" s="5" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D105" s="6">
         <v>96.424668665414998</v>
@@ -4612,7 +4612,7 @@
     </row>
     <row r="106" spans="1:48">
       <c r="A106" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B106" s="5">
         <v>35878</v>
@@ -4648,7 +4648,7 @@
     </row>
     <row r="107" spans="1:48">
       <c r="A107" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B107" s="5">
         <v>35879</v>
@@ -4681,7 +4681,7 @@
     </row>
     <row r="108" spans="1:48">
       <c r="A108" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B108" s="5">
         <v>35882</v>
@@ -4714,7 +4714,7 @@
     </row>
     <row r="109" spans="1:48">
       <c r="A109" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B109" s="5">
         <v>35883</v>
@@ -4747,7 +4747,7 @@
     </row>
     <row r="110" spans="1:48">
       <c r="A110" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B110" s="5">
         <v>35884</v>
@@ -4789,7 +4789,7 @@
     </row>
     <row r="111" spans="1:48">
       <c r="A111" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B111" s="5">
         <v>35885</v>
@@ -4825,7 +4825,7 @@
     </row>
     <row r="112" spans="1:48">
       <c r="A112" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B112" s="5">
         <v>35886</v>
@@ -4861,7 +4861,7 @@
     </row>
     <row r="113" spans="1:50">
       <c r="A113" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B113" s="5">
         <v>35887</v>
@@ -4894,7 +4894,7 @@
     </row>
     <row r="114" spans="1:50">
       <c r="A114" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B114" s="5">
         <v>35889</v>
@@ -4936,7 +4936,7 @@
     </row>
     <row r="115" spans="1:50">
       <c r="A115" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B115" s="5">
         <v>35890</v>
@@ -4969,7 +4969,7 @@
     </row>
     <row r="116" spans="1:50">
       <c r="A116" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B116" s="5">
         <v>35891</v>
@@ -5032,7 +5032,7 @@
     </row>
     <row r="117" spans="1:50" ht="15.75" customHeight="1">
       <c r="A117" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B117" s="5">
         <v>35782</v>
@@ -5065,7 +5065,7 @@
     </row>
     <row r="118" spans="1:50">
       <c r="A118" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B118" s="5">
         <v>35789</v>
@@ -5098,7 +5098,7 @@
     </row>
     <row r="119" spans="1:50">
       <c r="A119" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B119" s="5">
         <v>35804</v>
@@ -5131,7 +5131,7 @@
     </row>
     <row r="120" spans="1:50">
       <c r="A120" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B120" s="5">
         <v>35810</v>
@@ -5164,7 +5164,7 @@
     </row>
     <row r="121" spans="1:50">
       <c r="A121" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B121" s="5">
         <v>35813</v>
@@ -5197,7 +5197,7 @@
     </row>
     <row r="122" spans="1:50">
       <c r="A122" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B122" s="5">
         <v>35814</v>
@@ -5254,7 +5254,7 @@
     </row>
     <row r="123" spans="1:50">
       <c r="A123" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B123" s="5">
         <v>35817</v>
@@ -5287,7 +5287,7 @@
     </row>
     <row r="124" spans="1:50">
       <c r="A124" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B124" s="5">
         <v>35818</v>
@@ -5320,7 +5320,7 @@
     </row>
     <row r="125" spans="1:50">
       <c r="A125" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B125" s="5">
         <v>35822</v>
@@ -5353,7 +5353,7 @@
     </row>
     <row r="126" spans="1:50">
       <c r="A126" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B126" s="5">
         <v>35826</v>
@@ -5390,7 +5390,7 @@
     </row>
     <row r="127" spans="1:50">
       <c r="A127" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B127" s="5">
         <v>35827</v>
@@ -5423,7 +5423,7 @@
     </row>
     <row r="128" spans="1:50">
       <c r="A128" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B128" s="5">
         <v>35830</v>
@@ -5462,7 +5462,7 @@
     </row>
     <row r="129" spans="1:50">
       <c r="A129" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B129" s="5">
         <v>35831</v>
@@ -5501,7 +5501,7 @@
     </row>
     <row r="130" spans="1:50">
       <c r="A130" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B130" s="5">
         <v>35834</v>
@@ -5537,7 +5537,7 @@
     </row>
     <row r="131" spans="1:50">
       <c r="A131" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B131" s="5">
         <v>35837</v>
@@ -5573,7 +5573,7 @@
     </row>
     <row r="132" spans="1:50">
       <c r="A132" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B132" s="5">
         <v>35838</v>
@@ -5612,7 +5612,7 @@
     </row>
     <row r="133" spans="1:50">
       <c r="A133" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B133" s="5">
         <v>35842</v>
@@ -5672,7 +5672,7 @@
     </row>
     <row r="134" spans="1:50">
       <c r="A134" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B134" s="5">
         <v>35843</v>
@@ -5705,7 +5705,7 @@
     </row>
     <row r="135" spans="1:50">
       <c r="A135" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B135" s="5">
         <v>35844</v>
@@ -5738,7 +5738,7 @@
     </row>
     <row r="136" spans="1:50">
       <c r="A136" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B136" s="5">
         <v>35845</v>
@@ -5774,7 +5774,7 @@
     </row>
     <row r="137" spans="1:50">
       <c r="A137" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B137" s="5">
         <v>35846</v>
@@ -5807,7 +5807,7 @@
     </row>
     <row r="138" spans="1:50">
       <c r="A138" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B138" s="5">
         <v>35847</v>
@@ -5840,7 +5840,7 @@
     </row>
     <row r="139" spans="1:50">
       <c r="A139" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B139" s="5">
         <v>35848</v>
@@ -5876,7 +5876,7 @@
     </row>
     <row r="140" spans="1:50">
       <c r="A140" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B140" s="5">
         <v>35849</v>
@@ -5909,7 +5909,7 @@
     </row>
     <row r="141" spans="1:50">
       <c r="A141" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B141" s="5">
         <v>35851</v>
@@ -5951,7 +5951,7 @@
     </row>
     <row r="142" spans="1:50">
       <c r="A142" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B142" s="5">
         <v>35852</v>
@@ -5984,7 +5984,7 @@
     </row>
     <row r="143" spans="1:50">
       <c r="A143" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B143" s="5">
         <v>35853</v>
@@ -6017,7 +6017,7 @@
     </row>
     <row r="144" spans="1:50">
       <c r="A144" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B144" s="5">
         <v>35855</v>
@@ -6068,7 +6068,7 @@
     </row>
     <row r="145" spans="1:48">
       <c r="A145" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B145" s="5">
         <v>35856</v>
@@ -6104,7 +6104,7 @@
     </row>
     <row r="146" spans="1:48">
       <c r="A146" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B146" s="5">
         <v>35857</v>
@@ -6140,7 +6140,7 @@
     </row>
     <row r="147" spans="1:48">
       <c r="A147" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B147" s="5">
         <v>35858</v>
@@ -6182,7 +6182,7 @@
     </row>
     <row r="148" spans="1:48">
       <c r="A148" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B148" s="5">
         <v>35860</v>
@@ -6215,7 +6215,7 @@
     </row>
     <row r="149" spans="1:48">
       <c r="A149" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B149" s="5">
         <v>35861</v>
@@ -6248,7 +6248,7 @@
     </row>
     <row r="150" spans="1:48">
       <c r="A150" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B150" s="5">
         <v>35862</v>
@@ -6284,7 +6284,7 @@
     </row>
     <row r="151" spans="1:48">
       <c r="A151" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B151" s="5">
         <v>35863</v>
@@ -6317,7 +6317,7 @@
     </row>
     <row r="152" spans="1:48">
       <c r="A152" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B152" s="5">
         <v>35865</v>
@@ -6353,7 +6353,7 @@
     </row>
     <row r="153" spans="1:48">
       <c r="A153" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B153" s="5">
         <v>35866</v>
@@ -6392,7 +6392,7 @@
     </row>
     <row r="154" spans="1:48">
       <c r="A154" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B154" s="5">
         <v>35867</v>
@@ -6425,7 +6425,7 @@
     </row>
     <row r="155" spans="1:48">
       <c r="A155" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B155" s="5">
         <v>35868</v>
@@ -6464,7 +6464,7 @@
     </row>
     <row r="156" spans="1:48">
       <c r="A156" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B156" s="5">
         <v>35869</v>
@@ -6497,7 +6497,7 @@
     </row>
     <row r="157" spans="1:48">
       <c r="A157" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B157" s="5">
         <v>35870</v>
@@ -6530,7 +6530,7 @@
     </row>
     <row r="158" spans="1:48">
       <c r="A158" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B158" s="5">
         <v>35871</v>
@@ -6581,7 +6581,7 @@
     </row>
     <row r="159" spans="1:48">
       <c r="A159" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B159" s="5">
         <v>35872</v>
@@ -6617,7 +6617,7 @@
     </row>
     <row r="160" spans="1:48">
       <c r="A160" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B160" s="5">
         <v>35873</v>
@@ -6653,7 +6653,7 @@
     </row>
     <row r="161" spans="1:50">
       <c r="A161" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B161" s="5">
         <v>35876</v>
@@ -6689,13 +6689,13 @@
     </row>
     <row r="162" spans="1:50">
       <c r="A162" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B162" s="5">
         <v>35877</v>
       </c>
       <c r="C162" s="5" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D162" s="6">
         <v>95.5483163357178</v>
@@ -6797,7 +6797,7 @@
     </row>
     <row r="163" spans="1:50">
       <c r="A163" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B163" s="5">
         <v>35878</v>
@@ -6830,7 +6830,7 @@
     </row>
     <row r="164" spans="1:50">
       <c r="A164" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B164" s="5">
         <v>35879</v>
@@ -6863,7 +6863,7 @@
     </row>
     <row r="165" spans="1:50">
       <c r="A165" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B165" s="5">
         <v>35882</v>
@@ -6899,7 +6899,7 @@
     </row>
     <row r="166" spans="1:50">
       <c r="A166" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B166" s="5">
         <v>35883</v>
@@ -6938,7 +6938,7 @@
     </row>
     <row r="167" spans="1:50">
       <c r="A167" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B167" s="5">
         <v>35884</v>
@@ -6971,7 +6971,7 @@
     </row>
     <row r="168" spans="1:50">
       <c r="A168" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B168" s="5">
         <v>35885</v>
@@ -7016,7 +7016,7 @@
     </row>
     <row r="169" spans="1:50">
       <c r="A169" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B169" s="5">
         <v>35886</v>
@@ -7058,7 +7058,7 @@
     </row>
     <row r="170" spans="1:50">
       <c r="A170" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B170" s="5">
         <v>35889</v>
@@ -7094,7 +7094,7 @@
     </row>
     <row r="171" spans="1:50" ht="16.5" customHeight="1">
       <c r="A171" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B171" s="5">
         <v>35890</v>
@@ -7130,7 +7130,7 @@
     </row>
     <row r="172" spans="1:50">
       <c r="A172" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B172" s="5">
         <v>35891</v>
@@ -7184,7 +7184,7 @@
     </row>
     <row r="173" spans="1:50">
       <c r="A173" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B173" s="5">
         <v>35895</v>
@@ -7217,7 +7217,7 @@
     </row>
     <row r="174" spans="1:50">
       <c r="A174" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B174" s="5">
         <v>35795</v>
@@ -7250,7 +7250,7 @@
     </row>
     <row r="175" spans="1:50">
       <c r="A175" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B175" s="5">
         <v>35826</v>
@@ -7286,7 +7286,7 @@
     </row>
     <row r="176" spans="1:50">
       <c r="A176" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B176" s="5">
         <v>35828</v>
@@ -7319,7 +7319,7 @@
     </row>
     <row r="177" spans="1:50">
       <c r="A177" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B177" s="5">
         <v>35831</v>
@@ -7352,7 +7352,7 @@
     </row>
     <row r="178" spans="1:50">
       <c r="A178" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B178" s="5">
         <v>35835</v>
@@ -7385,7 +7385,7 @@
     </row>
     <row r="179" spans="1:50">
       <c r="A179" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B179" s="5">
         <v>35841</v>
@@ -7418,7 +7418,7 @@
     </row>
     <row r="180" spans="1:50">
       <c r="A180" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B180" s="5">
         <v>35842</v>
@@ -7451,7 +7451,7 @@
     </row>
     <row r="181" spans="1:50">
       <c r="A181" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B181" s="5">
         <v>35843</v>
@@ -7487,7 +7487,7 @@
     </row>
     <row r="182" spans="1:50">
       <c r="A182" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B182" s="5">
         <v>35844</v>
@@ -7523,7 +7523,7 @@
     </row>
     <row r="183" spans="1:50">
       <c r="A183" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B183" s="5">
         <v>35847</v>
@@ -7556,7 +7556,7 @@
     </row>
     <row r="184" spans="1:50">
       <c r="A184" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B184" s="5">
         <v>35851</v>
@@ -7589,7 +7589,7 @@
     </row>
     <row r="185" spans="1:50">
       <c r="A185" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B185" s="5">
         <v>35855</v>
@@ -7628,7 +7628,7 @@
     </row>
     <row r="186" spans="1:50">
       <c r="A186" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B186" s="5">
         <v>35861</v>
@@ -7661,7 +7661,7 @@
     </row>
     <row r="187" spans="1:50">
       <c r="A187" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B187" s="5">
         <v>35863</v>
@@ -7694,7 +7694,7 @@
     </row>
     <row r="188" spans="1:50">
       <c r="A188" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B188" s="5">
         <v>35864</v>
@@ -7727,7 +7727,7 @@
     </row>
     <row r="189" spans="1:50">
       <c r="A189" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B189" s="5">
         <v>35865</v>
@@ -7760,7 +7760,7 @@
     </row>
     <row r="190" spans="1:50">
       <c r="A190" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B190" s="5">
         <v>35866</v>
@@ -7793,7 +7793,7 @@
     </row>
     <row r="191" spans="1:50">
       <c r="A191" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B191" s="5">
         <v>35867</v>
@@ -7826,7 +7826,7 @@
     </row>
     <row r="192" spans="1:50">
       <c r="A192" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B192" s="5">
         <v>35868</v>
@@ -7862,7 +7862,7 @@
     </row>
     <row r="193" spans="1:48">
       <c r="A193" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B193" s="5">
         <v>35869</v>
@@ -7895,7 +7895,7 @@
     </row>
     <row r="194" spans="1:48">
       <c r="A194" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B194" s="5">
         <v>35870</v>
@@ -7937,7 +7937,7 @@
     </row>
     <row r="195" spans="1:48">
       <c r="A195" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B195" s="5">
         <v>35871</v>
@@ -7979,7 +7979,7 @@
     </row>
     <row r="196" spans="1:48">
       <c r="A196" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B196" s="5">
         <v>35872</v>
@@ -8015,7 +8015,7 @@
     </row>
     <row r="197" spans="1:48">
       <c r="A197" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B197" s="5">
         <v>35875</v>
@@ -8048,7 +8048,7 @@
     </row>
     <row r="198" spans="1:48">
       <c r="A198" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B198" s="5">
         <v>35877</v>
@@ -8081,7 +8081,7 @@
     </row>
     <row r="199" spans="1:48">
       <c r="A199" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B199" s="5">
         <v>35878</v>
@@ -8114,7 +8114,7 @@
     </row>
     <row r="200" spans="1:48">
       <c r="A200" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B200" s="5">
         <v>35879</v>
@@ -8153,7 +8153,7 @@
     </row>
     <row r="201" spans="1:48">
       <c r="A201" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B201" s="5">
         <v>35881</v>
@@ -8186,7 +8186,7 @@
     </row>
     <row r="202" spans="1:48">
       <c r="A202" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B202" s="5">
         <v>35882</v>
@@ -8225,7 +8225,7 @@
     </row>
     <row r="203" spans="1:48">
       <c r="A203" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B203" s="5">
         <v>35883</v>
@@ -8258,7 +8258,7 @@
     </row>
     <row r="204" spans="1:48">
       <c r="A204" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B204" s="5">
         <v>35884</v>
@@ -8309,7 +8309,7 @@
     </row>
     <row r="205" spans="1:48">
       <c r="A205" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B205" s="5">
         <v>35885</v>
@@ -8351,7 +8351,7 @@
     </row>
     <row r="206" spans="1:48">
       <c r="A206" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B206" s="5">
         <v>35886</v>
@@ -8387,7 +8387,7 @@
     </row>
     <row r="207" spans="1:48">
       <c r="A207" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B207" s="5">
         <v>35887</v>
@@ -8420,7 +8420,7 @@
     </row>
     <row r="208" spans="1:48">
       <c r="A208" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B208" s="5">
         <v>35888</v>
@@ -8453,7 +8453,7 @@
     </row>
     <row r="209" spans="1:50">
       <c r="A209" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B209" s="5">
         <v>35889</v>
@@ -8486,7 +8486,7 @@
     </row>
     <row r="210" spans="1:50">
       <c r="A210" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B210" s="5">
         <v>35890</v>
@@ -8522,7 +8522,7 @@
     </row>
     <row r="211" spans="1:50">
       <c r="A211" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B211" s="5">
         <v>35891</v>
@@ -8555,7 +8555,7 @@
     </row>
     <row r="212" spans="1:50">
       <c r="A212" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B212" s="5">
         <v>35892</v>
@@ -8588,7 +8588,7 @@
     </row>
     <row r="213" spans="1:50">
       <c r="A213" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B213" s="5">
         <v>35893</v>
@@ -8621,7 +8621,7 @@
     </row>
     <row r="214" spans="1:50">
       <c r="A214" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B214" s="5">
         <v>35895</v>
@@ -8654,7 +8654,7 @@
     </row>
     <row r="215" spans="1:50">
       <c r="A215" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B215" s="5">
         <v>35896</v>
@@ -8687,7 +8687,7 @@
     </row>
     <row r="216" spans="1:50">
       <c r="A216" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B216" s="5">
         <v>35897</v>
@@ -8729,7 +8729,7 @@
     </row>
     <row r="217" spans="1:50">
       <c r="A217" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B217" s="5">
         <v>35898</v>
@@ -8765,13 +8765,13 @@
     </row>
     <row r="218" spans="1:50">
       <c r="A218" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B218" s="5">
         <v>35899</v>
       </c>
       <c r="C218" s="5" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D218" s="6">
         <v>104.649220489977</v>
@@ -8840,7 +8840,7 @@
     </row>
     <row r="219" spans="1:50">
       <c r="A219" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B219" s="5">
         <v>35900</v>
@@ -8873,7 +8873,7 @@
     </row>
     <row r="220" spans="1:50">
       <c r="A220" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B220" s="5">
         <v>35903</v>
@@ -8909,7 +8909,7 @@
     </row>
     <row r="221" spans="1:50">
       <c r="A221" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B221" s="5">
         <v>35905</v>
@@ -8942,7 +8942,7 @@
     </row>
     <row r="222" spans="1:50">
       <c r="A222" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B222" s="5">
         <v>35906</v>
@@ -8978,7 +8978,7 @@
     </row>
     <row r="223" spans="1:50">
       <c r="A223" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B223" s="5">
         <v>35909</v>
@@ -9014,7 +9014,7 @@
     </row>
     <row r="224" spans="1:50">
       <c r="A224" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B224" s="5">
         <v>35911</v>
@@ -9056,7 +9056,7 @@
     </row>
     <row r="225" spans="1:49">
       <c r="A225" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B225" s="5">
         <v>35912</v>
@@ -9098,7 +9098,7 @@
     </row>
     <row r="226" spans="1:49">
       <c r="A226" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B226" s="5">
         <v>35916</v>
@@ -9131,7 +9131,7 @@
     </row>
     <row r="227" spans="1:49">
       <c r="A227" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B227" s="5">
         <v>35920</v>
@@ -9170,7 +9170,7 @@
     </row>
     <row r="228" spans="1:49">
       <c r="A228" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B228" s="5">
         <v>35924</v>
@@ -9203,7 +9203,7 @@
     </row>
     <row r="229" spans="1:49">
       <c r="A229" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B229" s="5">
         <v>35925</v>
@@ -9236,7 +9236,7 @@
     </row>
     <row r="230" spans="1:49">
       <c r="A230" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B230" s="5">
         <v>35926</v>
@@ -9299,7 +9299,7 @@
     </row>
     <row r="231" spans="1:49">
       <c r="A231" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B231" s="5">
         <v>35795</v>
@@ -9332,7 +9332,7 @@
     </row>
     <row r="232" spans="1:49">
       <c r="A232" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B232" s="5">
         <v>35829</v>
@@ -9365,7 +9365,7 @@
     </row>
     <row r="233" spans="1:49">
       <c r="A233" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B233" s="5">
         <v>35831</v>
@@ -9398,7 +9398,7 @@
     </row>
     <row r="234" spans="1:49">
       <c r="A234" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B234" s="5">
         <v>35835</v>
@@ -9431,7 +9431,7 @@
     </row>
     <row r="235" spans="1:49">
       <c r="A235" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B235" s="5">
         <v>35841</v>
@@ -9464,7 +9464,7 @@
     </row>
     <row r="236" spans="1:49">
       <c r="A236" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B236" s="5">
         <v>35842</v>
@@ -9521,7 +9521,7 @@
     </row>
     <row r="237" spans="1:49">
       <c r="A237" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B237" s="5">
         <v>35843</v>
@@ -9557,7 +9557,7 @@
     </row>
     <row r="238" spans="1:49">
       <c r="A238" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B238" s="5">
         <v>35844</v>
@@ -9593,7 +9593,7 @@
     </row>
     <row r="239" spans="1:49">
       <c r="A239" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B239" s="5">
         <v>35845</v>
@@ -9626,7 +9626,7 @@
     </row>
     <row r="240" spans="1:49">
       <c r="A240" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B240" s="5">
         <v>35847</v>
@@ -9659,7 +9659,7 @@
     </row>
     <row r="241" spans="1:42">
       <c r="A241" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B241" s="5">
         <v>35852</v>
@@ -9692,7 +9692,7 @@
     </row>
     <row r="242" spans="1:42">
       <c r="A242" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B242" s="5">
         <v>35856</v>
@@ -9725,7 +9725,7 @@
     </row>
     <row r="243" spans="1:42">
       <c r="A243" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B243" s="5">
         <v>35861</v>
@@ -9758,7 +9758,7 @@
     </row>
     <row r="244" spans="1:42">
       <c r="A244" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B244" s="5">
         <v>35862</v>
@@ -9794,7 +9794,7 @@
     </row>
     <row r="245" spans="1:42">
       <c r="A245" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B245" s="5">
         <v>35863</v>
@@ -9827,7 +9827,7 @@
     </row>
     <row r="246" spans="1:42">
       <c r="A246" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B246" s="5">
         <v>35865</v>
@@ -9860,7 +9860,7 @@
     </row>
     <row r="247" spans="1:42">
       <c r="A247" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B247" s="5">
         <v>35866</v>
@@ -9896,7 +9896,7 @@
     </row>
     <row r="248" spans="1:42">
       <c r="A248" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B248" s="5">
         <v>35867</v>
@@ -9929,7 +9929,7 @@
     </row>
     <row r="249" spans="1:42">
       <c r="A249" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B249" s="5">
         <v>35868</v>
@@ -9965,7 +9965,7 @@
     </row>
     <row r="250" spans="1:42">
       <c r="A250" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B250" s="5">
         <v>35869</v>
@@ -10004,7 +10004,7 @@
     </row>
     <row r="251" spans="1:42">
       <c r="A251" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B251" s="5">
         <v>35870</v>
@@ -10067,7 +10067,7 @@
     </row>
     <row r="252" spans="1:42">
       <c r="A252" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B252" s="5">
         <v>35871</v>
@@ -10112,7 +10112,7 @@
     </row>
     <row r="253" spans="1:42">
       <c r="A253" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B253" s="5">
         <v>35872</v>
@@ -10145,7 +10145,7 @@
     </row>
     <row r="254" spans="1:42">
       <c r="A254" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B254" s="5">
         <v>35874</v>
@@ -10178,7 +10178,7 @@
     </row>
     <row r="255" spans="1:42">
       <c r="A255" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B255" s="5">
         <v>35876</v>
@@ -10214,7 +10214,7 @@
     </row>
     <row r="256" spans="1:42">
       <c r="A256" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B256" s="5">
         <v>35877</v>
@@ -10247,7 +10247,7 @@
     </row>
     <row r="257" spans="1:48">
       <c r="A257" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B257" s="5">
         <v>35878</v>
@@ -10280,7 +10280,7 @@
     </row>
     <row r="258" spans="1:48">
       <c r="A258" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B258" s="5">
         <v>35879</v>
@@ -10313,7 +10313,7 @@
     </row>
     <row r="259" spans="1:48">
       <c r="A259" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B259" s="5">
         <v>35880</v>
@@ -10346,7 +10346,7 @@
     </row>
     <row r="260" spans="1:48">
       <c r="A260" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B260" s="5">
         <v>35881</v>
@@ -10385,7 +10385,7 @@
     </row>
     <row r="261" spans="1:48">
       <c r="A261" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B261" s="5">
         <v>35882</v>
@@ -10421,7 +10421,7 @@
     </row>
     <row r="262" spans="1:48">
       <c r="A262" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B262" s="5">
         <v>35883</v>
@@ -10457,7 +10457,7 @@
     </row>
     <row r="263" spans="1:48">
       <c r="A263" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B263" s="5">
         <v>35884</v>
@@ -10517,13 +10517,13 @@
     </row>
     <row r="264" spans="1:48">
       <c r="A264" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B264" s="5">
         <v>35885</v>
       </c>
       <c r="C264" s="5" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D264" s="6">
         <v>90.914127423822606</v>
@@ -10619,7 +10619,7 @@
     </row>
     <row r="265" spans="1:48">
       <c r="A265" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B265" s="5">
         <v>35886</v>
@@ -10655,7 +10655,7 @@
     </row>
     <row r="266" spans="1:48">
       <c r="A266" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B266" s="5">
         <v>35887</v>
@@ -10688,7 +10688,7 @@
     </row>
     <row r="267" spans="1:48">
       <c r="A267" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B267" s="5">
         <v>35888</v>
@@ -10745,7 +10745,7 @@
     </row>
     <row r="268" spans="1:48">
       <c r="A268" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B268" s="5">
         <v>35889</v>
@@ -10778,7 +10778,7 @@
     </row>
     <row r="269" spans="1:48">
       <c r="A269" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B269" s="5">
         <v>35890</v>
@@ -10811,7 +10811,7 @@
     </row>
     <row r="270" spans="1:48">
       <c r="A270" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B270" s="5">
         <v>35891</v>
@@ -10844,7 +10844,7 @@
     </row>
     <row r="271" spans="1:48">
       <c r="A271" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B271" s="5">
         <v>35892</v>
@@ -10880,7 +10880,7 @@
     </row>
     <row r="272" spans="1:48">
       <c r="A272" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B272" s="5">
         <v>35895</v>
@@ -10913,7 +10913,7 @@
     </row>
     <row r="273" spans="1:49">
       <c r="A273" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B273" s="5">
         <v>35897</v>
@@ -10955,7 +10955,7 @@
     </row>
     <row r="274" spans="1:49">
       <c r="A274" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B274" s="5">
         <v>35898</v>
@@ -10991,7 +10991,7 @@
     </row>
     <row r="275" spans="1:49">
       <c r="A275" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B275" s="5">
         <v>35899</v>
@@ -11024,7 +11024,7 @@
     </row>
     <row r="276" spans="1:49">
       <c r="A276" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B276" s="5">
         <v>35900</v>
@@ -11057,7 +11057,7 @@
     </row>
     <row r="277" spans="1:49">
       <c r="A277" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B277" s="5">
         <v>35903</v>
@@ -11093,7 +11093,7 @@
     </row>
     <row r="278" spans="1:49">
       <c r="A278" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B278" s="5">
         <v>35905</v>
@@ -11126,7 +11126,7 @@
     </row>
     <row r="279" spans="1:49">
       <c r="A279" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B279" s="5">
         <v>35906</v>
@@ -11159,7 +11159,7 @@
     </row>
     <row r="280" spans="1:49">
       <c r="A280" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B280" s="5">
         <v>35907</v>
@@ -11192,7 +11192,7 @@
     </row>
     <row r="281" spans="1:49">
       <c r="A281" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B281" s="5">
         <v>35909</v>
@@ -11225,7 +11225,7 @@
     </row>
     <row r="282" spans="1:49">
       <c r="A282" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B282" s="5">
         <v>35910</v>
@@ -11264,7 +11264,7 @@
     </row>
     <row r="283" spans="1:49">
       <c r="A283" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B283" s="5">
         <v>35911</v>
@@ -11300,7 +11300,7 @@
     </row>
     <row r="284" spans="1:49">
       <c r="A284" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B284" s="5">
         <v>35912</v>
@@ -11348,7 +11348,7 @@
     </row>
     <row r="285" spans="1:49">
       <c r="A285" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B285" s="5">
         <v>35913</v>
@@ -11384,7 +11384,7 @@
     </row>
     <row r="286" spans="1:49">
       <c r="A286" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B286" s="5">
         <v>35795</v>
@@ -11417,7 +11417,7 @@
     </row>
     <row r="287" spans="1:49">
       <c r="A287" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B287" s="5">
         <v>35802</v>
@@ -11450,7 +11450,7 @@
     </row>
     <row r="288" spans="1:49">
       <c r="A288" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B288" s="5">
         <v>35815</v>
@@ -11504,7 +11504,7 @@
     </row>
     <row r="289" spans="1:50">
       <c r="A289" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B289" s="5">
         <v>35826</v>
@@ -11540,7 +11540,7 @@
     </row>
     <row r="290" spans="1:50">
       <c r="A290" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B290" s="5">
         <v>35829</v>
@@ -11573,7 +11573,7 @@
     </row>
     <row r="291" spans="1:50">
       <c r="A291" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B291" s="5">
         <v>35830</v>
@@ -11606,7 +11606,7 @@
     </row>
     <row r="292" spans="1:50">
       <c r="A292" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B292" s="5">
         <v>35831</v>
@@ -11639,7 +11639,7 @@
     </row>
     <row r="293" spans="1:50">
       <c r="A293" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B293" s="5">
         <v>35835</v>
@@ -11672,7 +11672,7 @@
     </row>
     <row r="294" spans="1:50">
       <c r="A294" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B294" s="5">
         <v>35841</v>
@@ -11705,7 +11705,7 @@
     </row>
     <row r="295" spans="1:50">
       <c r="A295" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B295" s="5">
         <v>35843</v>
@@ -11744,7 +11744,7 @@
     </row>
     <row r="296" spans="1:50">
       <c r="A296" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B296" s="5">
         <v>35844</v>
@@ -11780,7 +11780,7 @@
     </row>
     <row r="297" spans="1:50">
       <c r="A297" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B297" s="5">
         <v>35845</v>
@@ -11813,7 +11813,7 @@
     </row>
     <row r="298" spans="1:50">
       <c r="A298" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B298" s="5">
         <v>35847</v>
@@ -11846,7 +11846,7 @@
     </row>
     <row r="299" spans="1:50">
       <c r="A299" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B299" s="5">
         <v>35851</v>
@@ -11879,7 +11879,7 @@
     </row>
     <row r="300" spans="1:50">
       <c r="A300" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B300" s="5">
         <v>35855</v>
@@ -11936,7 +11936,7 @@
     </row>
     <row r="301" spans="1:50">
       <c r="A301" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B301" s="5">
         <v>35857</v>
@@ -11969,7 +11969,7 @@
     </row>
     <row r="302" spans="1:50">
       <c r="A302" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B302" s="5">
         <v>35858</v>
@@ -12002,7 +12002,7 @@
     </row>
     <row r="303" spans="1:50">
       <c r="A303" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B303" s="5">
         <v>35861</v>
@@ -12035,7 +12035,7 @@
     </row>
     <row r="304" spans="1:50">
       <c r="A304" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B304" s="5">
         <v>35862</v>
@@ -12068,7 +12068,7 @@
     </row>
     <row r="305" spans="1:50">
       <c r="A305" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B305" s="5">
         <v>35865</v>
@@ -12104,7 +12104,7 @@
     </row>
     <row r="306" spans="1:50">
       <c r="A306" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B306" s="5">
         <v>35866</v>
@@ -12137,7 +12137,7 @@
     </row>
     <row r="307" spans="1:50">
       <c r="A307" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B307" s="5">
         <v>35869</v>
@@ -12188,7 +12188,7 @@
     </row>
     <row r="308" spans="1:50">
       <c r="A308" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B308" s="5">
         <v>35870</v>
@@ -12224,7 +12224,7 @@
     </row>
     <row r="309" spans="1:50">
       <c r="A309" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B309" s="5">
         <v>35871</v>
@@ -12272,7 +12272,7 @@
     </row>
     <row r="310" spans="1:50">
       <c r="A310" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B310" s="5">
         <v>35872</v>
@@ -12305,7 +12305,7 @@
     </row>
     <row r="311" spans="1:50">
       <c r="A311" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B311" s="5">
         <v>35875</v>
@@ -12341,7 +12341,7 @@
     </row>
     <row r="312" spans="1:50">
       <c r="A312" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B312" s="5">
         <v>35876</v>
@@ -12377,7 +12377,7 @@
     </row>
     <row r="313" spans="1:50">
       <c r="A313" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B313" s="5">
         <v>35879</v>
@@ -12416,7 +12416,7 @@
     </row>
     <row r="314" spans="1:50">
       <c r="A314" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B314" s="5">
         <v>35880</v>
@@ -12449,7 +12449,7 @@
     </row>
     <row r="315" spans="1:50">
       <c r="A315" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B315" s="5">
         <v>35881</v>
@@ -12482,7 +12482,7 @@
     </row>
     <row r="316" spans="1:50">
       <c r="A316" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B316" s="5">
         <v>35882</v>
@@ -12521,7 +12521,7 @@
     </row>
     <row r="317" spans="1:50">
       <c r="A317" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B317" s="5">
         <v>35883</v>
@@ -12557,7 +12557,7 @@
     </row>
     <row r="318" spans="1:50">
       <c r="A318" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B318" s="5">
         <v>35884</v>
@@ -12590,13 +12590,13 @@
     </row>
     <row r="319" spans="1:50">
       <c r="A319" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B319" s="5">
         <v>35885</v>
       </c>
       <c r="C319" s="5" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D319" s="6">
         <v>90.557029177718803</v>
@@ -12704,7 +12704,7 @@
     </row>
     <row r="320" spans="1:50">
       <c r="A320" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B320" s="5">
         <v>35886</v>
@@ -12740,7 +12740,7 @@
     </row>
     <row r="321" spans="1:50">
       <c r="A321" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B321" s="5">
         <v>35887</v>
@@ -12773,7 +12773,7 @@
     </row>
     <row r="322" spans="1:50">
       <c r="A322" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B322" s="5">
         <v>35889</v>
@@ -12806,7 +12806,7 @@
     </row>
     <row r="323" spans="1:50">
       <c r="A323" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B323" s="5">
         <v>35890</v>
@@ -12845,7 +12845,7 @@
     </row>
     <row r="324" spans="1:50">
       <c r="A324" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B324" s="5">
         <v>35892</v>
@@ -12878,7 +12878,7 @@
     </row>
     <row r="325" spans="1:50">
       <c r="A325" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B325" s="5">
         <v>35895</v>
@@ -12911,7 +12911,7 @@
     </row>
     <row r="326" spans="1:50">
       <c r="A326" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B326" s="5">
         <v>35896</v>
@@ -12947,7 +12947,7 @@
     </row>
     <row r="327" spans="1:50">
       <c r="A327" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B327" s="5">
         <v>35897</v>
@@ -12992,7 +12992,7 @@
     </row>
     <row r="328" spans="1:50">
       <c r="A328" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B328" s="5">
         <v>35898</v>
@@ -13037,7 +13037,7 @@
     </row>
     <row r="329" spans="1:50">
       <c r="A329" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B329" s="5">
         <v>35899</v>
@@ -13076,7 +13076,7 @@
     </row>
     <row r="330" spans="1:50">
       <c r="A330" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B330" s="5">
         <v>35900</v>
@@ -13109,7 +13109,7 @@
     </row>
     <row r="331" spans="1:50">
       <c r="A331" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B331" s="5">
         <v>35903</v>
@@ -13145,7 +13145,7 @@
     </row>
     <row r="332" spans="1:50">
       <c r="A332" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B332" s="5">
         <v>35904</v>
@@ -13184,7 +13184,7 @@
     </row>
     <row r="333" spans="1:50">
       <c r="A333" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B333" s="5">
         <v>35910</v>
@@ -13220,7 +13220,7 @@
     </row>
     <row r="334" spans="1:50">
       <c r="A334" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B334" s="5">
         <v>35911</v>
@@ -13259,7 +13259,7 @@
     </row>
     <row r="335" spans="1:50">
       <c r="A335" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B335" s="5">
         <v>35912</v>
@@ -13310,7 +13310,7 @@
     </row>
     <row r="336" spans="1:50">
       <c r="A336" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B336" s="5">
         <v>35913</v>
@@ -13343,7 +13343,7 @@
     </row>
     <row r="337" spans="1:50">
       <c r="A337" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B337" s="5">
         <v>35768</v>
@@ -13376,7 +13376,7 @@
     </row>
     <row r="338" spans="1:50">
       <c r="A338" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B338" s="5">
         <v>35774</v>
@@ -13409,7 +13409,7 @@
     </row>
     <row r="339" spans="1:50">
       <c r="A339" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B339" s="5">
         <v>35782</v>
@@ -13442,7 +13442,7 @@
     </row>
     <row r="340" spans="1:50">
       <c r="A340" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B340" s="5">
         <v>35790</v>
@@ -13475,7 +13475,7 @@
     </row>
     <row r="341" spans="1:50">
       <c r="A341" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B341" s="5">
         <v>35794</v>
@@ -13508,7 +13508,7 @@
     </row>
     <row r="342" spans="1:50">
       <c r="A342" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B342" s="5">
         <v>35796</v>
@@ -13541,7 +13541,7 @@
     </row>
     <row r="343" spans="1:50">
       <c r="A343" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B343" s="5">
         <v>35801</v>
@@ -13574,7 +13574,7 @@
     </row>
     <row r="344" spans="1:50">
       <c r="A344" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B344" s="5">
         <v>35803</v>
@@ -13607,7 +13607,7 @@
     </row>
     <row r="345" spans="1:50">
       <c r="A345" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B345" s="5">
         <v>35807</v>
@@ -13640,7 +13640,7 @@
     </row>
     <row r="346" spans="1:50">
       <c r="A346" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B346" s="5">
         <v>35813</v>
@@ -13673,7 +13673,7 @@
     </row>
     <row r="347" spans="1:50">
       <c r="A347" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B347" s="5">
         <v>35815</v>
@@ -13709,7 +13709,7 @@
     </row>
     <row r="348" spans="1:50">
       <c r="A348" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B348" s="5">
         <v>35816</v>
@@ -13745,7 +13745,7 @@
     </row>
     <row r="349" spans="1:50">
       <c r="A349" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B349" s="5">
         <v>35817</v>
@@ -13784,7 +13784,7 @@
     </row>
     <row r="350" spans="1:50">
       <c r="A350" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B350" s="5">
         <v>35820</v>
@@ -13820,7 +13820,7 @@
     </row>
     <row r="351" spans="1:50">
       <c r="A351" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B351" s="5">
         <v>35821</v>
@@ -13856,7 +13856,7 @@
     </row>
     <row r="352" spans="1:50">
       <c r="A352" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B352" s="5">
         <v>35822</v>
@@ -13889,7 +13889,7 @@
     </row>
     <row r="353" spans="1:42">
       <c r="A353" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B353" s="5">
         <v>35823</v>
@@ -13922,7 +13922,7 @@
     </row>
     <row r="354" spans="1:42">
       <c r="A354" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B354" s="5">
         <v>35824</v>
@@ -13955,7 +13955,7 @@
     </row>
     <row r="355" spans="1:42">
       <c r="A355" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B355" s="5">
         <v>35827</v>
@@ -13991,7 +13991,7 @@
     </row>
     <row r="356" spans="1:42">
       <c r="A356" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B356" s="5">
         <v>35830</v>
@@ -14024,7 +14024,7 @@
     </row>
     <row r="357" spans="1:42">
       <c r="A357" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B357" s="5">
         <v>35831</v>
@@ -14060,7 +14060,7 @@
     </row>
     <row r="358" spans="1:42">
       <c r="A358" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B358" s="5">
         <v>35832</v>
@@ -14093,7 +14093,7 @@
     </row>
     <row r="359" spans="1:42">
       <c r="A359" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B359" s="5">
         <v>35834</v>
@@ -14129,7 +14129,7 @@
     </row>
     <row r="360" spans="1:42">
       <c r="A360" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B360" s="5">
         <v>35835</v>
@@ -14162,7 +14162,7 @@
     </row>
     <row r="361" spans="1:42">
       <c r="A361" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B361" s="5">
         <v>35836</v>
@@ -14195,7 +14195,7 @@
     </row>
     <row r="362" spans="1:42">
       <c r="A362" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B362" s="5">
         <v>35837</v>
@@ -14228,7 +14228,7 @@
     </row>
     <row r="363" spans="1:42">
       <c r="A363" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B363" s="5">
         <v>35838</v>
@@ -14261,7 +14261,7 @@
     </row>
     <row r="364" spans="1:42">
       <c r="A364" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B364" s="5">
         <v>35840</v>
@@ -14294,7 +14294,7 @@
     </row>
     <row r="365" spans="1:42">
       <c r="A365" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B365" s="5">
         <v>35841</v>
@@ -14336,7 +14336,7 @@
     </row>
     <row r="366" spans="1:42">
       <c r="A366" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B366" s="5">
         <v>35843</v>
@@ -14378,7 +14378,7 @@
     </row>
     <row r="367" spans="1:42">
       <c r="A367" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B367" s="5">
         <v>35844</v>
@@ -14426,7 +14426,7 @@
     </row>
     <row r="368" spans="1:42">
       <c r="A368" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B368" s="5">
         <v>35845</v>
@@ -14459,7 +14459,7 @@
     </row>
     <row r="369" spans="1:50">
       <c r="A369" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B369" s="5">
         <v>35846</v>
@@ -14489,7 +14489,7 @@
     </row>
     <row r="370" spans="1:50">
       <c r="A370" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B370" s="5">
         <v>35848</v>
@@ -14522,7 +14522,7 @@
     </row>
     <row r="371" spans="1:50">
       <c r="A371" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B371" s="5">
         <v>35850</v>
@@ -14555,7 +14555,7 @@
     </row>
     <row r="372" spans="1:50">
       <c r="A372" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B372" s="5">
         <v>35851</v>
@@ -14594,7 +14594,7 @@
     </row>
     <row r="373" spans="1:50">
       <c r="A373" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B373" s="5">
         <v>35852</v>
@@ -14627,7 +14627,7 @@
     </row>
     <row r="374" spans="1:50">
       <c r="A374" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B374" s="5">
         <v>35854</v>
@@ -14669,7 +14669,7 @@
     </row>
     <row r="375" spans="1:50">
       <c r="A375" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B375" s="5">
         <v>35856</v>
@@ -14705,7 +14705,7 @@
     </row>
     <row r="376" spans="1:50">
       <c r="A376" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B376" s="5">
         <v>35857</v>
@@ -14756,7 +14756,7 @@
     </row>
     <row r="377" spans="1:50">
       <c r="A377" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B377" s="5">
         <v>35858</v>
@@ -14801,7 +14801,7 @@
     </row>
     <row r="378" spans="1:50">
       <c r="A378" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B378" s="5">
         <v>35859</v>
@@ -14834,7 +14834,7 @@
     </row>
     <row r="379" spans="1:50">
       <c r="A379" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B379" s="5">
         <v>35860</v>
@@ -14873,7 +14873,7 @@
     </row>
     <row r="380" spans="1:50">
       <c r="A380" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B380" s="5">
         <v>35861</v>
@@ -14906,7 +14906,7 @@
     </row>
     <row r="381" spans="1:50">
       <c r="A381" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B381" s="5">
         <v>35862</v>
@@ -14939,7 +14939,7 @@
     </row>
     <row r="382" spans="1:50">
       <c r="A382" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B382" s="5">
         <v>35863</v>
@@ -14972,7 +14972,7 @@
     </row>
     <row r="383" spans="1:50">
       <c r="A383" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B383" s="5">
         <v>35864</v>
@@ -15008,7 +15008,7 @@
     </row>
     <row r="384" spans="1:50">
       <c r="A384" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B384" s="5">
         <v>35865</v>
@@ -15041,7 +15041,7 @@
     </row>
     <row r="385" spans="1:50">
       <c r="A385" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B385" s="5">
         <v>35866</v>
@@ -15074,7 +15074,7 @@
     </row>
     <row r="386" spans="1:50">
       <c r="A386" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B386" s="5">
         <v>35868</v>
@@ -15107,7 +15107,7 @@
     </row>
     <row r="387" spans="1:50">
       <c r="A387" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B387" s="5">
         <v>35869</v>
@@ -15143,7 +15143,7 @@
     </row>
     <row r="388" spans="1:50">
       <c r="A388" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B388" s="5">
         <v>35871</v>
@@ -15191,7 +15191,7 @@
     </row>
     <row r="389" spans="1:50">
       <c r="A389" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B389" s="5">
         <v>35873</v>
@@ -15227,7 +15227,7 @@
     </row>
     <row r="390" spans="1:50">
       <c r="A390" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B390" s="5">
         <v>35874</v>
@@ -15263,7 +15263,7 @@
     </row>
     <row r="391" spans="1:50">
       <c r="A391" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B391" s="5">
         <v>35876</v>
@@ -15299,13 +15299,13 @@
     </row>
     <row r="392" spans="1:50">
       <c r="A392" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B392" s="5">
         <v>35877</v>
       </c>
       <c r="C392" s="5" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D392" s="6">
         <v>109.526726057906</v>
@@ -15398,7 +15398,7 @@
     </row>
     <row r="393" spans="1:50">
       <c r="A393" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B393" s="5">
         <v>35878</v>
@@ -15434,7 +15434,7 @@
     </row>
     <row r="394" spans="1:50">
       <c r="A394" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B394" s="5">
         <v>35768</v>
@@ -15467,7 +15467,7 @@
     </row>
     <row r="395" spans="1:50">
       <c r="A395" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B395" s="5">
         <v>35773</v>
@@ -15500,7 +15500,7 @@
     </row>
     <row r="396" spans="1:50">
       <c r="A396" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B396" s="5">
         <v>35781</v>
@@ -15533,7 +15533,7 @@
     </row>
     <row r="397" spans="1:50">
       <c r="A397" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B397" s="5">
         <v>35790</v>
@@ -15566,7 +15566,7 @@
     </row>
     <row r="398" spans="1:50">
       <c r="A398" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B398" s="5">
         <v>35794</v>
@@ -15599,7 +15599,7 @@
     </row>
     <row r="399" spans="1:50">
       <c r="A399" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B399" s="5">
         <v>35796</v>
@@ -15632,7 +15632,7 @@
     </row>
     <row r="400" spans="1:50">
       <c r="A400" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B400" s="5">
         <v>35800</v>
@@ -15665,7 +15665,7 @@
     </row>
     <row r="401" spans="1:36">
       <c r="A401" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B401" s="5">
         <v>35804</v>
@@ -15698,7 +15698,7 @@
     </row>
     <row r="402" spans="1:36">
       <c r="A402" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B402" s="5">
         <v>35808</v>
@@ -15731,7 +15731,7 @@
     </row>
     <row r="403" spans="1:36">
       <c r="A403" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B403" s="5">
         <v>35813</v>
@@ -15764,7 +15764,7 @@
     </row>
     <row r="404" spans="1:36">
       <c r="A404" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B404" s="5">
         <v>35814</v>
@@ -15797,7 +15797,7 @@
     </row>
     <row r="405" spans="1:36">
       <c r="A405" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B405" s="5">
         <v>35815</v>
@@ -15854,7 +15854,7 @@
     </row>
     <row r="406" spans="1:36">
       <c r="A406" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B406" s="5">
         <v>35816</v>
@@ -15893,7 +15893,7 @@
     </row>
     <row r="407" spans="1:36">
       <c r="A407" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B407" s="5">
         <v>35817</v>
@@ -15932,7 +15932,7 @@
     </row>
     <row r="408" spans="1:36">
       <c r="A408" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B408" s="5">
         <v>35819</v>
@@ -15965,7 +15965,7 @@
     </row>
     <row r="409" spans="1:36">
       <c r="A409" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B409" s="5">
         <v>35821</v>
@@ -16007,7 +16007,7 @@
     </row>
     <row r="410" spans="1:36">
       <c r="A410" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B410" s="5">
         <v>35822</v>
@@ -16040,7 +16040,7 @@
     </row>
     <row r="411" spans="1:36">
       <c r="A411" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B411" s="5">
         <v>35824</v>
@@ -16073,7 +16073,7 @@
     </row>
     <row r="412" spans="1:36">
       <c r="A412" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B412" s="5">
         <v>35828</v>
@@ -16109,7 +16109,7 @@
     </row>
     <row r="413" spans="1:36">
       <c r="A413" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B413" s="5">
         <v>35829</v>
@@ -16142,7 +16142,7 @@
     </row>
     <row r="414" spans="1:36">
       <c r="A414" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B414" s="5">
         <v>35830</v>
@@ -16175,7 +16175,7 @@
     </row>
     <row r="415" spans="1:36">
       <c r="A415" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B415" s="5">
         <v>35831</v>
@@ -16208,7 +16208,7 @@
     </row>
     <row r="416" spans="1:36">
       <c r="A416" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B416" s="5">
         <v>35832</v>
@@ -16244,7 +16244,7 @@
     </row>
     <row r="417" spans="1:42">
       <c r="A417" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B417" s="5">
         <v>35833</v>
@@ -16277,7 +16277,7 @@
     </row>
     <row r="418" spans="1:42">
       <c r="A418" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B418" s="5">
         <v>35835</v>
@@ -16316,7 +16316,7 @@
     </row>
     <row r="419" spans="1:42">
       <c r="A419" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B419" s="5">
         <v>35836</v>
@@ -16352,7 +16352,7 @@
     </row>
     <row r="420" spans="1:42">
       <c r="A420" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B420" s="5">
         <v>35839</v>
@@ -16388,7 +16388,7 @@
     </row>
     <row r="421" spans="1:42">
       <c r="A421" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B421" s="5">
         <v>35840</v>
@@ -16421,7 +16421,7 @@
     </row>
     <row r="422" spans="1:42">
       <c r="A422" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B422" s="5">
         <v>35841</v>
@@ -16454,7 +16454,7 @@
     </row>
     <row r="423" spans="1:42">
       <c r="A423" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B423" s="5">
         <v>35842</v>
@@ -16493,7 +16493,7 @@
     </row>
     <row r="424" spans="1:42">
       <c r="A424" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B424" s="5">
         <v>35843</v>
@@ -16562,7 +16562,7 @@
     </row>
     <row r="425" spans="1:42">
       <c r="A425" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B425" s="5">
         <v>35844</v>
@@ -16604,7 +16604,7 @@
     </row>
     <row r="426" spans="1:42">
       <c r="A426" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B426" s="5">
         <v>35846</v>
@@ -16637,7 +16637,7 @@
     </row>
     <row r="427" spans="1:42">
       <c r="A427" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B427" s="5">
         <v>35848</v>
@@ -16670,7 +16670,7 @@
     </row>
     <row r="428" spans="1:42">
       <c r="A428" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B428" s="5">
         <v>35849</v>
@@ -16709,7 +16709,7 @@
     </row>
     <row r="429" spans="1:42">
       <c r="A429" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B429" s="5">
         <v>35852</v>
@@ -16745,7 +16745,7 @@
     </row>
     <row r="430" spans="1:42">
       <c r="A430" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B430" s="5">
         <v>35853</v>
@@ -16778,7 +16778,7 @@
     </row>
     <row r="431" spans="1:42">
       <c r="A431" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B431" s="5">
         <v>35854</v>
@@ -16817,7 +16817,7 @@
     </row>
     <row r="432" spans="1:42">
       <c r="A432" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B432" s="5">
         <v>35855</v>
@@ -16850,7 +16850,7 @@
     </row>
     <row r="433" spans="1:49">
       <c r="A433" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B433" s="5">
         <v>35856</v>
@@ -16886,7 +16886,7 @@
     </row>
     <row r="434" spans="1:49">
       <c r="A434" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B434" s="5">
         <v>35857</v>
@@ -16940,7 +16940,7 @@
     </row>
     <row r="435" spans="1:49">
       <c r="A435" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B435" s="5">
         <v>35858</v>
@@ -16979,7 +16979,7 @@
     </row>
     <row r="436" spans="1:49">
       <c r="A436" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B436" s="5">
         <v>35859</v>
@@ -17012,7 +17012,7 @@
     </row>
     <row r="437" spans="1:49">
       <c r="A437" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B437" s="5">
         <v>35860</v>
@@ -17048,7 +17048,7 @@
     </row>
     <row r="438" spans="1:49">
       <c r="A438" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B438" s="5">
         <v>35861</v>
@@ -17105,7 +17105,7 @@
     </row>
     <row r="439" spans="1:49">
       <c r="A439" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B439" s="5">
         <v>35863</v>
@@ -17138,7 +17138,7 @@
     </row>
     <row r="440" spans="1:49">
       <c r="A440" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B440" s="5">
         <v>35864</v>
@@ -17174,7 +17174,7 @@
     </row>
     <row r="441" spans="1:49">
       <c r="A441" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B441" s="5">
         <v>35865</v>
@@ -17210,7 +17210,7 @@
     </row>
     <row r="442" spans="1:49">
       <c r="A442" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B442" s="5">
         <v>35867</v>
@@ -17246,7 +17246,7 @@
     </row>
     <row r="443" spans="1:49">
       <c r="A443" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B443" s="5">
         <v>35869</v>
@@ -17294,13 +17294,13 @@
     </row>
     <row r="444" spans="1:49">
       <c r="A444" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B444" s="5">
         <v>35870</v>
       </c>
       <c r="C444" s="5" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D444" s="6">
         <v>102.83020062021301</v>
@@ -17408,7 +17408,7 @@
     </row>
     <row r="445" spans="1:49">
       <c r="A445" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B445" s="5">
         <v>35768</v>
@@ -17441,7 +17441,7 @@
     </row>
     <row r="446" spans="1:49">
       <c r="A446" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B446" s="5">
         <v>35774</v>
@@ -17474,7 +17474,7 @@
     </row>
     <row r="447" spans="1:49">
       <c r="A447" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B447" s="5">
         <v>35776</v>
@@ -17507,7 +17507,7 @@
     </row>
     <row r="448" spans="1:49">
       <c r="A448" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B448" s="5">
         <v>35781</v>
@@ -17540,7 +17540,7 @@
     </row>
     <row r="449" spans="1:50">
       <c r="A449" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B449" s="5">
         <v>35790</v>
@@ -17573,7 +17573,7 @@
     </row>
     <row r="450" spans="1:50">
       <c r="A450" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B450" s="5">
         <v>35795</v>
@@ -17606,7 +17606,7 @@
     </row>
     <row r="451" spans="1:50">
       <c r="A451" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B451" s="5">
         <v>35797</v>
@@ -17639,7 +17639,7 @@
     </row>
     <row r="452" spans="1:50">
       <c r="A452" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B452" s="5">
         <v>35801</v>
@@ -17672,7 +17672,7 @@
     </row>
     <row r="453" spans="1:50">
       <c r="A453" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B453" s="5">
         <v>35803</v>
@@ -17705,7 +17705,7 @@
     </row>
     <row r="454" spans="1:50">
       <c r="A454" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B454" s="5">
         <v>35806</v>
@@ -17762,7 +17762,7 @@
     </row>
     <row r="455" spans="1:50">
       <c r="A455" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B455" s="5">
         <v>35808</v>
@@ -17795,7 +17795,7 @@
     </row>
     <row r="456" spans="1:50">
       <c r="A456" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B456" s="5">
         <v>35813</v>
@@ -17828,7 +17828,7 @@
     </row>
     <row r="457" spans="1:50">
       <c r="A457" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B457" s="5">
         <v>35814</v>
@@ -17864,7 +17864,7 @@
     </row>
     <row r="458" spans="1:50">
       <c r="A458" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B458" s="5">
         <v>35816</v>
@@ -17921,7 +17921,7 @@
     </row>
     <row r="459" spans="1:50">
       <c r="A459" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B459" s="5">
         <v>35817</v>
@@ -17966,7 +17966,7 @@
     </row>
     <row r="460" spans="1:50">
       <c r="A460" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B460" s="5">
         <v>35818</v>
@@ -17999,7 +17999,7 @@
     </row>
     <row r="461" spans="1:50">
       <c r="A461" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B461" s="5">
         <v>35820</v>
@@ -18032,7 +18032,7 @@
     </row>
     <row r="462" spans="1:50">
       <c r="A462" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B462" s="5">
         <v>35821</v>
@@ -18068,7 +18068,7 @@
     </row>
     <row r="463" spans="1:50">
       <c r="A463" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B463" s="5">
         <v>35824</v>
@@ -18104,7 +18104,7 @@
     </row>
     <row r="464" spans="1:50">
       <c r="A464" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B464" s="5">
         <v>35825</v>
@@ -18137,7 +18137,7 @@
     </row>
     <row r="465" spans="1:50">
       <c r="A465" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B465" s="5">
         <v>35826</v>
@@ -18173,7 +18173,7 @@
     </row>
     <row r="466" spans="1:50">
       <c r="A466" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B466" s="5">
         <v>35828</v>
@@ -18215,7 +18215,7 @@
     </row>
     <row r="467" spans="1:50">
       <c r="A467" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B467" s="5">
         <v>35829</v>
@@ -18248,7 +18248,7 @@
     </row>
     <row r="468" spans="1:50">
       <c r="A468" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B468" s="5">
         <v>35831</v>
@@ -18281,7 +18281,7 @@
     </row>
     <row r="469" spans="1:50">
       <c r="A469" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B469" s="5">
         <v>35832</v>
@@ -18317,7 +18317,7 @@
     </row>
     <row r="470" spans="1:50">
       <c r="A470" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B470" s="5">
         <v>35834</v>
@@ -18353,7 +18353,7 @@
     </row>
     <row r="471" spans="1:50">
       <c r="A471" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B471" s="5">
         <v>35835</v>
@@ -18389,7 +18389,7 @@
     </row>
     <row r="472" spans="1:50">
       <c r="A472" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B472" s="5">
         <v>35836</v>
@@ -18422,7 +18422,7 @@
     </row>
     <row r="473" spans="1:50">
       <c r="A473" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B473" s="5">
         <v>35838</v>
@@ -18458,7 +18458,7 @@
     </row>
     <row r="474" spans="1:50">
       <c r="A474" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B474" s="5">
         <v>35839</v>
@@ -18491,7 +18491,7 @@
     </row>
     <row r="475" spans="1:50">
       <c r="A475" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B475" s="5">
         <v>35841</v>
@@ -18533,7 +18533,7 @@
     </row>
     <row r="476" spans="1:50">
       <c r="A476" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B476" s="5">
         <v>35842</v>
@@ -18569,7 +18569,7 @@
     </row>
     <row r="477" spans="1:50">
       <c r="A477" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B477" s="5">
         <v>35844</v>
@@ -18617,7 +18617,7 @@
     </row>
     <row r="478" spans="1:50">
       <c r="A478" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B478" s="5">
         <v>35845</v>
@@ -18650,7 +18650,7 @@
     </row>
     <row r="479" spans="1:50">
       <c r="A479" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B479" s="5">
         <v>35846</v>
@@ -18710,7 +18710,7 @@
     </row>
     <row r="480" spans="1:50">
       <c r="A480" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B480" s="5">
         <v>35848</v>
@@ -18749,7 +18749,7 @@
     </row>
     <row r="481" spans="1:50">
       <c r="A481" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B481" s="5">
         <v>35849</v>
@@ -18782,7 +18782,7 @@
     </row>
     <row r="482" spans="1:50">
       <c r="A482" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B482" s="5">
         <v>35851</v>
@@ -18815,7 +18815,7 @@
     </row>
     <row r="483" spans="1:50">
       <c r="A483" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B483" s="5">
         <v>35852</v>
@@ -18854,7 +18854,7 @@
     </row>
     <row r="484" spans="1:50">
       <c r="A484" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B484" s="5">
         <v>35853</v>
@@ -18887,7 +18887,7 @@
     </row>
     <row r="485" spans="1:50">
       <c r="A485" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B485" s="5">
         <v>35854</v>
@@ -18920,7 +18920,7 @@
     </row>
     <row r="486" spans="1:50">
       <c r="A486" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B486" s="5">
         <v>35855</v>
@@ -18962,7 +18962,7 @@
     </row>
     <row r="487" spans="1:50">
       <c r="A487" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B487" s="5">
         <v>35856</v>
@@ -18998,7 +18998,7 @@
     </row>
     <row r="488" spans="1:50">
       <c r="A488" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B488" s="5">
         <v>35857</v>
@@ -19034,7 +19034,7 @@
     </row>
     <row r="489" spans="1:50">
       <c r="A489" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B489" s="5">
         <v>35858</v>
@@ -19067,7 +19067,7 @@
     </row>
     <row r="490" spans="1:50">
       <c r="A490" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B490" s="5">
         <v>35859</v>
@@ -19106,7 +19106,7 @@
     </row>
     <row r="491" spans="1:50">
       <c r="A491" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B491" s="5">
         <v>35860</v>
@@ -19142,7 +19142,7 @@
     </row>
     <row r="492" spans="1:50">
       <c r="A492" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B492" s="5">
         <v>35862</v>
@@ -19175,7 +19175,7 @@
     </row>
     <row r="493" spans="1:50">
       <c r="A493" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B493" s="5">
         <v>35864</v>
@@ -19217,7 +19217,7 @@
     </row>
     <row r="494" spans="1:50">
       <c r="A494" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B494" s="5">
         <v>35865</v>
@@ -19259,13 +19259,13 @@
     </row>
     <row r="495" spans="1:50">
       <c r="A495" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B495" s="5">
         <v>35866</v>
       </c>
       <c r="C495" s="5" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D495" s="6">
         <v>98.832891246684298</v>
@@ -19367,7 +19367,7 @@
     </row>
     <row r="496" spans="1:50">
       <c r="A496" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B496" s="5">
         <v>35867</v>
@@ -19403,7 +19403,7 @@
     </row>
     <row r="497" spans="1:36">
       <c r="A497" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B497" s="5">
         <v>35868</v>
@@ -19436,7 +19436,7 @@
     </row>
     <row r="498" spans="1:36">
       <c r="A498" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B498" s="5">
         <v>35870</v>
@@ -19469,7 +19469,7 @@
     </row>
     <row r="499" spans="1:36">
       <c r="A499" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B499" s="5">
         <v>35874</v>

</xml_diff>

<commit_message>
Cultivars more or less calibrated. Next step is looking at photoperiod sensitivity.
</commit_message>
<xml_diff>
--- a/Prototypes/Mungbean/Exp3observed.xlsx
+++ b/Prototypes/Mungbean/Exp3observed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pas075\Documents\ApsimX\Prototypes\Mungbean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B1E343E-4D49-47A9-A9D5-48FED1AF777E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81AC5934-06C2-49AA-9F8C-984272EE5EB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8C69385E-AA3F-4CF3-AF00-E1E4599E61EE}"/>
   </bookViews>
@@ -113,12 +113,6 @@
     <t>TotNO3160</t>
   </si>
   <si>
-    <t>Soybean.Phenology.FloweringDAS</t>
-  </si>
-  <si>
-    <t>Soybean.Phenology.EarlyPodDevelopmentDAS</t>
-  </si>
-  <si>
     <t>Soybean.Phenology.MaturityDAS</t>
   </si>
   <si>
@@ -216,6 +210,12 @@
   </si>
   <si>
     <t>Days after Sowing (usually first sowing)</t>
+  </si>
+  <si>
+    <t>Soybean.Phenology.StartPodDevDAS</t>
+  </si>
+  <si>
+    <t>Soybean.Phenology.StartFloweringDAS</t>
   </si>
 </sst>
 </file>
@@ -600,9 +600,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21968B1A-9F2D-47BD-B4B3-097E93366914}">
   <dimension ref="A1:AX499"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -619,16 +619,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>2</v>
@@ -664,7 +664,7 @@
         <v>12</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="S1" s="2" t="s">
         <v>13</v>
@@ -703,75 +703,75 @@
         <v>24</v>
       </c>
       <c r="AE1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AF1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AH1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AI1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AK1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AM1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AL1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AN1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AO1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AP1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="AO1" s="3" t="s">
+      <c r="AQ1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AP1" s="3" t="s">
+      <c r="AR1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="AQ1" s="3" t="s">
+      <c r="AS1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AR1" s="3" t="s">
+      <c r="AT1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AS1" s="3" t="s">
+      <c r="AU1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AT1" s="2" t="s">
+      <c r="AV1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="AU1" s="2" t="s">
+      <c r="AW1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AV1" s="3" t="s">
+      <c r="AX1" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="AW1" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="AX1" s="3" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:50">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B2" s="5">
         <v>35870</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D2" s="6">
         <v>102.83020062021301</v>
@@ -879,7 +879,7 @@
     </row>
     <row r="3" spans="1:50">
       <c r="A3" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B3" s="5">
         <v>35815</v>
@@ -936,7 +936,7 @@
     </row>
     <row r="4" spans="1:50">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B4" s="5">
         <v>35861</v>
@@ -990,7 +990,7 @@
     </row>
     <row r="5" spans="1:50">
       <c r="A5" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B5" s="5">
         <v>35843</v>
@@ -1062,7 +1062,7 @@
     </row>
     <row r="6" spans="1:50">
       <c r="A6" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B6" s="5">
         <v>35861</v>
@@ -1119,13 +1119,13 @@
     </row>
     <row r="7" spans="1:50">
       <c r="A7" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B7" s="5">
         <v>35866</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D7" s="6">
         <v>98.832891246684298</v>
@@ -1227,7 +1227,7 @@
     </row>
     <row r="8" spans="1:50">
       <c r="A8" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B8" s="5">
         <v>35846</v>
@@ -1287,7 +1287,7 @@
     </row>
     <row r="9" spans="1:50">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B9" s="5">
         <v>35815</v>
@@ -1344,13 +1344,13 @@
     </row>
     <row r="10" spans="1:50">
       <c r="A10" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B10" s="5">
         <v>35858</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D10" s="6">
         <v>90.914127423822606</v>
@@ -1446,7 +1446,7 @@
     </row>
     <row r="11" spans="1:50">
       <c r="A11" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B11" s="5">
         <v>35800</v>
@@ -1503,7 +1503,7 @@
     </row>
     <row r="12" spans="1:50">
       <c r="A12" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B12" s="5">
         <v>35828</v>
@@ -1563,7 +1563,7 @@
     </row>
     <row r="13" spans="1:50">
       <c r="A13" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B13" s="5">
         <v>35806</v>
@@ -1620,7 +1620,7 @@
     </row>
     <row r="14" spans="1:50">
       <c r="A14" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B14" s="5">
         <v>35828</v>
@@ -1677,13 +1677,13 @@
     </row>
     <row r="15" spans="1:50">
       <c r="A15" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B15" s="5">
         <v>35858</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D15" s="6">
         <v>90.557029177718803</v>
@@ -1791,7 +1791,7 @@
     </row>
     <row r="16" spans="1:50">
       <c r="A16" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B16" s="5">
         <v>35788</v>
@@ -1845,7 +1845,7 @@
     </row>
     <row r="17" spans="1:50">
       <c r="A17" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B17" s="5">
         <v>35843</v>
@@ -1914,13 +1914,13 @@
     </row>
     <row r="18" spans="1:50">
       <c r="A18" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B18" s="5">
         <v>35863</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D18" s="6">
         <v>95.5483163357178</v>
@@ -2022,7 +2022,7 @@
     </row>
     <row r="19" spans="1:50">
       <c r="A19" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B19" s="5">
         <v>35815</v>
@@ -2079,7 +2079,7 @@
     </row>
     <row r="20" spans="1:50">
       <c r="A20" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B20" s="5">
         <v>35861</v>
@@ -2136,7 +2136,7 @@
     </row>
     <row r="21" spans="1:50">
       <c r="A21" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B21" s="5">
         <v>35843</v>
@@ -2199,7 +2199,7 @@
     </row>
     <row r="22" spans="1:50">
       <c r="A22" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B22" s="5">
         <v>35782</v>
@@ -2247,7 +2247,7 @@
     </row>
     <row r="23" spans="1:50">
       <c r="A23" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B23" s="5">
         <v>35790</v>
@@ -2280,7 +2280,7 @@
     </row>
     <row r="24" spans="1:50">
       <c r="A24" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B24" s="5">
         <v>35795</v>
@@ -2313,7 +2313,7 @@
     </row>
     <row r="25" spans="1:50">
       <c r="A25" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B25" s="5">
         <v>35797</v>
@@ -2346,7 +2346,7 @@
     </row>
     <row r="26" spans="1:50">
       <c r="A26" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B26" s="5">
         <v>35800</v>
@@ -2379,7 +2379,7 @@
     </row>
     <row r="27" spans="1:50">
       <c r="A27" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B27" s="5">
         <v>35803</v>
@@ -2412,7 +2412,7 @@
     </row>
     <row r="28" spans="1:50">
       <c r="A28" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B28" s="5">
         <v>35807</v>
@@ -2445,7 +2445,7 @@
     </row>
     <row r="29" spans="1:50">
       <c r="A29" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B29" s="5">
         <v>35812</v>
@@ -2482,7 +2482,7 @@
     </row>
     <row r="30" spans="1:50">
       <c r="A30" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B30" s="5">
         <v>35813</v>
@@ -2515,7 +2515,7 @@
     </row>
     <row r="31" spans="1:50">
       <c r="A31" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B31" s="5">
         <v>35815</v>
@@ -2548,7 +2548,7 @@
     </row>
     <row r="32" spans="1:50">
       <c r="A32" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B32" s="5">
         <v>35816</v>
@@ -2584,7 +2584,7 @@
     </row>
     <row r="33" spans="1:50">
       <c r="A33" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B33" s="5">
         <v>35817</v>
@@ -2617,7 +2617,7 @@
     </row>
     <row r="34" spans="1:50">
       <c r="A34" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B34" s="5">
         <v>35818</v>
@@ -2650,7 +2650,7 @@
     </row>
     <row r="35" spans="1:50">
       <c r="A35" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B35" s="5">
         <v>35820</v>
@@ -2683,7 +2683,7 @@
     </row>
     <row r="36" spans="1:50">
       <c r="A36" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B36" s="5">
         <v>35824</v>
@@ -2716,7 +2716,7 @@
     </row>
     <row r="37" spans="1:50">
       <c r="A37" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B37" s="5">
         <v>35828</v>
@@ -2749,7 +2749,7 @@
     </row>
     <row r="38" spans="1:50">
       <c r="A38" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B38" s="5">
         <v>35830</v>
@@ -2788,7 +2788,7 @@
     </row>
     <row r="39" spans="1:50">
       <c r="A39" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B39" s="5">
         <v>35831</v>
@@ -2818,7 +2818,7 @@
     </row>
     <row r="40" spans="1:50">
       <c r="A40" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B40" s="5">
         <v>35833</v>
@@ -2854,7 +2854,7 @@
     </row>
     <row r="41" spans="1:50">
       <c r="A41" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B41" s="5">
         <v>35834</v>
@@ -2887,7 +2887,7 @@
     </row>
     <row r="42" spans="1:50">
       <c r="A42" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B42" s="5">
         <v>35836</v>
@@ -2920,7 +2920,7 @@
     </row>
     <row r="43" spans="1:50">
       <c r="A43" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B43" s="5">
         <v>35837</v>
@@ -2959,7 +2959,7 @@
     </row>
     <row r="44" spans="1:50">
       <c r="A44" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B44" s="5">
         <v>35839</v>
@@ -2992,7 +2992,7 @@
     </row>
     <row r="45" spans="1:50">
       <c r="A45" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B45" s="5">
         <v>35840</v>
@@ -3028,7 +3028,7 @@
     </row>
     <row r="46" spans="1:50">
       <c r="A46" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B46" s="5">
         <v>35842</v>
@@ -3070,7 +3070,7 @@
     </row>
     <row r="47" spans="1:50">
       <c r="A47" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B47" s="5">
         <v>35843</v>
@@ -3109,7 +3109,7 @@
     </row>
     <row r="48" spans="1:50">
       <c r="A48" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B48" s="5">
         <v>35844</v>
@@ -3154,7 +3154,7 @@
     </row>
     <row r="49" spans="1:48" ht="15.75" customHeight="1">
       <c r="A49" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B49" s="5">
         <v>35845</v>
@@ -3190,7 +3190,7 @@
     </row>
     <row r="50" spans="1:48">
       <c r="A50" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B50" s="5">
         <v>35848</v>
@@ -3223,7 +3223,7 @@
     </row>
     <row r="51" spans="1:48">
       <c r="A51" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B51" s="5">
         <v>35850</v>
@@ -3259,7 +3259,7 @@
     </row>
     <row r="52" spans="1:48">
       <c r="A52" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B52" s="5">
         <v>35851</v>
@@ -3292,7 +3292,7 @@
     </row>
     <row r="53" spans="1:48">
       <c r="A53" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B53" s="5">
         <v>35852</v>
@@ -3328,7 +3328,7 @@
     </row>
     <row r="54" spans="1:48">
       <c r="A54" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B54" s="5">
         <v>35853</v>
@@ -3361,7 +3361,7 @@
     </row>
     <row r="55" spans="1:48">
       <c r="A55" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B55" s="5">
         <v>35854</v>
@@ -3397,7 +3397,7 @@
     </row>
     <row r="56" spans="1:48">
       <c r="A56" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B56" s="5">
         <v>35855</v>
@@ -3430,7 +3430,7 @@
     </row>
     <row r="57" spans="1:48">
       <c r="A57" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B57" s="5">
         <v>35856</v>
@@ -3466,7 +3466,7 @@
     </row>
     <row r="58" spans="1:48">
       <c r="A58" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B58" s="5">
         <v>35857</v>
@@ -3526,7 +3526,7 @@
     </row>
     <row r="59" spans="1:48">
       <c r="A59" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B59" s="5">
         <v>35858</v>
@@ -3562,7 +3562,7 @@
     </row>
     <row r="60" spans="1:48">
       <c r="A60" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B60" s="5">
         <v>35859</v>
@@ -3595,7 +3595,7 @@
     </row>
     <row r="61" spans="1:48">
       <c r="A61" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B61" s="5">
         <v>35860</v>
@@ -3628,7 +3628,7 @@
     </row>
     <row r="62" spans="1:48">
       <c r="A62" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B62" s="5">
         <v>35861</v>
@@ -3661,7 +3661,7 @@
     </row>
     <row r="63" spans="1:48">
       <c r="A63" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B63" s="5">
         <v>35862</v>
@@ -3694,7 +3694,7 @@
     </row>
     <row r="64" spans="1:48">
       <c r="A64" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B64" s="5">
         <v>35863</v>
@@ -3727,7 +3727,7 @@
     </row>
     <row r="65" spans="1:49">
       <c r="A65" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B65" s="5">
         <v>35864</v>
@@ -3763,7 +3763,7 @@
     </row>
     <row r="66" spans="1:49">
       <c r="A66" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B66" s="5">
         <v>35865</v>
@@ -3796,7 +3796,7 @@
     </row>
     <row r="67" spans="1:49">
       <c r="A67" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B67" s="5">
         <v>35866</v>
@@ -3829,7 +3829,7 @@
     </row>
     <row r="68" spans="1:49">
       <c r="A68" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B68" s="5">
         <v>35868</v>
@@ -3859,7 +3859,7 @@
     </row>
     <row r="69" spans="1:49">
       <c r="A69" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B69" s="5">
         <v>35869</v>
@@ -3892,7 +3892,7 @@
     </row>
     <row r="70" spans="1:49">
       <c r="A70" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B70" s="5">
         <v>35870</v>
@@ -3931,13 +3931,13 @@
     </row>
     <row r="71" spans="1:49">
       <c r="A71" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B71" s="5">
         <v>35871</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D71" s="6">
         <v>104.081291759465</v>
@@ -4009,7 +4009,7 @@
     </row>
     <row r="72" spans="1:49">
       <c r="A72" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B72" s="5">
         <v>35872</v>
@@ -4042,7 +4042,7 @@
     </row>
     <row r="73" spans="1:49">
       <c r="A73" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B73" s="5">
         <v>35873</v>
@@ -4075,7 +4075,7 @@
     </row>
     <row r="74" spans="1:49">
       <c r="A74" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B74" s="5">
         <v>35876</v>
@@ -4108,7 +4108,7 @@
     </row>
     <row r="75" spans="1:49">
       <c r="A75" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B75" s="5">
         <v>35877</v>
@@ -4141,7 +4141,7 @@
     </row>
     <row r="76" spans="1:49">
       <c r="A76" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B76" s="5">
         <v>35878</v>
@@ -4174,7 +4174,7 @@
     </row>
     <row r="77" spans="1:49">
       <c r="A77" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B77" s="5">
         <v>35879</v>
@@ -4210,7 +4210,7 @@
     </row>
     <row r="78" spans="1:49">
       <c r="A78" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B78" s="5">
         <v>35881</v>
@@ -4246,7 +4246,7 @@
     </row>
     <row r="79" spans="1:49">
       <c r="A79" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B79" s="5">
         <v>35882</v>
@@ -4303,7 +4303,7 @@
     </row>
     <row r="80" spans="1:49">
       <c r="A80" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B80" s="5">
         <v>35884</v>
@@ -4336,7 +4336,7 @@
     </row>
     <row r="81" spans="1:36">
       <c r="A81" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B81" s="5">
         <v>35885</v>
@@ -4375,7 +4375,7 @@
     </row>
     <row r="82" spans="1:36">
       <c r="A82" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B82" s="5">
         <v>35886</v>
@@ -4411,7 +4411,7 @@
     </row>
     <row r="83" spans="1:36">
       <c r="A83" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B83" s="5">
         <v>35782</v>
@@ -4444,7 +4444,7 @@
     </row>
     <row r="84" spans="1:36">
       <c r="A84" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B84" s="5">
         <v>35790</v>
@@ -4477,7 +4477,7 @@
     </row>
     <row r="85" spans="1:36">
       <c r="A85" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B85" s="5">
         <v>35795</v>
@@ -4510,7 +4510,7 @@
     </row>
     <row r="86" spans="1:36">
       <c r="A86" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B86" s="5">
         <v>35797</v>
@@ -4543,7 +4543,7 @@
     </row>
     <row r="87" spans="1:36">
       <c r="A87" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B87" s="5">
         <v>35801</v>
@@ -4576,7 +4576,7 @@
     </row>
     <row r="88" spans="1:36">
       <c r="A88" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B88" s="5">
         <v>35803</v>
@@ -4609,7 +4609,7 @@
     </row>
     <row r="89" spans="1:36">
       <c r="A89" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B89" s="5">
         <v>35807</v>
@@ -4642,7 +4642,7 @@
     </row>
     <row r="90" spans="1:36">
       <c r="A90" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B90" s="5">
         <v>35813</v>
@@ -4675,7 +4675,7 @@
     </row>
     <row r="91" spans="1:36">
       <c r="A91" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B91" s="5">
         <v>35816</v>
@@ -4711,7 +4711,7 @@
     </row>
     <row r="92" spans="1:36">
       <c r="A92" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B92" s="5">
         <v>35817</v>
@@ -4747,7 +4747,7 @@
     </row>
     <row r="93" spans="1:36">
       <c r="A93" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B93" s="5">
         <v>35818</v>
@@ -4780,7 +4780,7 @@
     </row>
     <row r="94" spans="1:36">
       <c r="A94" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B94" s="5">
         <v>35820</v>
@@ -4813,7 +4813,7 @@
     </row>
     <row r="95" spans="1:36">
       <c r="A95" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B95" s="5">
         <v>35824</v>
@@ -4846,7 +4846,7 @@
     </row>
     <row r="96" spans="1:36">
       <c r="A96" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B96" s="5">
         <v>35829</v>
@@ -4885,7 +4885,7 @@
     </row>
     <row r="97" spans="1:42">
       <c r="A97" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B97" s="5">
         <v>35830</v>
@@ -4921,7 +4921,7 @@
     </row>
     <row r="98" spans="1:42">
       <c r="A98" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B98" s="5">
         <v>35831</v>
@@ -4957,7 +4957,7 @@
     </row>
     <row r="99" spans="1:42">
       <c r="A99" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B99" s="5">
         <v>35832</v>
@@ -4990,7 +4990,7 @@
     </row>
     <row r="100" spans="1:42">
       <c r="A100" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B100" s="5">
         <v>35833</v>
@@ -5026,7 +5026,7 @@
     </row>
     <row r="101" spans="1:42">
       <c r="A101" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B101" s="5">
         <v>35835</v>
@@ -5062,7 +5062,7 @@
     </row>
     <row r="102" spans="1:42">
       <c r="A102" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B102" s="5">
         <v>35836</v>
@@ -5098,7 +5098,7 @@
     </row>
     <row r="103" spans="1:42">
       <c r="A103" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B103" s="5">
         <v>35838</v>
@@ -5131,7 +5131,7 @@
     </row>
     <row r="104" spans="1:42">
       <c r="A104" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B104" s="5">
         <v>35839</v>
@@ -5164,7 +5164,7 @@
     </row>
     <row r="105" spans="1:42">
       <c r="A105" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B105" s="5">
         <v>35840</v>
@@ -5200,7 +5200,7 @@
     </row>
     <row r="106" spans="1:42">
       <c r="A106" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B106" s="5">
         <v>35841</v>
@@ -5233,7 +5233,7 @@
     </row>
     <row r="107" spans="1:42">
       <c r="A107" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B107" s="5">
         <v>35842</v>
@@ -5272,7 +5272,7 @@
     </row>
     <row r="108" spans="1:42">
       <c r="A108" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B108" s="5">
         <v>35844</v>
@@ -5317,7 +5317,7 @@
     </row>
     <row r="109" spans="1:42">
       <c r="A109" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B109" s="5">
         <v>35846</v>
@@ -5350,7 +5350,7 @@
     </row>
     <row r="110" spans="1:42">
       <c r="A110" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B110" s="5">
         <v>35848</v>
@@ -5386,7 +5386,7 @@
     </row>
     <row r="111" spans="1:42">
       <c r="A111" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B111" s="5">
         <v>35849</v>
@@ -5422,7 +5422,7 @@
     </row>
     <row r="112" spans="1:42">
       <c r="A112" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B112" s="5">
         <v>35851</v>
@@ -5455,7 +5455,7 @@
     </row>
     <row r="113" spans="1:48">
       <c r="A113" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B113" s="5">
         <v>35852</v>
@@ -5491,7 +5491,7 @@
     </row>
     <row r="114" spans="1:48">
       <c r="A114" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B114" s="5">
         <v>35853</v>
@@ -5524,7 +5524,7 @@
     </row>
     <row r="115" spans="1:48">
       <c r="A115" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B115" s="5">
         <v>35854</v>
@@ -5557,7 +5557,7 @@
     </row>
     <row r="116" spans="1:48">
       <c r="A116" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B116" s="5">
         <v>35855</v>
@@ -5599,7 +5599,7 @@
     </row>
     <row r="117" spans="1:48" ht="15.75" customHeight="1">
       <c r="A117" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B117" s="5">
         <v>35856</v>
@@ -5635,7 +5635,7 @@
     </row>
     <row r="118" spans="1:48">
       <c r="A118" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B118" s="5">
         <v>35857</v>
@@ -5680,7 +5680,7 @@
     </row>
     <row r="119" spans="1:48">
       <c r="A119" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B119" s="5">
         <v>35858</v>
@@ -5719,7 +5719,7 @@
     </row>
     <row r="120" spans="1:48">
       <c r="A120" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B120" s="5">
         <v>35859</v>
@@ -5755,7 +5755,7 @@
     </row>
     <row r="121" spans="1:48">
       <c r="A121" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B121" s="5">
         <v>35860</v>
@@ -5791,13 +5791,13 @@
     </row>
     <row r="122" spans="1:48">
       <c r="A122" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B122" s="5">
         <v>35863</v>
       </c>
       <c r="C122" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D122" s="6">
         <v>96.424668665414998</v>
@@ -5863,7 +5863,7 @@
     </row>
     <row r="123" spans="1:48">
       <c r="A123" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B123" s="5">
         <v>35864</v>
@@ -5899,7 +5899,7 @@
     </row>
     <row r="124" spans="1:48">
       <c r="A124" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B124" s="5">
         <v>35865</v>
@@ -5932,7 +5932,7 @@
     </row>
     <row r="125" spans="1:48">
       <c r="A125" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B125" s="5">
         <v>35868</v>
@@ -5965,7 +5965,7 @@
     </row>
     <row r="126" spans="1:48">
       <c r="A126" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B126" s="5">
         <v>35869</v>
@@ -5998,7 +5998,7 @@
     </row>
     <row r="127" spans="1:48">
       <c r="A127" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B127" s="5">
         <v>35870</v>
@@ -6040,7 +6040,7 @@
     </row>
     <row r="128" spans="1:48">
       <c r="A128" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B128" s="5">
         <v>35871</v>
@@ -6076,7 +6076,7 @@
     </row>
     <row r="129" spans="1:50">
       <c r="A129" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B129" s="5">
         <v>35872</v>
@@ -6112,7 +6112,7 @@
     </row>
     <row r="130" spans="1:50">
       <c r="A130" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B130" s="5">
         <v>35873</v>
@@ -6145,7 +6145,7 @@
     </row>
     <row r="131" spans="1:50">
       <c r="A131" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B131" s="5">
         <v>35875</v>
@@ -6187,7 +6187,7 @@
     </row>
     <row r="132" spans="1:50">
       <c r="A132" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B132" s="5">
         <v>35876</v>
@@ -6220,7 +6220,7 @@
     </row>
     <row r="133" spans="1:50">
       <c r="A133" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B133" s="5">
         <v>35877</v>
@@ -6283,7 +6283,7 @@
     </row>
     <row r="134" spans="1:50">
       <c r="A134" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B134" s="5">
         <v>35782</v>
@@ -6316,7 +6316,7 @@
     </row>
     <row r="135" spans="1:50">
       <c r="A135" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B135" s="5">
         <v>35775</v>
@@ -6349,7 +6349,7 @@
     </row>
     <row r="136" spans="1:50">
       <c r="A136" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B136" s="5">
         <v>35790</v>
@@ -6382,7 +6382,7 @@
     </row>
     <row r="137" spans="1:50">
       <c r="A137" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B137" s="5">
         <v>35796</v>
@@ -6415,7 +6415,7 @@
     </row>
     <row r="138" spans="1:50">
       <c r="A138" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B138" s="5">
         <v>35799</v>
@@ -6448,7 +6448,7 @@
     </row>
     <row r="139" spans="1:50">
       <c r="A139" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B139" s="5">
         <v>35803</v>
@@ -6481,7 +6481,7 @@
     </row>
     <row r="140" spans="1:50">
       <c r="A140" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B140" s="5">
         <v>35804</v>
@@ -6514,7 +6514,7 @@
     </row>
     <row r="141" spans="1:50">
       <c r="A141" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B141" s="5">
         <v>35808</v>
@@ -6547,7 +6547,7 @@
     </row>
     <row r="142" spans="1:50">
       <c r="A142" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B142" s="5">
         <v>35812</v>
@@ -6584,7 +6584,7 @@
     </row>
     <row r="143" spans="1:50">
       <c r="A143" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B143" s="5">
         <v>35813</v>
@@ -6617,7 +6617,7 @@
     </row>
     <row r="144" spans="1:50">
       <c r="A144" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B144" s="5">
         <v>35816</v>
@@ -6656,7 +6656,7 @@
     </row>
     <row r="145" spans="1:50">
       <c r="A145" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B145" s="5">
         <v>35817</v>
@@ -6695,7 +6695,7 @@
     </row>
     <row r="146" spans="1:50">
       <c r="A146" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B146" s="5">
         <v>35820</v>
@@ -6731,7 +6731,7 @@
     </row>
     <row r="147" spans="1:50">
       <c r="A147" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B147" s="5">
         <v>35823</v>
@@ -6767,7 +6767,7 @@
     </row>
     <row r="148" spans="1:50">
       <c r="A148" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B148" s="5">
         <v>35824</v>
@@ -6806,7 +6806,7 @@
     </row>
     <row r="149" spans="1:50">
       <c r="A149" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B149" s="5">
         <v>35829</v>
@@ -6839,7 +6839,7 @@
     </row>
     <row r="150" spans="1:50">
       <c r="A150" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B150" s="5">
         <v>35830</v>
@@ -6872,7 +6872,7 @@
     </row>
     <row r="151" spans="1:50">
       <c r="A151" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B151" s="5">
         <v>35831</v>
@@ -6908,7 +6908,7 @@
     </row>
     <row r="152" spans="1:50">
       <c r="A152" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B152" s="5">
         <v>35832</v>
@@ -6941,7 +6941,7 @@
     </row>
     <row r="153" spans="1:50">
       <c r="A153" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B153" s="5">
         <v>35833</v>
@@ -6974,7 +6974,7 @@
     </row>
     <row r="154" spans="1:50">
       <c r="A154" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B154" s="5">
         <v>35834</v>
@@ -7010,7 +7010,7 @@
     </row>
     <row r="155" spans="1:50">
       <c r="A155" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B155" s="5">
         <v>35835</v>
@@ -7043,7 +7043,7 @@
     </row>
     <row r="156" spans="1:50">
       <c r="A156" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B156" s="5">
         <v>35837</v>
@@ -7085,7 +7085,7 @@
     </row>
     <row r="157" spans="1:50">
       <c r="A157" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B157" s="5">
         <v>35838</v>
@@ -7118,7 +7118,7 @@
     </row>
     <row r="158" spans="1:50">
       <c r="A158" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B158" s="5">
         <v>35839</v>
@@ -7151,7 +7151,7 @@
     </row>
     <row r="159" spans="1:50">
       <c r="A159" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B159" s="5">
         <v>35841</v>
@@ -7202,7 +7202,7 @@
     </row>
     <row r="160" spans="1:50">
       <c r="A160" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B160" s="5">
         <v>35842</v>
@@ -7238,7 +7238,7 @@
     </row>
     <row r="161" spans="1:48">
       <c r="A161" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B161" s="5">
         <v>35843</v>
@@ -7274,7 +7274,7 @@
     </row>
     <row r="162" spans="1:48">
       <c r="A162" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B162" s="5">
         <v>35844</v>
@@ -7316,7 +7316,7 @@
     </row>
     <row r="163" spans="1:48">
       <c r="A163" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B163" s="5">
         <v>35846</v>
@@ -7349,7 +7349,7 @@
     </row>
     <row r="164" spans="1:48">
       <c r="A164" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B164" s="5">
         <v>35847</v>
@@ -7382,7 +7382,7 @@
     </row>
     <row r="165" spans="1:48">
       <c r="A165" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B165" s="5">
         <v>35848</v>
@@ -7418,7 +7418,7 @@
     </row>
     <row r="166" spans="1:48">
       <c r="A166" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B166" s="5">
         <v>35849</v>
@@ -7451,7 +7451,7 @@
     </row>
     <row r="167" spans="1:48">
       <c r="A167" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B167" s="5">
         <v>35851</v>
@@ -7487,7 +7487,7 @@
     </row>
     <row r="168" spans="1:48">
       <c r="A168" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B168" s="5">
         <v>35852</v>
@@ -7526,7 +7526,7 @@
     </row>
     <row r="169" spans="1:48">
       <c r="A169" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B169" s="5">
         <v>35853</v>
@@ -7559,7 +7559,7 @@
     </row>
     <row r="170" spans="1:48">
       <c r="A170" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B170" s="5">
         <v>35854</v>
@@ -7598,7 +7598,7 @@
     </row>
     <row r="171" spans="1:48" ht="16.5" customHeight="1">
       <c r="A171" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B171" s="5">
         <v>35855</v>
@@ -7631,7 +7631,7 @@
     </row>
     <row r="172" spans="1:48">
       <c r="A172" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B172" s="5">
         <v>35856</v>
@@ -7664,7 +7664,7 @@
     </row>
     <row r="173" spans="1:48">
       <c r="A173" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B173" s="5">
         <v>35857</v>
@@ -7715,7 +7715,7 @@
     </row>
     <row r="174" spans="1:48">
       <c r="A174" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B174" s="5">
         <v>35858</v>
@@ -7751,7 +7751,7 @@
     </row>
     <row r="175" spans="1:48">
       <c r="A175" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B175" s="5">
         <v>35859</v>
@@ -7787,7 +7787,7 @@
     </row>
     <row r="176" spans="1:48">
       <c r="A176" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B176" s="5">
         <v>35862</v>
@@ -7823,7 +7823,7 @@
     </row>
     <row r="177" spans="1:50">
       <c r="A177" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B177" s="5">
         <v>35864</v>
@@ -7856,7 +7856,7 @@
     </row>
     <row r="178" spans="1:50">
       <c r="A178" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B178" s="5">
         <v>35865</v>
@@ -7889,7 +7889,7 @@
     </row>
     <row r="179" spans="1:50">
       <c r="A179" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B179" s="5">
         <v>35868</v>
@@ -7925,7 +7925,7 @@
     </row>
     <row r="180" spans="1:50">
       <c r="A180" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B180" s="5">
         <v>35869</v>
@@ -7964,7 +7964,7 @@
     </row>
     <row r="181" spans="1:50">
       <c r="A181" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B181" s="5">
         <v>35870</v>
@@ -7997,7 +7997,7 @@
     </row>
     <row r="182" spans="1:50">
       <c r="A182" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B182" s="5">
         <v>35871</v>
@@ -8042,7 +8042,7 @@
     </row>
     <row r="183" spans="1:50">
       <c r="A183" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B183" s="5">
         <v>35872</v>
@@ -8084,7 +8084,7 @@
     </row>
     <row r="184" spans="1:50">
       <c r="A184" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B184" s="5">
         <v>35875</v>
@@ -8120,7 +8120,7 @@
     </row>
     <row r="185" spans="1:50">
       <c r="A185" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B185" s="5">
         <v>35876</v>
@@ -8156,7 +8156,7 @@
     </row>
     <row r="186" spans="1:50">
       <c r="A186" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B186" s="5">
         <v>35877</v>
@@ -8210,7 +8210,7 @@
     </row>
     <row r="187" spans="1:50">
       <c r="A187" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B187" s="5">
         <v>35881</v>
@@ -8243,7 +8243,7 @@
     </row>
     <row r="188" spans="1:50">
       <c r="A188" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B188" s="5">
         <v>35795</v>
@@ -8276,7 +8276,7 @@
     </row>
     <row r="189" spans="1:50">
       <c r="A189" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B189" s="5">
         <v>35799</v>
@@ -8312,7 +8312,7 @@
     </row>
     <row r="190" spans="1:50">
       <c r="A190" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B190" s="5">
         <v>35801</v>
@@ -8345,7 +8345,7 @@
     </row>
     <row r="191" spans="1:50">
       <c r="A191" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B191" s="5">
         <v>35804</v>
@@ -8378,7 +8378,7 @@
     </row>
     <row r="192" spans="1:50">
       <c r="A192" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B192" s="5">
         <v>35808</v>
@@ -8411,7 +8411,7 @@
     </row>
     <row r="193" spans="1:50">
       <c r="A193" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B193" s="5">
         <v>35814</v>
@@ -8444,7 +8444,7 @@
     </row>
     <row r="194" spans="1:50">
       <c r="A194" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B194" s="5">
         <v>35815</v>
@@ -8477,7 +8477,7 @@
     </row>
     <row r="195" spans="1:50">
       <c r="A195" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B195" s="5">
         <v>35816</v>
@@ -8513,7 +8513,7 @@
     </row>
     <row r="196" spans="1:50">
       <c r="A196" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B196" s="5">
         <v>35817</v>
@@ -8549,7 +8549,7 @@
     </row>
     <row r="197" spans="1:50">
       <c r="A197" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B197" s="5">
         <v>35820</v>
@@ -8582,7 +8582,7 @@
     </row>
     <row r="198" spans="1:50">
       <c r="A198" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B198" s="5">
         <v>35824</v>
@@ -8615,7 +8615,7 @@
     </row>
     <row r="199" spans="1:50">
       <c r="A199" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B199" s="5">
         <v>35828</v>
@@ -8654,7 +8654,7 @@
     </row>
     <row r="200" spans="1:50">
       <c r="A200" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B200" s="5">
         <v>35834</v>
@@ -8687,7 +8687,7 @@
     </row>
     <row r="201" spans="1:50">
       <c r="A201" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B201" s="5">
         <v>35836</v>
@@ -8720,7 +8720,7 @@
     </row>
     <row r="202" spans="1:50">
       <c r="A202" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B202" s="5">
         <v>35837</v>
@@ -8753,7 +8753,7 @@
     </row>
     <row r="203" spans="1:50">
       <c r="A203" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B203" s="5">
         <v>35838</v>
@@ -8786,7 +8786,7 @@
     </row>
     <row r="204" spans="1:50">
       <c r="A204" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B204" s="5">
         <v>35839</v>
@@ -8819,7 +8819,7 @@
     </row>
     <row r="205" spans="1:50">
       <c r="A205" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B205" s="5">
         <v>35840</v>
@@ -8852,7 +8852,7 @@
     </row>
     <row r="206" spans="1:50">
       <c r="A206" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B206" s="5">
         <v>35841</v>
@@ -8888,7 +8888,7 @@
     </row>
     <row r="207" spans="1:50">
       <c r="A207" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B207" s="5">
         <v>35842</v>
@@ -8921,7 +8921,7 @@
     </row>
     <row r="208" spans="1:50">
       <c r="A208" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B208" s="5">
         <v>35843</v>
@@ -8963,7 +8963,7 @@
     </row>
     <row r="209" spans="1:48">
       <c r="A209" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B209" s="5">
         <v>35844</v>
@@ -9005,7 +9005,7 @@
     </row>
     <row r="210" spans="1:48">
       <c r="A210" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B210" s="5">
         <v>35845</v>
@@ -9041,7 +9041,7 @@
     </row>
     <row r="211" spans="1:48">
       <c r="A211" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B211" s="5">
         <v>35848</v>
@@ -9074,7 +9074,7 @@
     </row>
     <row r="212" spans="1:48">
       <c r="A212" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B212" s="5">
         <v>35850</v>
@@ -9107,7 +9107,7 @@
     </row>
     <row r="213" spans="1:48">
       <c r="A213" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B213" s="5">
         <v>35851</v>
@@ -9140,7 +9140,7 @@
     </row>
     <row r="214" spans="1:48">
       <c r="A214" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B214" s="5">
         <v>35852</v>
@@ -9179,7 +9179,7 @@
     </row>
     <row r="215" spans="1:48">
       <c r="A215" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B215" s="5">
         <v>35854</v>
@@ -9212,7 +9212,7 @@
     </row>
     <row r="216" spans="1:48">
       <c r="A216" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B216" s="5">
         <v>35855</v>
@@ -9251,7 +9251,7 @@
     </row>
     <row r="217" spans="1:48">
       <c r="A217" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B217" s="5">
         <v>35856</v>
@@ -9284,7 +9284,7 @@
     </row>
     <row r="218" spans="1:48">
       <c r="A218" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B218" s="5">
         <v>35857</v>
@@ -9335,7 +9335,7 @@
     </row>
     <row r="219" spans="1:48">
       <c r="A219" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B219" s="5">
         <v>35858</v>
@@ -9377,7 +9377,7 @@
     </row>
     <row r="220" spans="1:48">
       <c r="A220" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B220" s="5">
         <v>35859</v>
@@ -9413,7 +9413,7 @@
     </row>
     <row r="221" spans="1:48">
       <c r="A221" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B221" s="5">
         <v>35860</v>
@@ -9446,7 +9446,7 @@
     </row>
     <row r="222" spans="1:48">
       <c r="A222" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B222" s="5">
         <v>35861</v>
@@ -9479,7 +9479,7 @@
     </row>
     <row r="223" spans="1:48">
       <c r="A223" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B223" s="5">
         <v>35862</v>
@@ -9512,7 +9512,7 @@
     </row>
     <row r="224" spans="1:48">
       <c r="A224" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B224" s="5">
         <v>35863</v>
@@ -9548,7 +9548,7 @@
     </row>
     <row r="225" spans="1:50">
       <c r="A225" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B225" s="5">
         <v>35864</v>
@@ -9581,7 +9581,7 @@
     </row>
     <row r="226" spans="1:50">
       <c r="A226" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B226" s="5">
         <v>35865</v>
@@ -9614,7 +9614,7 @@
     </row>
     <row r="227" spans="1:50">
       <c r="A227" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B227" s="5">
         <v>35866</v>
@@ -9647,7 +9647,7 @@
     </row>
     <row r="228" spans="1:50">
       <c r="A228" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B228" s="5">
         <v>35868</v>
@@ -9680,7 +9680,7 @@
     </row>
     <row r="229" spans="1:50">
       <c r="A229" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B229" s="5">
         <v>35869</v>
@@ -9713,7 +9713,7 @@
     </row>
     <row r="230" spans="1:50">
       <c r="A230" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B230" s="5">
         <v>35870</v>
@@ -9755,7 +9755,7 @@
     </row>
     <row r="231" spans="1:50">
       <c r="A231" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B231" s="5">
         <v>35871</v>
@@ -9791,13 +9791,13 @@
     </row>
     <row r="232" spans="1:50">
       <c r="A232" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B232" s="5">
         <v>35872</v>
       </c>
       <c r="C232" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D232" s="6">
         <v>104.649220489977</v>
@@ -9866,7 +9866,7 @@
     </row>
     <row r="233" spans="1:50">
       <c r="A233" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B233" s="5">
         <v>35873</v>
@@ -9899,7 +9899,7 @@
     </row>
     <row r="234" spans="1:50">
       <c r="A234" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B234" s="5">
         <v>35876</v>
@@ -9935,7 +9935,7 @@
     </row>
     <row r="235" spans="1:50">
       <c r="A235" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B235" s="5">
         <v>35878</v>
@@ -9968,7 +9968,7 @@
     </row>
     <row r="236" spans="1:50">
       <c r="A236" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B236" s="5">
         <v>35879</v>
@@ -10004,7 +10004,7 @@
     </row>
     <row r="237" spans="1:50">
       <c r="A237" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B237" s="5">
         <v>35882</v>
@@ -10040,7 +10040,7 @@
     </row>
     <row r="238" spans="1:50">
       <c r="A238" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B238" s="5">
         <v>35884</v>
@@ -10082,7 +10082,7 @@
     </row>
     <row r="239" spans="1:50">
       <c r="A239" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B239" s="5">
         <v>35885</v>
@@ -10124,7 +10124,7 @@
     </row>
     <row r="240" spans="1:50">
       <c r="A240" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B240" s="5">
         <v>35889</v>
@@ -10157,7 +10157,7 @@
     </row>
     <row r="241" spans="1:49">
       <c r="A241" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B241" s="5">
         <v>35893</v>
@@ -10196,7 +10196,7 @@
     </row>
     <row r="242" spans="1:49">
       <c r="A242" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B242" s="5">
         <v>35897</v>
@@ -10229,7 +10229,7 @@
     </row>
     <row r="243" spans="1:49">
       <c r="A243" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B243" s="5">
         <v>35898</v>
@@ -10262,7 +10262,7 @@
     </row>
     <row r="244" spans="1:49">
       <c r="A244" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B244" s="5">
         <v>35899</v>
@@ -10325,7 +10325,7 @@
     </row>
     <row r="245" spans="1:49">
       <c r="A245" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B245" s="5">
         <v>35795</v>
@@ -10358,7 +10358,7 @@
     </row>
     <row r="246" spans="1:49">
       <c r="A246" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B246" s="5">
         <v>35802</v>
@@ -10391,7 +10391,7 @@
     </row>
     <row r="247" spans="1:49">
       <c r="A247" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B247" s="5">
         <v>35804</v>
@@ -10424,7 +10424,7 @@
     </row>
     <row r="248" spans="1:49">
       <c r="A248" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B248" s="5">
         <v>35808</v>
@@ -10457,7 +10457,7 @@
     </row>
     <row r="249" spans="1:49">
       <c r="A249" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B249" s="5">
         <v>35814</v>
@@ -10490,7 +10490,7 @@
     </row>
     <row r="250" spans="1:49">
       <c r="A250" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B250" s="5">
         <v>35816</v>
@@ -10526,7 +10526,7 @@
     </row>
     <row r="251" spans="1:49">
       <c r="A251" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B251" s="5">
         <v>35817</v>
@@ -10562,7 +10562,7 @@
     </row>
     <row r="252" spans="1:49">
       <c r="A252" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B252" s="5">
         <v>35818</v>
@@ -10595,7 +10595,7 @@
     </row>
     <row r="253" spans="1:49">
       <c r="A253" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B253" s="5">
         <v>35820</v>
@@ -10628,7 +10628,7 @@
     </row>
     <row r="254" spans="1:49">
       <c r="A254" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B254" s="5">
         <v>35825</v>
@@ -10661,7 +10661,7 @@
     </row>
     <row r="255" spans="1:49">
       <c r="A255" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B255" s="5">
         <v>35829</v>
@@ -10694,7 +10694,7 @@
     </row>
     <row r="256" spans="1:49">
       <c r="A256" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B256" s="5">
         <v>35834</v>
@@ -10727,7 +10727,7 @@
     </row>
     <row r="257" spans="1:42">
       <c r="A257" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B257" s="5">
         <v>35835</v>
@@ -10763,7 +10763,7 @@
     </row>
     <row r="258" spans="1:42">
       <c r="A258" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B258" s="5">
         <v>35836</v>
@@ -10796,7 +10796,7 @@
     </row>
     <row r="259" spans="1:42">
       <c r="A259" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B259" s="5">
         <v>35838</v>
@@ -10829,7 +10829,7 @@
     </row>
     <row r="260" spans="1:42">
       <c r="A260" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B260" s="5">
         <v>35839</v>
@@ -10865,7 +10865,7 @@
     </row>
     <row r="261" spans="1:42">
       <c r="A261" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B261" s="5">
         <v>35840</v>
@@ -10898,7 +10898,7 @@
     </row>
     <row r="262" spans="1:42">
       <c r="A262" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B262" s="5">
         <v>35841</v>
@@ -10934,7 +10934,7 @@
     </row>
     <row r="263" spans="1:42">
       <c r="A263" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B263" s="5">
         <v>35842</v>
@@ -10973,7 +10973,7 @@
     </row>
     <row r="264" spans="1:42">
       <c r="A264" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B264" s="5">
         <v>35844</v>
@@ -11018,7 +11018,7 @@
     </row>
     <row r="265" spans="1:42">
       <c r="A265" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B265" s="5">
         <v>35845</v>
@@ -11051,7 +11051,7 @@
     </row>
     <row r="266" spans="1:42">
       <c r="A266" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B266" s="5">
         <v>35847</v>
@@ -11084,7 +11084,7 @@
     </row>
     <row r="267" spans="1:42">
       <c r="A267" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B267" s="5">
         <v>35849</v>
@@ -11120,7 +11120,7 @@
     </row>
     <row r="268" spans="1:42">
       <c r="A268" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B268" s="5">
         <v>35850</v>
@@ -11153,7 +11153,7 @@
     </row>
     <row r="269" spans="1:42">
       <c r="A269" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B269" s="5">
         <v>35851</v>
@@ -11186,7 +11186,7 @@
     </row>
     <row r="270" spans="1:42">
       <c r="A270" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B270" s="5">
         <v>35852</v>
@@ -11219,7 +11219,7 @@
     </row>
     <row r="271" spans="1:42">
       <c r="A271" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B271" s="5">
         <v>35853</v>
@@ -11252,7 +11252,7 @@
     </row>
     <row r="272" spans="1:42">
       <c r="A272" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B272" s="5">
         <v>35854</v>
@@ -11291,7 +11291,7 @@
     </row>
     <row r="273" spans="1:48">
       <c r="A273" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B273" s="5">
         <v>35855</v>
@@ -11327,7 +11327,7 @@
     </row>
     <row r="274" spans="1:48">
       <c r="A274" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B274" s="5">
         <v>35856</v>
@@ -11363,7 +11363,7 @@
     </row>
     <row r="275" spans="1:48">
       <c r="A275" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B275" s="5">
         <v>35857</v>
@@ -11423,7 +11423,7 @@
     </row>
     <row r="276" spans="1:48">
       <c r="A276" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B276" s="5">
         <v>35859</v>
@@ -11459,7 +11459,7 @@
     </row>
     <row r="277" spans="1:48">
       <c r="A277" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B277" s="5">
         <v>35860</v>
@@ -11492,7 +11492,7 @@
     </row>
     <row r="278" spans="1:48">
       <c r="A278" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B278" s="5">
         <v>35862</v>
@@ -11525,7 +11525,7 @@
     </row>
     <row r="279" spans="1:48">
       <c r="A279" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B279" s="5">
         <v>35863</v>
@@ -11558,7 +11558,7 @@
     </row>
     <row r="280" spans="1:48">
       <c r="A280" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B280" s="5">
         <v>35864</v>
@@ -11591,7 +11591,7 @@
     </row>
     <row r="281" spans="1:48">
       <c r="A281" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B281" s="5">
         <v>35865</v>
@@ -11627,7 +11627,7 @@
     </row>
     <row r="282" spans="1:48">
       <c r="A282" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B282" s="5">
         <v>35868</v>
@@ -11660,7 +11660,7 @@
     </row>
     <row r="283" spans="1:48">
       <c r="A283" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B283" s="5">
         <v>35870</v>
@@ -11702,7 +11702,7 @@
     </row>
     <row r="284" spans="1:48">
       <c r="A284" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B284" s="5">
         <v>35871</v>
@@ -11738,7 +11738,7 @@
     </row>
     <row r="285" spans="1:48">
       <c r="A285" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B285" s="5">
         <v>35872</v>
@@ -11771,7 +11771,7 @@
     </row>
     <row r="286" spans="1:48">
       <c r="A286" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B286" s="5">
         <v>35873</v>
@@ -11804,7 +11804,7 @@
     </row>
     <row r="287" spans="1:48">
       <c r="A287" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B287" s="5">
         <v>35876</v>
@@ -11840,7 +11840,7 @@
     </row>
     <row r="288" spans="1:48">
       <c r="A288" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B288" s="5">
         <v>35878</v>
@@ -11873,7 +11873,7 @@
     </row>
     <row r="289" spans="1:50">
       <c r="A289" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B289" s="5">
         <v>35879</v>
@@ -11906,7 +11906,7 @@
     </row>
     <row r="290" spans="1:50">
       <c r="A290" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B290" s="5">
         <v>35880</v>
@@ -11939,7 +11939,7 @@
     </row>
     <row r="291" spans="1:50">
       <c r="A291" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B291" s="5">
         <v>35882</v>
@@ -11972,7 +11972,7 @@
     </row>
     <row r="292" spans="1:50">
       <c r="A292" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B292" s="5">
         <v>35883</v>
@@ -12011,7 +12011,7 @@
     </row>
     <row r="293" spans="1:50">
       <c r="A293" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B293" s="5">
         <v>35884</v>
@@ -12047,7 +12047,7 @@
     </row>
     <row r="294" spans="1:50">
       <c r="A294" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B294" s="5">
         <v>35885</v>
@@ -12095,7 +12095,7 @@
     </row>
     <row r="295" spans="1:50">
       <c r="A295" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B295" s="5">
         <v>35886</v>
@@ -12131,7 +12131,7 @@
     </row>
     <row r="296" spans="1:50">
       <c r="A296" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B296" s="5">
         <v>35795</v>
@@ -12164,7 +12164,7 @@
     </row>
     <row r="297" spans="1:50">
       <c r="A297" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B297" s="5">
         <v>35775</v>
@@ -12197,7 +12197,7 @@
     </row>
     <row r="298" spans="1:50">
       <c r="A298" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B298" s="5">
         <v>35799</v>
@@ -12233,7 +12233,7 @@
     </row>
     <row r="299" spans="1:50">
       <c r="A299" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B299" s="5">
         <v>35802</v>
@@ -12266,7 +12266,7 @@
     </row>
     <row r="300" spans="1:50">
       <c r="A300" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B300" s="5">
         <v>35803</v>
@@ -12299,7 +12299,7 @@
     </row>
     <row r="301" spans="1:50">
       <c r="A301" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B301" s="5">
         <v>35804</v>
@@ -12332,7 +12332,7 @@
     </row>
     <row r="302" spans="1:50">
       <c r="A302" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B302" s="5">
         <v>35808</v>
@@ -12365,7 +12365,7 @@
     </row>
     <row r="303" spans="1:50">
       <c r="A303" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B303" s="5">
         <v>35814</v>
@@ -12398,7 +12398,7 @@
     </row>
     <row r="304" spans="1:50">
       <c r="A304" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B304" s="5">
         <v>35816</v>
@@ -12437,7 +12437,7 @@
     </row>
     <row r="305" spans="1:50">
       <c r="A305" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B305" s="5">
         <v>35817</v>
@@ -12473,7 +12473,7 @@
     </row>
     <row r="306" spans="1:50">
       <c r="A306" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B306" s="5">
         <v>35818</v>
@@ -12506,7 +12506,7 @@
     </row>
     <row r="307" spans="1:50">
       <c r="A307" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B307" s="5">
         <v>35820</v>
@@ -12539,7 +12539,7 @@
     </row>
     <row r="308" spans="1:50">
       <c r="A308" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B308" s="5">
         <v>35824</v>
@@ -12572,7 +12572,7 @@
     </row>
     <row r="309" spans="1:50">
       <c r="A309" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B309" s="5">
         <v>35830</v>
@@ -12605,7 +12605,7 @@
     </row>
     <row r="310" spans="1:50">
       <c r="A310" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B310" s="5">
         <v>35831</v>
@@ -12638,7 +12638,7 @@
     </row>
     <row r="311" spans="1:50">
       <c r="A311" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B311" s="5">
         <v>35834</v>
@@ -12671,7 +12671,7 @@
     </row>
     <row r="312" spans="1:50">
       <c r="A312" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B312" s="5">
         <v>35835</v>
@@ -12704,7 +12704,7 @@
     </row>
     <row r="313" spans="1:50">
       <c r="A313" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B313" s="5">
         <v>35838</v>
@@ -12740,7 +12740,7 @@
     </row>
     <row r="314" spans="1:50">
       <c r="A314" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B314" s="5">
         <v>35839</v>
@@ -12773,7 +12773,7 @@
     </row>
     <row r="315" spans="1:50">
       <c r="A315" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B315" s="5">
         <v>35842</v>
@@ -12824,7 +12824,7 @@
     </row>
     <row r="316" spans="1:50">
       <c r="A316" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B316" s="5">
         <v>35843</v>
@@ -12860,7 +12860,7 @@
     </row>
     <row r="317" spans="1:50">
       <c r="A317" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B317" s="5">
         <v>35844</v>
@@ -12908,7 +12908,7 @@
     </row>
     <row r="318" spans="1:50">
       <c r="A318" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B318" s="5">
         <v>35845</v>
@@ -12941,7 +12941,7 @@
     </row>
     <row r="319" spans="1:50">
       <c r="A319" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B319" s="5">
         <v>35848</v>
@@ -12977,7 +12977,7 @@
     </row>
     <row r="320" spans="1:50">
       <c r="A320" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B320" s="5">
         <v>35849</v>
@@ -13013,7 +13013,7 @@
     </row>
     <row r="321" spans="1:50">
       <c r="A321" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B321" s="5">
         <v>35852</v>
@@ -13052,7 +13052,7 @@
     </row>
     <row r="322" spans="1:50">
       <c r="A322" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B322" s="5">
         <v>35853</v>
@@ -13085,7 +13085,7 @@
     </row>
     <row r="323" spans="1:50">
       <c r="A323" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B323" s="5">
         <v>35854</v>
@@ -13118,7 +13118,7 @@
     </row>
     <row r="324" spans="1:50">
       <c r="A324" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B324" s="5">
         <v>35855</v>
@@ -13157,7 +13157,7 @@
     </row>
     <row r="325" spans="1:50">
       <c r="A325" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B325" s="5">
         <v>35856</v>
@@ -13193,7 +13193,7 @@
     </row>
     <row r="326" spans="1:50">
       <c r="A326" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B326" s="5">
         <v>35857</v>
@@ -13226,7 +13226,7 @@
     </row>
     <row r="327" spans="1:50">
       <c r="A327" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B327" s="5">
         <v>35859</v>
@@ -13262,7 +13262,7 @@
     </row>
     <row r="328" spans="1:50">
       <c r="A328" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B328" s="5">
         <v>35860</v>
@@ -13295,7 +13295,7 @@
     </row>
     <row r="329" spans="1:50">
       <c r="A329" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B329" s="5">
         <v>35862</v>
@@ -13328,7 +13328,7 @@
     </row>
     <row r="330" spans="1:50">
       <c r="A330" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B330" s="5">
         <v>35863</v>
@@ -13367,7 +13367,7 @@
     </row>
     <row r="331" spans="1:50">
       <c r="A331" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B331" s="5">
         <v>35865</v>
@@ -13400,7 +13400,7 @@
     </row>
     <row r="332" spans="1:50">
       <c r="A332" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B332" s="5">
         <v>35868</v>
@@ -13433,7 +13433,7 @@
     </row>
     <row r="333" spans="1:50">
       <c r="A333" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B333" s="5">
         <v>35869</v>
@@ -13469,7 +13469,7 @@
     </row>
     <row r="334" spans="1:50">
       <c r="A334" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B334" s="5">
         <v>35870</v>
@@ -13514,7 +13514,7 @@
     </row>
     <row r="335" spans="1:50">
       <c r="A335" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B335" s="5">
         <v>35871</v>
@@ -13559,7 +13559,7 @@
     </row>
     <row r="336" spans="1:50">
       <c r="A336" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B336" s="5">
         <v>35872</v>
@@ -13598,7 +13598,7 @@
     </row>
     <row r="337" spans="1:49">
       <c r="A337" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B337" s="5">
         <v>35873</v>
@@ -13631,7 +13631,7 @@
     </row>
     <row r="338" spans="1:49">
       <c r="A338" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B338" s="5">
         <v>35876</v>
@@ -13667,7 +13667,7 @@
     </row>
     <row r="339" spans="1:49">
       <c r="A339" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B339" s="5">
         <v>35877</v>
@@ -13706,7 +13706,7 @@
     </row>
     <row r="340" spans="1:49">
       <c r="A340" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B340" s="5">
         <v>35883</v>
@@ -13742,7 +13742,7 @@
     </row>
     <row r="341" spans="1:49">
       <c r="A341" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B341" s="5">
         <v>35884</v>
@@ -13781,7 +13781,7 @@
     </row>
     <row r="342" spans="1:49">
       <c r="A342" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B342" s="5">
         <v>35885</v>
@@ -13832,7 +13832,7 @@
     </row>
     <row r="343" spans="1:49">
       <c r="A343" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B343" s="5">
         <v>35886</v>
@@ -13865,7 +13865,7 @@
     </row>
     <row r="344" spans="1:49">
       <c r="A344" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B344" s="5">
         <v>35768</v>
@@ -13898,7 +13898,7 @@
     </row>
     <row r="345" spans="1:49">
       <c r="A345" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B345" s="5">
         <v>35774</v>
@@ -13931,7 +13931,7 @@
     </row>
     <row r="346" spans="1:49">
       <c r="A346" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B346" s="5">
         <v>35782</v>
@@ -13964,7 +13964,7 @@
     </row>
     <row r="347" spans="1:49">
       <c r="A347" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B347" s="5">
         <v>35790</v>
@@ -13997,7 +13997,7 @@
     </row>
     <row r="348" spans="1:49">
       <c r="A348" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B348" s="5">
         <v>35794</v>
@@ -14030,7 +14030,7 @@
     </row>
     <row r="349" spans="1:49">
       <c r="A349" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B349" s="5">
         <v>35796</v>
@@ -14063,7 +14063,7 @@
     </row>
     <row r="350" spans="1:49">
       <c r="A350" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B350" s="5">
         <v>35801</v>
@@ -14096,7 +14096,7 @@
     </row>
     <row r="351" spans="1:49">
       <c r="A351" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B351" s="5">
         <v>35803</v>
@@ -14129,7 +14129,7 @@
     </row>
     <row r="352" spans="1:49">
       <c r="A352" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B352" s="5">
         <v>35807</v>
@@ -14162,7 +14162,7 @@
     </row>
     <row r="353" spans="1:50">
       <c r="A353" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B353" s="5">
         <v>35813</v>
@@ -14195,7 +14195,7 @@
     </row>
     <row r="354" spans="1:50">
       <c r="A354" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B354" s="5">
         <v>35815</v>
@@ -14231,7 +14231,7 @@
     </row>
     <row r="355" spans="1:50">
       <c r="A355" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B355" s="5">
         <v>35816</v>
@@ -14267,7 +14267,7 @@
     </row>
     <row r="356" spans="1:50">
       <c r="A356" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B356" s="5">
         <v>35817</v>
@@ -14306,7 +14306,7 @@
     </row>
     <row r="357" spans="1:50">
       <c r="A357" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B357" s="5">
         <v>35820</v>
@@ -14342,7 +14342,7 @@
     </row>
     <row r="358" spans="1:50">
       <c r="A358" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B358" s="5">
         <v>35821</v>
@@ -14378,7 +14378,7 @@
     </row>
     <row r="359" spans="1:50">
       <c r="A359" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B359" s="5">
         <v>35822</v>
@@ -14411,7 +14411,7 @@
     </row>
     <row r="360" spans="1:50">
       <c r="A360" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B360" s="5">
         <v>35823</v>
@@ -14444,7 +14444,7 @@
     </row>
     <row r="361" spans="1:50">
       <c r="A361" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B361" s="5">
         <v>35824</v>
@@ -14477,7 +14477,7 @@
     </row>
     <row r="362" spans="1:50">
       <c r="A362" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B362" s="5">
         <v>35827</v>
@@ -14513,7 +14513,7 @@
     </row>
     <row r="363" spans="1:50">
       <c r="A363" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B363" s="5">
         <v>35830</v>
@@ -14546,7 +14546,7 @@
     </row>
     <row r="364" spans="1:50">
       <c r="A364" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B364" s="5">
         <v>35831</v>
@@ -14582,7 +14582,7 @@
     </row>
     <row r="365" spans="1:50">
       <c r="A365" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B365" s="5">
         <v>35832</v>
@@ -14615,7 +14615,7 @@
     </row>
     <row r="366" spans="1:50">
       <c r="A366" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B366" s="5">
         <v>35834</v>
@@ -14651,7 +14651,7 @@
     </row>
     <row r="367" spans="1:50">
       <c r="A367" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B367" s="5">
         <v>35835</v>
@@ -14684,7 +14684,7 @@
     </row>
     <row r="368" spans="1:50">
       <c r="A368" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B368" s="5">
         <v>35836</v>
@@ -14717,7 +14717,7 @@
     </row>
     <row r="369" spans="1:48">
       <c r="A369" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B369" s="5">
         <v>35837</v>
@@ -14750,7 +14750,7 @@
     </row>
     <row r="370" spans="1:48">
       <c r="A370" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B370" s="5">
         <v>35838</v>
@@ -14783,7 +14783,7 @@
     </row>
     <row r="371" spans="1:48">
       <c r="A371" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B371" s="5">
         <v>35840</v>
@@ -14816,7 +14816,7 @@
     </row>
     <row r="372" spans="1:48">
       <c r="A372" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B372" s="5">
         <v>35841</v>
@@ -14858,7 +14858,7 @@
     </row>
     <row r="373" spans="1:48">
       <c r="A373" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B373" s="5">
         <v>35843</v>
@@ -14900,7 +14900,7 @@
     </row>
     <row r="374" spans="1:48">
       <c r="A374" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B374" s="5">
         <v>35844</v>
@@ -14948,7 +14948,7 @@
     </row>
     <row r="375" spans="1:48">
       <c r="A375" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B375" s="5">
         <v>35845</v>
@@ -14981,7 +14981,7 @@
     </row>
     <row r="376" spans="1:48">
       <c r="A376" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B376" s="5">
         <v>35846</v>
@@ -15011,7 +15011,7 @@
     </row>
     <row r="377" spans="1:48">
       <c r="A377" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B377" s="5">
         <v>35848</v>
@@ -15044,7 +15044,7 @@
     </row>
     <row r="378" spans="1:48">
       <c r="A378" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B378" s="5">
         <v>35850</v>
@@ -15077,7 +15077,7 @@
     </row>
     <row r="379" spans="1:48">
       <c r="A379" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B379" s="5">
         <v>35851</v>
@@ -15116,7 +15116,7 @@
     </row>
     <row r="380" spans="1:48">
       <c r="A380" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B380" s="5">
         <v>35852</v>
@@ -15149,7 +15149,7 @@
     </row>
     <row r="381" spans="1:48">
       <c r="A381" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B381" s="5">
         <v>35854</v>
@@ -15191,7 +15191,7 @@
     </row>
     <row r="382" spans="1:48">
       <c r="A382" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B382" s="5">
         <v>35856</v>
@@ -15227,7 +15227,7 @@
     </row>
     <row r="383" spans="1:48">
       <c r="A383" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B383" s="5">
         <v>35857</v>
@@ -15278,7 +15278,7 @@
     </row>
     <row r="384" spans="1:48">
       <c r="A384" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B384" s="5">
         <v>35858</v>
@@ -15323,7 +15323,7 @@
     </row>
     <row r="385" spans="1:50">
       <c r="A385" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B385" s="5">
         <v>35859</v>
@@ -15356,7 +15356,7 @@
     </row>
     <row r="386" spans="1:50">
       <c r="A386" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B386" s="5">
         <v>35860</v>
@@ -15395,7 +15395,7 @@
     </row>
     <row r="387" spans="1:50">
       <c r="A387" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B387" s="5">
         <v>35861</v>
@@ -15428,7 +15428,7 @@
     </row>
     <row r="388" spans="1:50">
       <c r="A388" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B388" s="5">
         <v>35862</v>
@@ -15461,7 +15461,7 @@
     </row>
     <row r="389" spans="1:50">
       <c r="A389" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B389" s="5">
         <v>35863</v>
@@ -15494,7 +15494,7 @@
     </row>
     <row r="390" spans="1:50">
       <c r="A390" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B390" s="5">
         <v>35864</v>
@@ -15530,7 +15530,7 @@
     </row>
     <row r="391" spans="1:50">
       <c r="A391" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B391" s="5">
         <v>35865</v>
@@ -15563,7 +15563,7 @@
     </row>
     <row r="392" spans="1:50">
       <c r="A392" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B392" s="5">
         <v>35866</v>
@@ -15596,7 +15596,7 @@
     </row>
     <row r="393" spans="1:50">
       <c r="A393" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B393" s="5">
         <v>35868</v>
@@ -15629,7 +15629,7 @@
     </row>
     <row r="394" spans="1:50">
       <c r="A394" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B394" s="5">
         <v>35869</v>
@@ -15665,7 +15665,7 @@
     </row>
     <row r="395" spans="1:50">
       <c r="A395" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B395" s="5">
         <v>35871</v>
@@ -15713,7 +15713,7 @@
     </row>
     <row r="396" spans="1:50">
       <c r="A396" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B396" s="5">
         <v>35873</v>
@@ -15749,7 +15749,7 @@
     </row>
     <row r="397" spans="1:50">
       <c r="A397" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B397" s="5">
         <v>35874</v>
@@ -15785,7 +15785,7 @@
     </row>
     <row r="398" spans="1:50">
       <c r="A398" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B398" s="5">
         <v>35876</v>
@@ -15821,13 +15821,13 @@
     </row>
     <row r="399" spans="1:50">
       <c r="A399" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B399" s="5">
         <v>35877</v>
       </c>
       <c r="C399" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D399" s="6">
         <v>109.526726057906</v>
@@ -15920,7 +15920,7 @@
     </row>
     <row r="400" spans="1:50">
       <c r="A400" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B400" s="5">
         <v>35878</v>
@@ -15956,7 +15956,7 @@
     </row>
     <row r="401" spans="1:36">
       <c r="A401" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B401" s="5">
         <v>35768</v>
@@ -15989,7 +15989,7 @@
     </row>
     <row r="402" spans="1:36">
       <c r="A402" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B402" s="5">
         <v>35773</v>
@@ -16022,7 +16022,7 @@
     </row>
     <row r="403" spans="1:36">
       <c r="A403" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B403" s="5">
         <v>35781</v>
@@ -16055,7 +16055,7 @@
     </row>
     <row r="404" spans="1:36">
       <c r="A404" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B404" s="5">
         <v>35790</v>
@@ -16088,7 +16088,7 @@
     </row>
     <row r="405" spans="1:36">
       <c r="A405" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B405" s="5">
         <v>35794</v>
@@ -16121,7 +16121,7 @@
     </row>
     <row r="406" spans="1:36">
       <c r="A406" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B406" s="5">
         <v>35796</v>
@@ -16154,7 +16154,7 @@
     </row>
     <row r="407" spans="1:36">
       <c r="A407" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B407" s="5">
         <v>35800</v>
@@ -16187,7 +16187,7 @@
     </row>
     <row r="408" spans="1:36">
       <c r="A408" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B408" s="5">
         <v>35804</v>
@@ -16220,7 +16220,7 @@
     </row>
     <row r="409" spans="1:36">
       <c r="A409" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B409" s="5">
         <v>35808</v>
@@ -16253,7 +16253,7 @@
     </row>
     <row r="410" spans="1:36">
       <c r="A410" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B410" s="5">
         <v>35813</v>
@@ -16286,7 +16286,7 @@
     </row>
     <row r="411" spans="1:36">
       <c r="A411" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B411" s="5">
         <v>35814</v>
@@ -16319,7 +16319,7 @@
     </row>
     <row r="412" spans="1:36">
       <c r="A412" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B412" s="5">
         <v>35816</v>
@@ -16358,7 +16358,7 @@
     </row>
     <row r="413" spans="1:36">
       <c r="A413" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B413" s="5">
         <v>35817</v>
@@ -16397,7 +16397,7 @@
     </row>
     <row r="414" spans="1:36">
       <c r="A414" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B414" s="5">
         <v>35819</v>
@@ -16430,7 +16430,7 @@
     </row>
     <row r="415" spans="1:36">
       <c r="A415" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B415" s="5">
         <v>35821</v>
@@ -16472,7 +16472,7 @@
     </row>
     <row r="416" spans="1:36">
       <c r="A416" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B416" s="5">
         <v>35822</v>
@@ -16505,7 +16505,7 @@
     </row>
     <row r="417" spans="1:42">
       <c r="A417" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B417" s="5">
         <v>35824</v>
@@ -16538,7 +16538,7 @@
     </row>
     <row r="418" spans="1:42">
       <c r="A418" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B418" s="5">
         <v>35828</v>
@@ -16574,7 +16574,7 @@
     </row>
     <row r="419" spans="1:42">
       <c r="A419" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B419" s="5">
         <v>35829</v>
@@ -16607,7 +16607,7 @@
     </row>
     <row r="420" spans="1:42">
       <c r="A420" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B420" s="5">
         <v>35830</v>
@@ -16640,7 +16640,7 @@
     </row>
     <row r="421" spans="1:42">
       <c r="A421" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B421" s="5">
         <v>35831</v>
@@ -16673,7 +16673,7 @@
     </row>
     <row r="422" spans="1:42">
       <c r="A422" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B422" s="5">
         <v>35832</v>
@@ -16709,7 +16709,7 @@
     </row>
     <row r="423" spans="1:42">
       <c r="A423" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B423" s="5">
         <v>35833</v>
@@ -16742,7 +16742,7 @@
     </row>
     <row r="424" spans="1:42">
       <c r="A424" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B424" s="5">
         <v>35835</v>
@@ -16781,7 +16781,7 @@
     </row>
     <row r="425" spans="1:42">
       <c r="A425" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B425" s="5">
         <v>35836</v>
@@ -16817,7 +16817,7 @@
     </row>
     <row r="426" spans="1:42">
       <c r="A426" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B426" s="5">
         <v>35839</v>
@@ -16853,7 +16853,7 @@
     </row>
     <row r="427" spans="1:42">
       <c r="A427" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B427" s="5">
         <v>35840</v>
@@ -16886,7 +16886,7 @@
     </row>
     <row r="428" spans="1:42">
       <c r="A428" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B428" s="5">
         <v>35841</v>
@@ -16919,7 +16919,7 @@
     </row>
     <row r="429" spans="1:42">
       <c r="A429" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B429" s="5">
         <v>35842</v>
@@ -16958,7 +16958,7 @@
     </row>
     <row r="430" spans="1:42">
       <c r="A430" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B430" s="5">
         <v>35844</v>
@@ -17000,7 +17000,7 @@
     </row>
     <row r="431" spans="1:42">
       <c r="A431" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B431" s="5">
         <v>35846</v>
@@ -17033,7 +17033,7 @@
     </row>
     <row r="432" spans="1:42">
       <c r="A432" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B432" s="5">
         <v>35848</v>
@@ -17066,7 +17066,7 @@
     </row>
     <row r="433" spans="1:49">
       <c r="A433" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B433" s="5">
         <v>35849</v>
@@ -17105,7 +17105,7 @@
     </row>
     <row r="434" spans="1:49">
       <c r="A434" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B434" s="5">
         <v>35852</v>
@@ -17141,7 +17141,7 @@
     </row>
     <row r="435" spans="1:49">
       <c r="A435" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B435" s="5">
         <v>35853</v>
@@ -17174,7 +17174,7 @@
     </row>
     <row r="436" spans="1:49">
       <c r="A436" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B436" s="5">
         <v>35854</v>
@@ -17213,7 +17213,7 @@
     </row>
     <row r="437" spans="1:49">
       <c r="A437" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B437" s="5">
         <v>35855</v>
@@ -17246,7 +17246,7 @@
     </row>
     <row r="438" spans="1:49">
       <c r="A438" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B438" s="5">
         <v>35856</v>
@@ -17282,7 +17282,7 @@
     </row>
     <row r="439" spans="1:49">
       <c r="A439" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B439" s="5">
         <v>35857</v>
@@ -17336,7 +17336,7 @@
     </row>
     <row r="440" spans="1:49">
       <c r="A440" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B440" s="5">
         <v>35858</v>
@@ -17375,7 +17375,7 @@
     </row>
     <row r="441" spans="1:49">
       <c r="A441" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B441" s="5">
         <v>35859</v>
@@ -17408,7 +17408,7 @@
     </row>
     <row r="442" spans="1:49">
       <c r="A442" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B442" s="5">
         <v>35860</v>
@@ -17444,7 +17444,7 @@
     </row>
     <row r="443" spans="1:49">
       <c r="A443" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B443" s="5">
         <v>35863</v>
@@ -17477,7 +17477,7 @@
     </row>
     <row r="444" spans="1:49">
       <c r="A444" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B444" s="5">
         <v>35864</v>
@@ -17513,7 +17513,7 @@
     </row>
     <row r="445" spans="1:49">
       <c r="A445" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B445" s="5">
         <v>35865</v>
@@ -17549,7 +17549,7 @@
     </row>
     <row r="446" spans="1:49">
       <c r="A446" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B446" s="5">
         <v>35867</v>
@@ -17585,7 +17585,7 @@
     </row>
     <row r="447" spans="1:49">
       <c r="A447" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B447" s="5">
         <v>35869</v>
@@ -17633,7 +17633,7 @@
     </row>
     <row r="448" spans="1:49">
       <c r="A448" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B448" s="5">
         <v>35768</v>
@@ -17666,7 +17666,7 @@
     </row>
     <row r="449" spans="1:50">
       <c r="A449" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B449" s="5">
         <v>35774</v>
@@ -17699,7 +17699,7 @@
     </row>
     <row r="450" spans="1:50">
       <c r="A450" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B450" s="5">
         <v>35776</v>
@@ -17732,7 +17732,7 @@
     </row>
     <row r="451" spans="1:50">
       <c r="A451" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B451" s="5">
         <v>35781</v>
@@ -17765,7 +17765,7 @@
     </row>
     <row r="452" spans="1:50">
       <c r="A452" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B452" s="5">
         <v>35790</v>
@@ -17798,7 +17798,7 @@
     </row>
     <row r="453" spans="1:50">
       <c r="A453" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B453" s="5">
         <v>35795</v>
@@ -17831,7 +17831,7 @@
     </row>
     <row r="454" spans="1:50">
       <c r="A454" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B454" s="5">
         <v>35797</v>
@@ -17864,7 +17864,7 @@
     </row>
     <row r="455" spans="1:50">
       <c r="A455" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B455" s="5">
         <v>35801</v>
@@ -17897,7 +17897,7 @@
     </row>
     <row r="456" spans="1:50">
       <c r="A456" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B456" s="5">
         <v>35803</v>
@@ -17930,7 +17930,7 @@
     </row>
     <row r="457" spans="1:50">
       <c r="A457" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B457" s="5">
         <v>35808</v>
@@ -17963,7 +17963,7 @@
     </row>
     <row r="458" spans="1:50">
       <c r="A458" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B458" s="5">
         <v>35813</v>
@@ -17996,7 +17996,7 @@
     </row>
     <row r="459" spans="1:50">
       <c r="A459" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B459" s="5">
         <v>35814</v>
@@ -18032,7 +18032,7 @@
     </row>
     <row r="460" spans="1:50">
       <c r="A460" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B460" s="5">
         <v>35816</v>
@@ -18089,7 +18089,7 @@
     </row>
     <row r="461" spans="1:50">
       <c r="A461" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B461" s="5">
         <v>35817</v>
@@ -18134,7 +18134,7 @@
     </row>
     <row r="462" spans="1:50">
       <c r="A462" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B462" s="5">
         <v>35818</v>
@@ -18167,7 +18167,7 @@
     </row>
     <row r="463" spans="1:50">
       <c r="A463" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B463" s="5">
         <v>35820</v>
@@ -18200,7 +18200,7 @@
     </row>
     <row r="464" spans="1:50">
       <c r="A464" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B464" s="5">
         <v>35821</v>
@@ -18236,7 +18236,7 @@
     </row>
     <row r="465" spans="1:42">
       <c r="A465" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B465" s="5">
         <v>35824</v>
@@ -18272,7 +18272,7 @@
     </row>
     <row r="466" spans="1:42">
       <c r="A466" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B466" s="5">
         <v>35825</v>
@@ -18305,7 +18305,7 @@
     </row>
     <row r="467" spans="1:42">
       <c r="A467" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B467" s="5">
         <v>35826</v>
@@ -18341,7 +18341,7 @@
     </row>
     <row r="468" spans="1:42">
       <c r="A468" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B468" s="5">
         <v>35828</v>
@@ -18383,7 +18383,7 @@
     </row>
     <row r="469" spans="1:42">
       <c r="A469" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B469" s="5">
         <v>35829</v>
@@ -18416,7 +18416,7 @@
     </row>
     <row r="470" spans="1:42">
       <c r="A470" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B470" s="5">
         <v>35831</v>
@@ -18449,7 +18449,7 @@
     </row>
     <row r="471" spans="1:42">
       <c r="A471" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B471" s="5">
         <v>35832</v>
@@ -18485,7 +18485,7 @@
     </row>
     <row r="472" spans="1:42">
       <c r="A472" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B472" s="5">
         <v>35834</v>
@@ -18521,7 +18521,7 @@
     </row>
     <row r="473" spans="1:42">
       <c r="A473" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B473" s="5">
         <v>35835</v>
@@ -18557,7 +18557,7 @@
     </row>
     <row r="474" spans="1:42">
       <c r="A474" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B474" s="5">
         <v>35836</v>
@@ -18590,7 +18590,7 @@
     </row>
     <row r="475" spans="1:42">
       <c r="A475" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B475" s="5">
         <v>35838</v>
@@ -18626,7 +18626,7 @@
     </row>
     <row r="476" spans="1:42">
       <c r="A476" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B476" s="5">
         <v>35839</v>
@@ -18659,7 +18659,7 @@
     </row>
     <row r="477" spans="1:42">
       <c r="A477" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B477" s="5">
         <v>35841</v>
@@ -18701,7 +18701,7 @@
     </row>
     <row r="478" spans="1:42">
       <c r="A478" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B478" s="5">
         <v>35842</v>
@@ -18737,7 +18737,7 @@
     </row>
     <row r="479" spans="1:42">
       <c r="A479" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B479" s="5">
         <v>35844</v>
@@ -18785,7 +18785,7 @@
     </row>
     <row r="480" spans="1:42">
       <c r="A480" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B480" s="5">
         <v>35845</v>
@@ -18818,7 +18818,7 @@
     </row>
     <row r="481" spans="1:49">
       <c r="A481" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B481" s="5">
         <v>35848</v>
@@ -18857,7 +18857,7 @@
     </row>
     <row r="482" spans="1:49">
       <c r="A482" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B482" s="5">
         <v>35849</v>
@@ -18890,7 +18890,7 @@
     </row>
     <row r="483" spans="1:49">
       <c r="A483" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B483" s="5">
         <v>35851</v>
@@ -18923,7 +18923,7 @@
     </row>
     <row r="484" spans="1:49">
       <c r="A484" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B484" s="5">
         <v>35852</v>
@@ -18962,7 +18962,7 @@
     </row>
     <row r="485" spans="1:49">
       <c r="A485" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B485" s="5">
         <v>35853</v>
@@ -18995,7 +18995,7 @@
     </row>
     <row r="486" spans="1:49">
       <c r="A486" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B486" s="5">
         <v>35854</v>
@@ -19028,7 +19028,7 @@
     </row>
     <row r="487" spans="1:49">
       <c r="A487" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B487" s="5">
         <v>35855</v>
@@ -19070,7 +19070,7 @@
     </row>
     <row r="488" spans="1:49">
       <c r="A488" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B488" s="5">
         <v>35856</v>
@@ -19106,7 +19106,7 @@
     </row>
     <row r="489" spans="1:49">
       <c r="A489" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B489" s="5">
         <v>35857</v>
@@ -19142,7 +19142,7 @@
     </row>
     <row r="490" spans="1:49">
       <c r="A490" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B490" s="5">
         <v>35858</v>
@@ -19175,7 +19175,7 @@
     </row>
     <row r="491" spans="1:49">
       <c r="A491" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B491" s="5">
         <v>35859</v>
@@ -19214,7 +19214,7 @@
     </row>
     <row r="492" spans="1:49">
       <c r="A492" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B492" s="5">
         <v>35860</v>
@@ -19250,7 +19250,7 @@
     </row>
     <row r="493" spans="1:49">
       <c r="A493" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B493" s="5">
         <v>35862</v>
@@ -19283,7 +19283,7 @@
     </row>
     <row r="494" spans="1:49">
       <c r="A494" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B494" s="5">
         <v>35864</v>
@@ -19325,7 +19325,7 @@
     </row>
     <row r="495" spans="1:49">
       <c r="A495" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B495" s="5">
         <v>35865</v>
@@ -19367,7 +19367,7 @@
     </row>
     <row r="496" spans="1:49">
       <c r="A496" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B496" s="5">
         <v>35867</v>
@@ -19403,7 +19403,7 @@
     </row>
     <row r="497" spans="1:36">
       <c r="A497" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B497" s="5">
         <v>35868</v>
@@ -19436,7 +19436,7 @@
     </row>
     <row r="498" spans="1:36">
       <c r="A498" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B498" s="5">
         <v>35870</v>
@@ -19469,7 +19469,7 @@
     </row>
     <row r="499" spans="1:36">
       <c r="A499" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B499" s="5">
         <v>35874</v>

</xml_diff>

<commit_message>
Dilution and water improved
</commit_message>
<xml_diff>
--- a/Prototypes/Mungbean/Exp3observed.xlsx
+++ b/Prototypes/Mungbean/Exp3observed.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pas075\Documents\ApsimX\Prototypes\Mungbean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A3B0468-3B5F-4702-BA5D-0BB700814FF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF9CC480-A1A3-4B12-B537-AAD0347F27A6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8C69385E-AA3F-4CF3-AF00-E1E4599E61EE}"/>
   </bookViews>
@@ -601,17 +601,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21968B1A-9F2D-47BD-B4B3-097E93366914}">
-  <dimension ref="A1:AY499"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:AY531"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
+      <selection pane="bottomLeft" activeCell="C506" sqref="C506"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="3" width="19.140625" customWidth="1"/>
+    <col min="1" max="1" width="35.7109375" customWidth="1"/>
+    <col min="2" max="3" width="19.140625" customWidth="1"/>
     <col min="4" max="5" width="9.42578125" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:51">
@@ -769,7 +772,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:51">
+    <row r="2" spans="1:51" hidden="1">
       <c r="A2" s="2" t="s">
         <v>50</v>
       </c>
@@ -814,7 +817,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="3" spans="1:51">
+    <row r="3" spans="1:51" hidden="1">
       <c r="A3" s="2" t="s">
         <v>47</v>
       </c>
@@ -850,7 +853,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="4" spans="1:51">
+    <row r="4" spans="1:51" hidden="1">
       <c r="A4" s="2" t="s">
         <v>47</v>
       </c>
@@ -892,7 +895,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="5" spans="1:51">
+    <row r="5" spans="1:51" hidden="1">
       <c r="A5" s="2" t="s">
         <v>53</v>
       </c>
@@ -949,7 +952,7 @@
         <v>2.59</v>
       </c>
     </row>
-    <row r="6" spans="1:51">
+    <row r="6" spans="1:51" hidden="1">
       <c r="A6" s="2" t="s">
         <v>48</v>
       </c>
@@ -994,7 +997,7 @@
         <v>1873</v>
       </c>
     </row>
-    <row r="7" spans="1:51">
+    <row r="7" spans="1:51" hidden="1">
       <c r="A7" s="2" t="s">
         <v>54</v>
       </c>
@@ -1048,7 +1051,7 @@
         <v>2.78</v>
       </c>
     </row>
-    <row r="8" spans="1:51">
+    <row r="8" spans="1:51" hidden="1">
       <c r="A8" s="2" t="s">
         <v>49</v>
       </c>
@@ -1087,7 +1090,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="9" spans="1:51">
+    <row r="9" spans="1:51" hidden="1">
       <c r="A9" s="2" t="s">
         <v>52</v>
       </c>
@@ -1123,7 +1126,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="10" spans="1:51">
+    <row r="10" spans="1:51" hidden="1">
       <c r="A10" s="2" t="s">
         <v>51</v>
       </c>
@@ -1174,7 +1177,7 @@
         <v>2.78</v>
       </c>
     </row>
-    <row r="11" spans="1:51">
+    <row r="11" spans="1:51" hidden="1">
       <c r="A11" s="2" t="s">
         <v>55</v>
       </c>
@@ -1219,7 +1222,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="12" spans="1:51">
+    <row r="12" spans="1:51" hidden="1">
       <c r="A12" s="2" t="s">
         <v>52</v>
       </c>
@@ -1258,7 +1261,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="13" spans="1:51">
+    <row r="13" spans="1:51" hidden="1">
       <c r="A13" s="2" t="s">
         <v>55</v>
       </c>
@@ -1297,7 +1300,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="14" spans="1:51">
+    <row r="14" spans="1:51" hidden="1">
       <c r="A14" s="2" t="s">
         <v>50</v>
       </c>
@@ -1333,7 +1336,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="15" spans="1:51">
+    <row r="15" spans="1:51" hidden="1">
       <c r="A15" s="2" t="s">
         <v>48</v>
       </c>
@@ -1369,7 +1372,7 @@
         <v>1873</v>
       </c>
     </row>
-    <row r="16" spans="1:51">
+    <row r="16" spans="1:51" hidden="1">
       <c r="A16" s="2" t="s">
         <v>49</v>
       </c>
@@ -1405,7 +1408,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="17" spans="1:47">
+    <row r="17" spans="1:47" hidden="1">
       <c r="A17" s="2" t="s">
         <v>51</v>
       </c>
@@ -1441,7 +1444,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="18" spans="1:47">
+    <row r="18" spans="1:47" hidden="1">
       <c r="A18" s="2" t="s">
         <v>48</v>
       </c>
@@ -1477,7 +1480,7 @@
         <v>1873</v>
       </c>
     </row>
-    <row r="19" spans="1:47">
+    <row r="19" spans="1:47" hidden="1">
       <c r="A19" s="2" t="s">
         <v>47</v>
       </c>
@@ -1513,7 +1516,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="20" spans="1:47">
+    <row r="20" spans="1:47" hidden="1">
       <c r="A20" s="2" t="s">
         <v>52</v>
       </c>
@@ -1549,7 +1552,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="21" spans="1:47">
+    <row r="21" spans="1:47" hidden="1">
       <c r="A21" s="2" t="s">
         <v>50</v>
       </c>
@@ -1624,7 +1627,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="22" spans="1:47">
+    <row r="22" spans="1:47" hidden="1">
       <c r="A22" s="2" t="s">
         <v>55</v>
       </c>
@@ -1660,7 +1663,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="23" spans="1:47">
+    <row r="23" spans="1:47" hidden="1">
       <c r="A23" s="2" t="s">
         <v>54</v>
       </c>
@@ -1696,7 +1699,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="24" spans="1:47">
+    <row r="24" spans="1:47" hidden="1">
       <c r="A24" s="2" t="s">
         <v>54</v>
       </c>
@@ -1732,7 +1735,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="25" spans="1:47">
+    <row r="25" spans="1:47" hidden="1">
       <c r="A25" s="2" t="s">
         <v>53</v>
       </c>
@@ -1768,7 +1771,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="26" spans="1:47">
+    <row r="26" spans="1:47" hidden="1">
       <c r="A26" s="2" t="s">
         <v>51</v>
       </c>
@@ -1804,7 +1807,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="27" spans="1:47">
+    <row r="27" spans="1:47" hidden="1">
       <c r="A27" s="2" t="s">
         <v>49</v>
       </c>
@@ -1840,7 +1843,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="28" spans="1:47">
+    <row r="28" spans="1:47" hidden="1">
       <c r="A28" t="s">
         <v>55</v>
       </c>
@@ -1885,7 +1888,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="29" spans="1:47">
+    <row r="29" spans="1:47" hidden="1">
       <c r="A29" s="2" t="s">
         <v>53</v>
       </c>
@@ -1921,7 +1924,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="30" spans="1:47">
+    <row r="30" spans="1:47" hidden="1">
       <c r="A30" s="2" t="s">
         <v>55</v>
       </c>
@@ -1960,7 +1963,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="31" spans="1:47">
+    <row r="31" spans="1:47" hidden="1">
       <c r="A31" s="2" t="s">
         <v>52</v>
       </c>
@@ -1996,7 +1999,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="32" spans="1:47">
+    <row r="32" spans="1:47" hidden="1">
       <c r="A32" s="2" t="s">
         <v>50</v>
       </c>
@@ -2032,7 +2035,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="33" spans="1:37">
+    <row r="33" spans="1:37" hidden="1">
       <c r="A33" s="2" t="s">
         <v>50</v>
       </c>
@@ -2068,7 +2071,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="34" spans="1:37">
+    <row r="34" spans="1:37" hidden="1">
       <c r="A34" s="2" t="s">
         <v>53</v>
       </c>
@@ -2104,7 +2107,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="35" spans="1:37">
+    <row r="35" spans="1:37" hidden="1">
       <c r="A35" s="2" t="s">
         <v>53</v>
       </c>
@@ -2140,7 +2143,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="36" spans="1:37">
+    <row r="36" spans="1:37" hidden="1">
       <c r="A36" s="2" t="s">
         <v>55</v>
       </c>
@@ -2176,7 +2179,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="37" spans="1:37">
+    <row r="37" spans="1:37" hidden="1">
       <c r="A37" s="2" t="s">
         <v>47</v>
       </c>
@@ -2212,7 +2215,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="38" spans="1:37">
+    <row r="38" spans="1:37" hidden="1">
       <c r="A38" s="2" t="s">
         <v>54</v>
       </c>
@@ -2248,7 +2251,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="39" spans="1:37">
+    <row r="39" spans="1:37" hidden="1">
       <c r="A39" s="2" t="s">
         <v>51</v>
       </c>
@@ -2284,7 +2287,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="40" spans="1:37">
+    <row r="40" spans="1:37" hidden="1">
       <c r="A40" s="2" t="s">
         <v>49</v>
       </c>
@@ -2320,7 +2323,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="41" spans="1:37">
+    <row r="41" spans="1:37" hidden="1">
       <c r="A41" s="2" t="s">
         <v>48</v>
       </c>
@@ -2356,7 +2359,7 @@
         <v>1873</v>
       </c>
     </row>
-    <row r="42" spans="1:37">
+    <row r="42" spans="1:37" hidden="1">
       <c r="A42" s="2" t="s">
         <v>47</v>
       </c>
@@ -2392,7 +2395,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="43" spans="1:37">
+    <row r="43" spans="1:37" hidden="1">
       <c r="A43" s="2" t="s">
         <v>55</v>
       </c>
@@ -2428,7 +2431,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="44" spans="1:37">
+    <row r="44" spans="1:37" hidden="1">
       <c r="A44" s="2" t="s">
         <v>51</v>
       </c>
@@ -2464,7 +2467,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="45" spans="1:37">
+    <row r="45" spans="1:37" hidden="1">
       <c r="A45" s="2" t="s">
         <v>55</v>
       </c>
@@ -2506,7 +2509,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="46" spans="1:37">
+    <row r="46" spans="1:37" hidden="1">
       <c r="A46" s="2" t="s">
         <v>52</v>
       </c>
@@ -2545,7 +2548,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="47" spans="1:37">
+    <row r="47" spans="1:37" hidden="1">
       <c r="A47" s="2" t="s">
         <v>55</v>
       </c>
@@ -2581,7 +2584,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="48" spans="1:37">
+    <row r="48" spans="1:37" hidden="1">
       <c r="A48" s="2" t="s">
         <v>51</v>
       </c>
@@ -2620,7 +2623,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="49" spans="1:51" ht="15.75" customHeight="1">
+    <row r="49" spans="1:51" ht="15.75" hidden="1" customHeight="1">
       <c r="A49" s="2" t="s">
         <v>55</v>
       </c>
@@ -2659,7 +2662,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="50" spans="1:51">
+    <row r="50" spans="1:51" hidden="1">
       <c r="A50" s="2" t="s">
         <v>48</v>
       </c>
@@ -2698,7 +2701,7 @@
         <v>1873</v>
       </c>
     </row>
-    <row r="51" spans="1:51">
+    <row r="51" spans="1:51" hidden="1">
       <c r="A51" s="2" t="s">
         <v>51</v>
       </c>
@@ -2734,7 +2737,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="52" spans="1:51">
+    <row r="52" spans="1:51" hidden="1">
       <c r="A52" s="2" t="s">
         <v>53</v>
       </c>
@@ -2794,7 +2797,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="53" spans="1:51">
+    <row r="53" spans="1:51" hidden="1">
       <c r="A53" s="2" t="s">
         <v>54</v>
       </c>
@@ -2830,7 +2833,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="54" spans="1:51">
+    <row r="54" spans="1:51" hidden="1">
       <c r="A54" s="2" t="s">
         <v>48</v>
       </c>
@@ -2866,7 +2869,7 @@
         <v>1873</v>
       </c>
     </row>
-    <row r="55" spans="1:51">
+    <row r="55" spans="1:51" hidden="1">
       <c r="A55" s="2" t="s">
         <v>50</v>
       </c>
@@ -2902,7 +2905,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="56" spans="1:51">
+    <row r="56" spans="1:51" hidden="1">
       <c r="A56" s="2" t="s">
         <v>47</v>
       </c>
@@ -2938,7 +2941,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="57" spans="1:51">
+    <row r="57" spans="1:51" hidden="1">
       <c r="A57" s="2" t="s">
         <v>55</v>
       </c>
@@ -2977,7 +2980,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="58" spans="1:51">
+    <row r="58" spans="1:51" hidden="1">
       <c r="A58" s="2" t="s">
         <v>49</v>
       </c>
@@ -3013,7 +3016,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="59" spans="1:51">
+    <row r="59" spans="1:51" hidden="1">
       <c r="A59" s="2" t="s">
         <v>48</v>
       </c>
@@ -3052,7 +3055,7 @@
         <v>1873</v>
       </c>
     </row>
-    <row r="60" spans="1:51">
+    <row r="60" spans="1:51" hidden="1">
       <c r="A60" s="2" t="s">
         <v>53</v>
       </c>
@@ -3088,7 +3091,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="61" spans="1:51">
+    <row r="61" spans="1:51" hidden="1">
       <c r="A61" s="2" t="s">
         <v>49</v>
       </c>
@@ -3127,7 +3130,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="62" spans="1:51">
+    <row r="62" spans="1:51" hidden="1">
       <c r="A62" s="2" t="s">
         <v>53</v>
       </c>
@@ -3181,7 +3184,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:51">
+    <row r="63" spans="1:51" hidden="1">
       <c r="A63" s="2" t="s">
         <v>51</v>
       </c>
@@ -3220,7 +3223,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="64" spans="1:51">
+    <row r="64" spans="1:51" hidden="1">
       <c r="A64" s="2" t="s">
         <v>49</v>
       </c>
@@ -3265,7 +3268,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="65" spans="1:47">
+    <row r="65" spans="1:47" hidden="1">
       <c r="A65" s="2" t="s">
         <v>53</v>
       </c>
@@ -3304,7 +3307,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="66" spans="1:47">
+    <row r="66" spans="1:47" hidden="1">
       <c r="A66" s="2" t="s">
         <v>53</v>
       </c>
@@ -3415,7 +3418,7 @@
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="67" spans="1:47">
+    <row r="67" spans="1:47" hidden="1">
       <c r="A67" s="2" t="s">
         <v>52</v>
       </c>
@@ -3454,7 +3457,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="68" spans="1:47">
+    <row r="68" spans="1:47" hidden="1">
       <c r="A68" s="2" t="s">
         <v>49</v>
       </c>
@@ -3496,7 +3499,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="69" spans="1:47">
+    <row r="69" spans="1:47" hidden="1">
       <c r="A69" s="2" t="s">
         <v>49</v>
       </c>
@@ -3532,7 +3535,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="70" spans="1:47">
+    <row r="70" spans="1:47" hidden="1">
       <c r="A70" s="2" t="s">
         <v>50</v>
       </c>
@@ -3568,7 +3571,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="71" spans="1:47">
+    <row r="71" spans="1:47" hidden="1">
       <c r="A71" s="2" t="s">
         <v>55</v>
       </c>
@@ -3604,7 +3607,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="72" spans="1:47">
+    <row r="72" spans="1:47" hidden="1">
       <c r="A72" s="2" t="s">
         <v>55</v>
       </c>
@@ -3640,7 +3643,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="73" spans="1:47">
+    <row r="73" spans="1:47" hidden="1">
       <c r="A73" s="2" t="s">
         <v>53</v>
       </c>
@@ -3676,7 +3679,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="74" spans="1:47">
+    <row r="74" spans="1:47" hidden="1">
       <c r="A74" s="2" t="s">
         <v>47</v>
       </c>
@@ -3712,7 +3715,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="75" spans="1:47">
+    <row r="75" spans="1:47" hidden="1">
       <c r="A75" s="2" t="s">
         <v>52</v>
       </c>
@@ -3748,7 +3751,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="76" spans="1:47">
+    <row r="76" spans="1:47" hidden="1">
       <c r="A76" s="2" t="s">
         <v>50</v>
       </c>
@@ -3787,7 +3790,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="77" spans="1:47">
+    <row r="77" spans="1:47" hidden="1">
       <c r="A77" s="2" t="s">
         <v>52</v>
       </c>
@@ -3823,7 +3826,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="78" spans="1:47">
+    <row r="78" spans="1:47" hidden="1">
       <c r="A78" s="2" t="s">
         <v>49</v>
       </c>
@@ -3859,7 +3862,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="79" spans="1:47">
+    <row r="79" spans="1:47" hidden="1">
       <c r="A79" s="2" t="s">
         <v>53</v>
       </c>
@@ -3895,7 +3898,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="80" spans="1:47">
+    <row r="80" spans="1:47" hidden="1">
       <c r="A80" s="2" t="s">
         <v>49</v>
       </c>
@@ -3931,7 +3934,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="81" spans="1:37">
+    <row r="81" spans="1:37" hidden="1">
       <c r="A81" s="2" t="s">
         <v>50</v>
       </c>
@@ -3976,7 +3979,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="82" spans="1:37">
+    <row r="82" spans="1:37" hidden="1">
       <c r="A82" s="2" t="s">
         <v>48</v>
       </c>
@@ -4015,7 +4018,7 @@
         <v>1873</v>
       </c>
     </row>
-    <row r="83" spans="1:37">
+    <row r="83" spans="1:37" hidden="1">
       <c r="A83" t="s">
         <v>53</v>
       </c>
@@ -4057,7 +4060,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="84" spans="1:37">
+    <row r="84" spans="1:37" hidden="1">
       <c r="A84" s="2" t="s">
         <v>55</v>
       </c>
@@ -4102,7 +4105,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="85" spans="1:37">
+    <row r="85" spans="1:37" hidden="1">
       <c r="A85" s="2" t="s">
         <v>52</v>
       </c>
@@ -4144,7 +4147,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="86" spans="1:37">
+    <row r="86" spans="1:37" hidden="1">
       <c r="A86" s="2" t="s">
         <v>53</v>
       </c>
@@ -4186,7 +4189,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="87" spans="1:37">
+    <row r="87" spans="1:37" hidden="1">
       <c r="A87" s="2" t="s">
         <v>52</v>
       </c>
@@ -4222,7 +4225,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="88" spans="1:37">
+    <row r="88" spans="1:37" hidden="1">
       <c r="A88" s="2" t="s">
         <v>47</v>
       </c>
@@ -4258,7 +4261,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="89" spans="1:37">
+    <row r="89" spans="1:37" hidden="1">
       <c r="A89" s="2" t="s">
         <v>53</v>
       </c>
@@ -4297,7 +4300,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="90" spans="1:37">
+    <row r="90" spans="1:37" hidden="1">
       <c r="A90" s="2" t="s">
         <v>49</v>
       </c>
@@ -4333,7 +4336,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="91" spans="1:37">
+    <row r="91" spans="1:37" hidden="1">
       <c r="A91" s="2" t="s">
         <v>50</v>
       </c>
@@ -4369,7 +4372,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="92" spans="1:37">
+    <row r="92" spans="1:37" hidden="1">
       <c r="A92" s="2" t="s">
         <v>47</v>
       </c>
@@ -4405,7 +4408,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="93" spans="1:37">
+    <row r="93" spans="1:37" hidden="1">
       <c r="A93" s="2" t="s">
         <v>52</v>
       </c>
@@ -4444,7 +4447,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="94" spans="1:37">
+    <row r="94" spans="1:37" hidden="1">
       <c r="A94" s="2" t="s">
         <v>52</v>
       </c>
@@ -4486,7 +4489,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="95" spans="1:37">
+    <row r="95" spans="1:37" hidden="1">
       <c r="A95" s="2" t="s">
         <v>49</v>
       </c>
@@ -4525,7 +4528,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="96" spans="1:37">
+    <row r="96" spans="1:37" hidden="1">
       <c r="A96" s="2" t="s">
         <v>50</v>
       </c>
@@ -4561,7 +4564,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="97" spans="1:37">
+    <row r="97" spans="1:37" hidden="1">
       <c r="A97" s="2" t="s">
         <v>50</v>
       </c>
@@ -4600,7 +4603,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="98" spans="1:37">
+    <row r="98" spans="1:37" hidden="1">
       <c r="A98" s="2" t="s">
         <v>51</v>
       </c>
@@ -4639,7 +4642,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="99" spans="1:37">
+    <row r="99" spans="1:37" hidden="1">
       <c r="A99" s="2" t="s">
         <v>49</v>
       </c>
@@ -4678,7 +4681,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="100" spans="1:37">
+    <row r="100" spans="1:37" hidden="1">
       <c r="A100" s="2" t="s">
         <v>50</v>
       </c>
@@ -4717,7 +4720,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="101" spans="1:37">
+    <row r="101" spans="1:37" hidden="1">
       <c r="A101" s="2" t="s">
         <v>54</v>
       </c>
@@ -4753,7 +4756,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="102" spans="1:37">
+    <row r="102" spans="1:37" hidden="1">
       <c r="A102" s="2" t="s">
         <v>50</v>
       </c>
@@ -4789,7 +4792,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="103" spans="1:37">
+    <row r="103" spans="1:37" hidden="1">
       <c r="A103" s="2" t="s">
         <v>51</v>
       </c>
@@ -4825,7 +4828,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="104" spans="1:37">
+    <row r="104" spans="1:37" hidden="1">
       <c r="A104" s="2" t="s">
         <v>51</v>
       </c>
@@ -4861,7 +4864,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="105" spans="1:37">
+    <row r="105" spans="1:37" hidden="1">
       <c r="A105" s="2" t="s">
         <v>47</v>
       </c>
@@ -4897,7 +4900,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="106" spans="1:37">
+    <row r="106" spans="1:37" hidden="1">
       <c r="A106" s="2" t="s">
         <v>48</v>
       </c>
@@ -4939,7 +4942,7 @@
         <v>1873</v>
       </c>
     </row>
-    <row r="107" spans="1:37">
+    <row r="107" spans="1:37" hidden="1">
       <c r="A107" s="2" t="s">
         <v>55</v>
       </c>
@@ -4975,7 +4978,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="108" spans="1:37">
+    <row r="108" spans="1:37" hidden="1">
       <c r="A108" s="2" t="s">
         <v>52</v>
       </c>
@@ -5011,7 +5014,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="109" spans="1:37">
+    <row r="109" spans="1:37" hidden="1">
       <c r="A109" s="2" t="s">
         <v>47</v>
       </c>
@@ -5047,7 +5050,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="110" spans="1:37">
+    <row r="110" spans="1:37" hidden="1">
       <c r="A110" s="2" t="s">
         <v>49</v>
       </c>
@@ -5083,7 +5086,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="111" spans="1:37">
+    <row r="111" spans="1:37" hidden="1">
       <c r="A111" s="2" t="s">
         <v>54</v>
       </c>
@@ -5119,7 +5122,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="112" spans="1:37">
+    <row r="112" spans="1:37" hidden="1">
       <c r="A112" s="2" t="s">
         <v>48</v>
       </c>
@@ -5155,7 +5158,7 @@
         <v>1873</v>
       </c>
     </row>
-    <row r="113" spans="1:51">
+    <row r="113" spans="1:51" hidden="1">
       <c r="A113" s="2" t="s">
         <v>48</v>
       </c>
@@ -5194,7 +5197,7 @@
         <v>1873</v>
       </c>
     </row>
-    <row r="114" spans="1:51">
+    <row r="114" spans="1:51" hidden="1">
       <c r="A114" s="2" t="s">
         <v>53</v>
       </c>
@@ -5230,7 +5233,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="115" spans="1:51">
+    <row r="115" spans="1:51" hidden="1">
       <c r="A115" s="2" t="s">
         <v>50</v>
       </c>
@@ -5269,7 +5272,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="116" spans="1:51">
+    <row r="116" spans="1:51" hidden="1">
       <c r="A116" s="2" t="s">
         <v>48</v>
       </c>
@@ -5305,7 +5308,7 @@
         <v>1873</v>
       </c>
     </row>
-    <row r="117" spans="1:51" ht="15.75" customHeight="1">
+    <row r="117" spans="1:51" ht="15.75" hidden="1" customHeight="1">
       <c r="A117" s="2" t="s">
         <v>54</v>
       </c>
@@ -5341,7 +5344,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="118" spans="1:51">
+    <row r="118" spans="1:51" hidden="1">
       <c r="A118" s="2" t="s">
         <v>51</v>
       </c>
@@ -5377,7 +5380,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="119" spans="1:51">
+    <row r="119" spans="1:51" hidden="1">
       <c r="A119" s="2" t="s">
         <v>49</v>
       </c>
@@ -5416,7 +5419,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="120" spans="1:51">
+    <row r="120" spans="1:51" hidden="1">
       <c r="A120" s="2" t="s">
         <v>47</v>
       </c>
@@ -5455,7 +5458,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="121" spans="1:51">
+    <row r="121" spans="1:51" hidden="1">
       <c r="A121" s="2" t="s">
         <v>47</v>
       </c>
@@ -5491,7 +5494,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="122" spans="1:51">
+    <row r="122" spans="1:51" hidden="1">
       <c r="A122" s="2" t="s">
         <v>47</v>
       </c>
@@ -5536,7 +5539,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="123" spans="1:51">
+    <row r="123" spans="1:51" hidden="1">
       <c r="A123" s="2" t="s">
         <v>54</v>
       </c>
@@ -5590,7 +5593,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="124" spans="1:51">
+    <row r="124" spans="1:51" hidden="1">
       <c r="A124" s="2" t="s">
         <v>55</v>
       </c>
@@ -5629,7 +5632,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="125" spans="1:51">
+    <row r="125" spans="1:51" hidden="1">
       <c r="A125" s="2" t="s">
         <v>53</v>
       </c>
@@ -5665,7 +5668,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="126" spans="1:51">
+    <row r="126" spans="1:51" hidden="1">
       <c r="A126" s="2" t="s">
         <v>54</v>
       </c>
@@ -5701,7 +5704,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="127" spans="1:51">
+    <row r="127" spans="1:51" hidden="1">
       <c r="A127" s="2" t="s">
         <v>47</v>
       </c>
@@ -5737,7 +5740,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="128" spans="1:51">
+    <row r="128" spans="1:51" hidden="1">
       <c r="A128" s="2" t="s">
         <v>54</v>
       </c>
@@ -5776,7 +5779,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="129" spans="1:37">
+    <row r="129" spans="1:37" hidden="1">
       <c r="A129" s="2" t="s">
         <v>52</v>
       </c>
@@ -5812,7 +5815,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="130" spans="1:37">
+    <row r="130" spans="1:37" hidden="1">
       <c r="A130" s="2" t="s">
         <v>50</v>
       </c>
@@ -5851,7 +5854,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="131" spans="1:37">
+    <row r="131" spans="1:37" hidden="1">
       <c r="A131" s="2" t="s">
         <v>47</v>
       </c>
@@ -5887,7 +5890,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="132" spans="1:37">
+    <row r="132" spans="1:37" hidden="1">
       <c r="A132" s="2" t="s">
         <v>51</v>
       </c>
@@ -5926,7 +5929,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="133" spans="1:37">
+    <row r="133" spans="1:37" hidden="1">
       <c r="A133" s="2" t="s">
         <v>50</v>
       </c>
@@ -5962,7 +5965,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="134" spans="1:37">
+    <row r="134" spans="1:37" hidden="1">
       <c r="A134" s="2" t="s">
         <v>54</v>
       </c>
@@ -6022,7 +6025,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="135" spans="1:37">
+    <row r="135" spans="1:37" hidden="1">
       <c r="A135" s="2" t="s">
         <v>54</v>
       </c>
@@ -6064,7 +6067,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="136" spans="1:37">
+    <row r="136" spans="1:37" hidden="1">
       <c r="A136" s="2" t="s">
         <v>49</v>
       </c>
@@ -6103,7 +6106,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="137" spans="1:37">
+    <row r="137" spans="1:37" hidden="1">
       <c r="A137" s="2" t="s">
         <v>52</v>
       </c>
@@ -6139,7 +6142,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="138" spans="1:37">
+    <row r="138" spans="1:37" hidden="1">
       <c r="A138" s="2" t="s">
         <v>55</v>
       </c>
@@ -6175,7 +6178,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="139" spans="1:37">
+    <row r="139" spans="1:37" hidden="1">
       <c r="A139" s="2" t="s">
         <v>53</v>
       </c>
@@ -6217,7 +6220,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="140" spans="1:37">
+    <row r="140" spans="1:37" hidden="1">
       <c r="A140" s="2" t="s">
         <v>54</v>
       </c>
@@ -6253,7 +6256,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="141" spans="1:37">
+    <row r="141" spans="1:37" hidden="1">
       <c r="A141" s="2" t="s">
         <v>47</v>
       </c>
@@ -6295,7 +6298,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="142" spans="1:37">
+    <row r="142" spans="1:37" hidden="1">
       <c r="A142" s="2" t="s">
         <v>49</v>
       </c>
@@ -6331,7 +6334,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="143" spans="1:37">
+    <row r="143" spans="1:37" hidden="1">
       <c r="A143" s="2" t="s">
         <v>49</v>
       </c>
@@ -6367,7 +6370,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="144" spans="1:37">
+    <row r="144" spans="1:37" hidden="1">
       <c r="A144" s="2" t="s">
         <v>51</v>
       </c>
@@ -6403,7 +6406,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="145" spans="1:51">
+    <row r="145" spans="1:51" hidden="1">
       <c r="A145" s="2" t="s">
         <v>54</v>
       </c>
@@ -6445,7 +6448,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="146" spans="1:51">
+    <row r="146" spans="1:51" hidden="1">
       <c r="A146" s="2" t="s">
         <v>54</v>
       </c>
@@ -6481,7 +6484,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="147" spans="1:51">
+    <row r="147" spans="1:51" hidden="1">
       <c r="A147" s="2" t="s">
         <v>53</v>
       </c>
@@ -6517,7 +6520,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="148" spans="1:51">
+    <row r="148" spans="1:51" hidden="1">
       <c r="A148" s="2" t="s">
         <v>51</v>
       </c>
@@ -6559,7 +6562,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="149" spans="1:51">
+    <row r="149" spans="1:51" hidden="1">
       <c r="A149" s="2" t="s">
         <v>53</v>
       </c>
@@ -6595,7 +6598,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="150" spans="1:51">
+    <row r="150" spans="1:51" hidden="1">
       <c r="A150" s="2" t="s">
         <v>52</v>
       </c>
@@ -6631,7 +6634,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="151" spans="1:51">
+    <row r="151" spans="1:51" hidden="1">
       <c r="A151" s="2" t="s">
         <v>48</v>
       </c>
@@ -6670,7 +6673,7 @@
         <v>1873</v>
       </c>
     </row>
-    <row r="152" spans="1:51">
+    <row r="152" spans="1:51" hidden="1">
       <c r="A152" t="s">
         <v>54</v>
       </c>
@@ -6718,7 +6721,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="153" spans="1:51">
+    <row r="153" spans="1:51" hidden="1">
       <c r="A153" t="s">
         <v>53</v>
       </c>
@@ -6760,7 +6763,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="154" spans="1:51">
+    <row r="154" spans="1:51" hidden="1">
       <c r="A154" s="2" t="s">
         <v>47</v>
       </c>
@@ -6796,7 +6799,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="155" spans="1:51">
+    <row r="155" spans="1:51" hidden="1">
       <c r="A155" s="2" t="s">
         <v>52</v>
       </c>
@@ -6832,7 +6835,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="156" spans="1:51">
+    <row r="156" spans="1:51" hidden="1">
       <c r="A156" s="2" t="s">
         <v>54</v>
       </c>
@@ -6874,7 +6877,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="157" spans="1:51">
+    <row r="157" spans="1:51" hidden="1">
       <c r="A157" s="2" t="s">
         <v>49</v>
       </c>
@@ -6910,7 +6913,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="158" spans="1:51">
+    <row r="158" spans="1:51" hidden="1">
       <c r="A158" s="2" t="s">
         <v>55</v>
       </c>
@@ -6970,7 +6973,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="159" spans="1:51">
+    <row r="159" spans="1:51" hidden="1">
       <c r="A159" s="2" t="s">
         <v>52</v>
       </c>
@@ -7006,7 +7009,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="160" spans="1:51">
+    <row r="160" spans="1:51" hidden="1">
       <c r="A160" s="2" t="s">
         <v>49</v>
       </c>
@@ -7042,7 +7045,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="161" spans="1:51">
+    <row r="161" spans="1:51" hidden="1">
       <c r="A161" s="2" t="s">
         <v>55</v>
       </c>
@@ -7078,7 +7081,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="162" spans="1:51">
+    <row r="162" spans="1:51" hidden="1">
       <c r="A162" s="2" t="s">
         <v>50</v>
       </c>
@@ -7114,7 +7117,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="163" spans="1:51">
+    <row r="163" spans="1:51" hidden="1">
       <c r="A163" s="2" t="s">
         <v>48</v>
       </c>
@@ -7150,7 +7153,7 @@
         <v>1873</v>
       </c>
     </row>
-    <row r="164" spans="1:51">
+    <row r="164" spans="1:51" hidden="1">
       <c r="A164" s="2" t="s">
         <v>54</v>
       </c>
@@ -7186,7 +7189,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="165" spans="1:51">
+    <row r="165" spans="1:51" hidden="1">
       <c r="A165" s="2" t="s">
         <v>54</v>
       </c>
@@ -7228,7 +7231,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="166" spans="1:51">
+    <row r="166" spans="1:51" hidden="1">
       <c r="A166" s="2" t="s">
         <v>55</v>
       </c>
@@ -7267,7 +7270,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="167" spans="1:51">
+    <row r="167" spans="1:51" hidden="1">
       <c r="A167" s="2" t="s">
         <v>50</v>
       </c>
@@ -7309,7 +7312,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="168" spans="1:51">
+    <row r="168" spans="1:51" hidden="1">
       <c r="A168" s="2" t="s">
         <v>51</v>
       </c>
@@ -7345,7 +7348,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="169" spans="1:51">
+    <row r="169" spans="1:51" hidden="1">
       <c r="A169" s="2" t="s">
         <v>51</v>
       </c>
@@ -7384,7 +7387,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="170" spans="1:51">
+    <row r="170" spans="1:51" hidden="1">
       <c r="A170" s="2" t="s">
         <v>48</v>
       </c>
@@ -7426,7 +7429,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="171" spans="1:51" ht="16.5" customHeight="1">
+    <row r="171" spans="1:51" ht="16.5" hidden="1" customHeight="1">
       <c r="A171" s="2" t="s">
         <v>53</v>
       </c>
@@ -7465,7 +7468,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="172" spans="1:51">
+    <row r="172" spans="1:51" hidden="1">
       <c r="A172" s="2" t="s">
         <v>51</v>
       </c>
@@ -7501,7 +7504,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="173" spans="1:51">
+    <row r="173" spans="1:51" hidden="1">
       <c r="A173" s="2" t="s">
         <v>48</v>
       </c>
@@ -7585,7 +7588,7 @@
         <v>6.9</v>
       </c>
     </row>
-    <row r="175" spans="1:51">
+    <row r="175" spans="1:51" hidden="1">
       <c r="A175" s="2" t="s">
         <v>47</v>
       </c>
@@ -7621,7 +7624,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="176" spans="1:51">
+    <row r="176" spans="1:51" hidden="1">
       <c r="A176" s="2" t="s">
         <v>50</v>
       </c>
@@ -7657,7 +7660,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="177" spans="1:51">
+    <row r="177" spans="1:51" hidden="1">
       <c r="A177" s="2" t="s">
         <v>50</v>
       </c>
@@ -7693,7 +7696,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="178" spans="1:51">
+    <row r="178" spans="1:51" hidden="1">
       <c r="A178" s="2" t="s">
         <v>48</v>
       </c>
@@ -7729,7 +7732,7 @@
         <v>1873</v>
       </c>
     </row>
-    <row r="179" spans="1:51">
+    <row r="179" spans="1:51" hidden="1">
       <c r="A179" s="2" t="s">
         <v>52</v>
       </c>
@@ -7771,7 +7774,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="180" spans="1:51">
+    <row r="180" spans="1:51" hidden="1">
       <c r="A180" s="2" t="s">
         <v>49</v>
       </c>
@@ -7813,7 +7816,7 @@
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="181" spans="1:51">
+    <row r="181" spans="1:51" hidden="1">
       <c r="A181" s="2" t="s">
         <v>52</v>
       </c>
@@ -7858,7 +7861,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="182" spans="1:51">
+    <row r="182" spans="1:51" hidden="1">
       <c r="A182" s="2" t="s">
         <v>47</v>
       </c>
@@ -7894,7 +7897,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="183" spans="1:51">
+    <row r="183" spans="1:51" hidden="1">
       <c r="A183" s="2" t="s">
         <v>49</v>
       </c>
@@ -7930,7 +7933,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="184" spans="1:51">
+    <row r="184" spans="1:51" hidden="1">
       <c r="A184" s="2" t="s">
         <v>55</v>
       </c>
@@ -7969,7 +7972,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="185" spans="1:51">
+    <row r="185" spans="1:51" hidden="1">
       <c r="A185" s="2" t="s">
         <v>47</v>
       </c>
@@ -8005,7 +8008,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="186" spans="1:51">
+    <row r="186" spans="1:51" hidden="1">
       <c r="A186" s="2" t="s">
         <v>52</v>
       </c>
@@ -8041,7 +8044,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="187" spans="1:51">
+    <row r="187" spans="1:51" hidden="1">
       <c r="A187" t="s">
         <v>52</v>
       </c>
@@ -8156,7 +8159,7 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="188" spans="1:51">
+    <row r="188" spans="1:51" hidden="1">
       <c r="A188" s="2" t="s">
         <v>50</v>
       </c>
@@ -8214,7 +8217,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="189" spans="1:51">
+    <row r="189" spans="1:51" hidden="1">
       <c r="A189" t="s">
         <v>50</v>
       </c>
@@ -8268,7 +8271,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="190" spans="1:51">
+    <row r="190" spans="1:51" hidden="1">
       <c r="A190" s="2" t="s">
         <v>50</v>
       </c>
@@ -8341,7 +8344,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="191" spans="1:51">
+    <row r="191" spans="1:51" hidden="1">
       <c r="A191" s="2" t="s">
         <v>52</v>
       </c>
@@ -8399,7 +8402,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="192" spans="1:51">
+    <row r="192" spans="1:51" hidden="1">
       <c r="A192" s="2" t="s">
         <v>55</v>
       </c>
@@ -8508,7 +8511,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="193" spans="1:51">
+    <row r="193" spans="1:51" hidden="1">
       <c r="A193" s="2" t="s">
         <v>55</v>
       </c>
@@ -8569,7 +8572,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="194" spans="1:51">
+    <row r="194" spans="1:51" hidden="1">
       <c r="A194" t="s">
         <v>52</v>
       </c>
@@ -8626,7 +8629,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="195" spans="1:51">
+    <row r="195" spans="1:51" hidden="1">
       <c r="A195" s="2" t="s">
         <v>51</v>
       </c>
@@ -8729,7 +8732,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="196" spans="1:51">
+    <row r="196" spans="1:51" hidden="1">
       <c r="A196" s="2" t="s">
         <v>53</v>
       </c>
@@ -8790,7 +8793,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="197" spans="1:51">
+    <row r="197" spans="1:51" hidden="1">
       <c r="A197" s="2" t="s">
         <v>54</v>
       </c>
@@ -8905,7 +8908,7 @@
         <v>0.59</v>
       </c>
     </row>
-    <row r="198" spans="1:51">
+    <row r="198" spans="1:51" hidden="1">
       <c r="A198" s="2" t="s">
         <v>54</v>
       </c>
@@ -8960,7 +8963,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="199" spans="1:51">
+    <row r="199" spans="1:51" hidden="1">
       <c r="A199" s="2" t="s">
         <v>52</v>
       </c>
@@ -9030,7 +9033,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="200" spans="1:51">
+    <row r="200" spans="1:51" hidden="1">
       <c r="A200" t="s">
         <v>51</v>
       </c>
@@ -9087,7 +9090,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="201" spans="1:51">
+    <row r="201" spans="1:51" hidden="1">
       <c r="A201" s="2" t="s">
         <v>51</v>
       </c>
@@ -9145,7 +9148,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="202" spans="1:51">
+    <row r="202" spans="1:51" hidden="1">
       <c r="A202" s="2" t="s">
         <v>51</v>
       </c>
@@ -9209,7 +9212,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="203" spans="1:51">
+    <row r="203" spans="1:51" hidden="1">
       <c r="A203" s="2" t="s">
         <v>47</v>
       </c>
@@ -9257,7 +9260,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="204" spans="1:51">
+    <row r="204" spans="1:51" hidden="1">
       <c r="A204" s="2" t="s">
         <v>47</v>
       </c>
@@ -9295,7 +9298,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="205" spans="1:51">
+    <row r="205" spans="1:51" hidden="1">
       <c r="A205" s="2" t="s">
         <v>47</v>
       </c>
@@ -9329,7 +9332,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="206" spans="1:51">
+    <row r="206" spans="1:51" hidden="1">
       <c r="A206" s="2" t="s">
         <v>47</v>
       </c>
@@ -9366,7 +9369,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="207" spans="1:51">
+    <row r="207" spans="1:51" hidden="1">
       <c r="A207" s="2" t="s">
         <v>47</v>
       </c>
@@ -9400,7 +9403,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="208" spans="1:51">
+    <row r="208" spans="1:51" hidden="1">
       <c r="A208" s="2" t="s">
         <v>47</v>
       </c>
@@ -9440,7 +9443,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="209" spans="1:51">
+    <row r="209" spans="1:51" hidden="1">
       <c r="A209" s="2" t="s">
         <v>47</v>
       </c>
@@ -9471,7 +9474,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="210" spans="1:51">
+    <row r="210" spans="1:51" hidden="1">
       <c r="A210" s="2" t="s">
         <v>47</v>
       </c>
@@ -9508,7 +9511,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="211" spans="1:51">
+    <row r="211" spans="1:51" hidden="1">
       <c r="A211" s="2" t="s">
         <v>47</v>
       </c>
@@ -9542,7 +9545,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="212" spans="1:51">
+    <row r="212" spans="1:51" hidden="1">
       <c r="A212" s="2" t="s">
         <v>47</v>
       </c>
@@ -9576,7 +9579,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="213" spans="1:51">
+    <row r="213" spans="1:51" hidden="1">
       <c r="A213" s="2" t="s">
         <v>47</v>
       </c>
@@ -9613,7 +9616,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="214" spans="1:51">
+    <row r="214" spans="1:51" hidden="1">
       <c r="A214" s="2" t="s">
         <v>47</v>
       </c>
@@ -9653,7 +9656,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="215" spans="1:51">
+    <row r="215" spans="1:51" hidden="1">
       <c r="A215" s="2" t="s">
         <v>47</v>
       </c>
@@ -9699,7 +9702,7 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="216" spans="1:51">
+    <row r="216" spans="1:51" hidden="1">
       <c r="A216" s="2" t="s">
         <v>47</v>
       </c>
@@ -9736,7 +9739,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="217" spans="1:51">
+    <row r="217" spans="1:51" hidden="1">
       <c r="A217" s="2" t="s">
         <v>47</v>
       </c>
@@ -9773,7 +9776,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="218" spans="1:51">
+    <row r="218" spans="1:51" hidden="1">
       <c r="A218" s="2" t="s">
         <v>47</v>
       </c>
@@ -9807,7 +9810,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="219" spans="1:51">
+    <row r="219" spans="1:51" hidden="1">
       <c r="A219" s="2" t="s">
         <v>47</v>
       </c>
@@ -9841,7 +9844,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="220" spans="1:51">
+    <row r="220" spans="1:51" hidden="1">
       <c r="A220" s="2" t="s">
         <v>47</v>
       </c>
@@ -9878,7 +9881,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="221" spans="1:51">
+    <row r="221" spans="1:51" hidden="1">
       <c r="A221" s="2" t="s">
         <v>47</v>
       </c>
@@ -9915,7 +9918,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="222" spans="1:51">
+    <row r="222" spans="1:51" hidden="1">
       <c r="A222" s="2" t="s">
         <v>47</v>
       </c>
@@ -9976,7 +9979,7 @@
         <v>5.16</v>
       </c>
     </row>
-    <row r="223" spans="1:51">
+    <row r="223" spans="1:51" hidden="1">
       <c r="A223" s="2" t="s">
         <v>47</v>
       </c>
@@ -10013,7 +10016,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="224" spans="1:51">
+    <row r="224" spans="1:51" hidden="1">
       <c r="A224" s="2" t="s">
         <v>47</v>
       </c>
@@ -10047,7 +10050,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="225" spans="1:50">
+    <row r="225" spans="1:50" hidden="1">
       <c r="A225" s="2" t="s">
         <v>47</v>
       </c>
@@ -10081,7 +10084,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="226" spans="1:50">
+    <row r="226" spans="1:50" hidden="1">
       <c r="A226" s="2" t="s">
         <v>47</v>
       </c>
@@ -10115,7 +10118,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="227" spans="1:50">
+    <row r="227" spans="1:50" hidden="1">
       <c r="A227" s="2" t="s">
         <v>47</v>
       </c>
@@ -10152,7 +10155,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="228" spans="1:50">
+    <row r="228" spans="1:50" hidden="1">
       <c r="A228" s="2" t="s">
         <v>47</v>
       </c>
@@ -10186,7 +10189,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="229" spans="1:50">
+    <row r="229" spans="1:50" hidden="1">
       <c r="A229" s="2" t="s">
         <v>47</v>
       </c>
@@ -10220,7 +10223,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="230" spans="1:50">
+    <row r="230" spans="1:50" hidden="1">
       <c r="A230" s="2" t="s">
         <v>47</v>
       </c>
@@ -10251,7 +10254,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="231" spans="1:50">
+    <row r="231" spans="1:50" hidden="1">
       <c r="A231" s="2" t="s">
         <v>47</v>
       </c>
@@ -10285,7 +10288,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="232" spans="1:50">
+    <row r="232" spans="1:50" hidden="1">
       <c r="A232" s="2" t="s">
         <v>47</v>
       </c>
@@ -10325,7 +10328,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="233" spans="1:50">
+    <row r="233" spans="1:50" hidden="1">
       <c r="A233" s="2" t="s">
         <v>47</v>
       </c>
@@ -10404,7 +10407,7 @@
         <v>0.63</v>
       </c>
     </row>
-    <row r="234" spans="1:50">
+    <row r="234" spans="1:50" hidden="1">
       <c r="A234" s="2" t="s">
         <v>47</v>
       </c>
@@ -10438,7 +10441,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="235" spans="1:50">
+    <row r="235" spans="1:50" hidden="1">
       <c r="A235" s="2" t="s">
         <v>47</v>
       </c>
@@ -10472,7 +10475,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="236" spans="1:50">
+    <row r="236" spans="1:50" hidden="1">
       <c r="A236" s="2" t="s">
         <v>47</v>
       </c>
@@ -10506,7 +10509,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="237" spans="1:50">
+    <row r="237" spans="1:50" hidden="1">
       <c r="A237" s="2" t="s">
         <v>47</v>
       </c>
@@ -10540,7 +10543,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="238" spans="1:50">
+    <row r="238" spans="1:50" hidden="1">
       <c r="A238" s="2" t="s">
         <v>47</v>
       </c>
@@ -10577,7 +10580,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="239" spans="1:50">
+    <row r="239" spans="1:50" hidden="1">
       <c r="A239" s="2" t="s">
         <v>47</v>
       </c>
@@ -10614,7 +10617,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="240" spans="1:50">
+    <row r="240" spans="1:50" hidden="1">
       <c r="A240" s="2" t="s">
         <v>47</v>
       </c>
@@ -10672,7 +10675,7 @@
         <v>2.68</v>
       </c>
     </row>
-    <row r="241" spans="1:43">
+    <row r="241" spans="1:43" hidden="1">
       <c r="A241" s="2" t="s">
         <v>47</v>
       </c>
@@ -10706,7 +10709,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="242" spans="1:43">
+    <row r="242" spans="1:43" hidden="1">
       <c r="A242" s="2" t="s">
         <v>47</v>
       </c>
@@ -10743,7 +10746,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="243" spans="1:43">
+    <row r="243" spans="1:43" hidden="1">
       <c r="A243" s="2" t="s">
         <v>50</v>
       </c>
@@ -10777,7 +10780,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="244" spans="1:43">
+    <row r="244" spans="1:43" hidden="1">
       <c r="A244" s="2" t="s">
         <v>50</v>
       </c>
@@ -10814,7 +10817,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="245" spans="1:43">
+    <row r="245" spans="1:43" hidden="1">
       <c r="A245" s="2" t="s">
         <v>50</v>
       </c>
@@ -10851,7 +10854,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="246" spans="1:43">
+    <row r="246" spans="1:43" hidden="1">
       <c r="A246" s="2" t="s">
         <v>50</v>
       </c>
@@ -10888,7 +10891,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="247" spans="1:43">
+    <row r="247" spans="1:43" hidden="1">
       <c r="A247" s="2" t="s">
         <v>50</v>
       </c>
@@ -10922,7 +10925,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="248" spans="1:43">
+    <row r="248" spans="1:43" hidden="1">
       <c r="A248" s="2" t="s">
         <v>50</v>
       </c>
@@ -10959,7 +10962,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="249" spans="1:43">
+    <row r="249" spans="1:43" hidden="1">
       <c r="A249" s="2" t="s">
         <v>50</v>
       </c>
@@ -10996,7 +10999,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="250" spans="1:43">
+    <row r="250" spans="1:43" hidden="1">
       <c r="A250" s="2" t="s">
         <v>50</v>
       </c>
@@ -11030,7 +11033,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="251" spans="1:43">
+    <row r="251" spans="1:43" hidden="1">
       <c r="A251" s="2" t="s">
         <v>50</v>
       </c>
@@ -11067,7 +11070,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="252" spans="1:43">
+    <row r="252" spans="1:43" hidden="1">
       <c r="A252" s="2" t="s">
         <v>50</v>
       </c>
@@ -11107,7 +11110,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="253" spans="1:43">
+    <row r="253" spans="1:43" hidden="1">
       <c r="A253" s="2" t="s">
         <v>50</v>
       </c>
@@ -11153,7 +11156,7 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="254" spans="1:43">
+    <row r="254" spans="1:43" hidden="1">
       <c r="A254" s="2" t="s">
         <v>50</v>
       </c>
@@ -11187,7 +11190,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="255" spans="1:43">
+    <row r="255" spans="1:43" hidden="1">
       <c r="A255" s="2" t="s">
         <v>50</v>
       </c>
@@ -11224,7 +11227,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="256" spans="1:43">
+    <row r="256" spans="1:43" hidden="1">
       <c r="A256" s="2" t="s">
         <v>50</v>
       </c>
@@ -11258,7 +11261,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="257" spans="1:50">
+    <row r="257" spans="1:50" hidden="1">
       <c r="A257" s="2" t="s">
         <v>50</v>
       </c>
@@ -11292,7 +11295,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="258" spans="1:50">
+    <row r="258" spans="1:50" hidden="1">
       <c r="A258" s="2" t="s">
         <v>50</v>
       </c>
@@ -11326,7 +11329,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="259" spans="1:50">
+    <row r="259" spans="1:50" hidden="1">
       <c r="A259" s="2" t="s">
         <v>50</v>
       </c>
@@ -11363,7 +11366,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="260" spans="1:50">
+    <row r="260" spans="1:50" hidden="1">
       <c r="A260" s="2" t="s">
         <v>50</v>
       </c>
@@ -11409,7 +11412,7 @@
         <v>4.2699999999999996</v>
       </c>
     </row>
-    <row r="261" spans="1:50">
+    <row r="261" spans="1:50" hidden="1">
       <c r="A261" s="2" t="s">
         <v>50</v>
       </c>
@@ -11449,7 +11452,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="262" spans="1:50">
+    <row r="262" spans="1:50" hidden="1">
       <c r="A262" s="2" t="s">
         <v>50</v>
       </c>
@@ -11486,7 +11489,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="263" spans="1:50">
+    <row r="263" spans="1:50" hidden="1">
       <c r="A263" s="2" t="s">
         <v>50</v>
       </c>
@@ -11523,7 +11526,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="264" spans="1:50">
+    <row r="264" spans="1:50" hidden="1">
       <c r="A264" s="2" t="s">
         <v>50</v>
       </c>
@@ -11557,7 +11560,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="265" spans="1:50">
+    <row r="265" spans="1:50" hidden="1">
       <c r="A265" s="2" t="s">
         <v>50</v>
       </c>
@@ -11591,7 +11594,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="266" spans="1:50">
+    <row r="266" spans="1:50" hidden="1">
       <c r="A266" s="2" t="s">
         <v>50</v>
       </c>
@@ -11625,7 +11628,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="267" spans="1:50">
+    <row r="267" spans="1:50" hidden="1">
       <c r="A267" s="2" t="s">
         <v>50</v>
       </c>
@@ -11662,7 +11665,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="268" spans="1:50">
+    <row r="268" spans="1:50" hidden="1">
       <c r="A268" s="2" t="s">
         <v>50</v>
       </c>
@@ -11699,7 +11702,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="269" spans="1:50">
+    <row r="269" spans="1:50" hidden="1">
       <c r="A269" s="2" t="s">
         <v>50</v>
       </c>
@@ -11733,7 +11736,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="270" spans="1:50">
+    <row r="270" spans="1:50" hidden="1">
       <c r="A270" s="2" t="s">
         <v>50</v>
       </c>
@@ -11776,7 +11779,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="271" spans="1:50">
+    <row r="271" spans="1:50" hidden="1">
       <c r="A271" t="s">
         <v>50</v>
       </c>
@@ -11810,7 +11813,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="272" spans="1:50">
+    <row r="272" spans="1:50" hidden="1">
       <c r="A272" s="2" t="s">
         <v>50</v>
       </c>
@@ -11874,7 +11877,7 @@
         <v>1.98</v>
       </c>
     </row>
-    <row r="273" spans="1:51">
+    <row r="273" spans="1:51" hidden="1">
       <c r="A273" s="2" t="s">
         <v>53</v>
       </c>
@@ -11913,7 +11916,7 @@
         <v>53</v>
       </c>
       <c r="B274" s="5">
-        <v>35775</v>
+        <v>35789</v>
       </c>
       <c r="C274" s="5"/>
       <c r="D274" s="6">
@@ -11947,7 +11950,7 @@
         <v>53</v>
       </c>
       <c r="B275" s="5">
-        <v>35803</v>
+        <v>35817</v>
       </c>
       <c r="C275" s="5"/>
       <c r="D275" s="6">
@@ -11976,7 +11979,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="276" spans="1:51">
+    <row r="276" spans="1:51" hidden="1">
       <c r="A276" s="2" t="s">
         <v>53</v>
       </c>
@@ -12019,7 +12022,7 @@
         <v>53</v>
       </c>
       <c r="B277" s="5">
-        <v>35817</v>
+        <v>35831</v>
       </c>
       <c r="C277" s="5"/>
       <c r="D277" s="6">
@@ -12054,7 +12057,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="278" spans="1:51">
+    <row r="278" spans="1:51" hidden="1">
       <c r="A278" s="2" t="s">
         <v>53</v>
       </c>
@@ -12091,7 +12094,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="279" spans="1:51">
+    <row r="279" spans="1:51" hidden="1">
       <c r="A279" s="2" t="s">
         <v>53</v>
       </c>
@@ -12130,7 +12133,7 @@
         <v>53</v>
       </c>
       <c r="B280" s="5">
-        <v>35831</v>
+        <v>35814</v>
       </c>
       <c r="C280" s="5"/>
       <c r="D280" s="6">
@@ -12162,7 +12165,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="281" spans="1:51">
+    <row r="281" spans="1:51" hidden="1">
       <c r="A281" s="2" t="s">
         <v>53</v>
       </c>
@@ -12196,7 +12199,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="282" spans="1:51">
+    <row r="282" spans="1:51" hidden="1">
       <c r="A282" s="2" t="s">
         <v>53</v>
       </c>
@@ -12235,7 +12238,7 @@
         <v>53</v>
       </c>
       <c r="B283" s="5">
-        <v>35837</v>
+        <v>35851</v>
       </c>
       <c r="C283" s="5"/>
       <c r="D283" s="6">
@@ -12273,7 +12276,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="284" spans="1:51">
+    <row r="284" spans="1:51" hidden="1">
       <c r="A284" s="2" t="s">
         <v>53</v>
       </c>
@@ -12307,7 +12310,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="285" spans="1:51">
+    <row r="285" spans="1:51" hidden="1">
       <c r="A285" t="s">
         <v>53</v>
       </c>
@@ -12344,7 +12347,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="286" spans="1:51">
+    <row r="286" spans="1:51" hidden="1">
       <c r="A286" s="2" t="s">
         <v>53</v>
       </c>
@@ -12381,7 +12384,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="287" spans="1:51">
+    <row r="287" spans="1:51" hidden="1">
       <c r="A287" s="2" t="s">
         <v>53</v>
       </c>
@@ -12424,7 +12427,7 @@
         <v>2.3E-2</v>
       </c>
     </row>
-    <row r="288" spans="1:51">
+    <row r="288" spans="1:51" hidden="1">
       <c r="A288" s="2" t="s">
         <v>53</v>
       </c>
@@ -12458,7 +12461,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="289" spans="1:51">
+    <row r="289" spans="1:51" hidden="1">
       <c r="A289" s="2" t="s">
         <v>53</v>
       </c>
@@ -12492,7 +12495,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="290" spans="1:51">
+    <row r="290" spans="1:51" hidden="1">
       <c r="A290" s="2" t="s">
         <v>53</v>
       </c>
@@ -12529,7 +12532,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="291" spans="1:51">
+    <row r="291" spans="1:51" hidden="1">
       <c r="A291" s="2" t="s">
         <v>53</v>
       </c>
@@ -12566,7 +12569,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="292" spans="1:51">
+    <row r="292" spans="1:51" hidden="1">
       <c r="A292" s="2" t="s">
         <v>53</v>
       </c>
@@ -12600,7 +12603,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="293" spans="1:51">
+    <row r="293" spans="1:51" hidden="1">
       <c r="A293" s="2" t="s">
         <v>53</v>
       </c>
@@ -12634,7 +12637,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="294" spans="1:51">
+    <row r="294" spans="1:51" hidden="1">
       <c r="A294" t="s">
         <v>53</v>
       </c>
@@ -12668,7 +12671,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="295" spans="1:51">
+    <row r="295" spans="1:51" hidden="1">
       <c r="A295" s="2" t="s">
         <v>53</v>
       </c>
@@ -12720,7 +12723,7 @@
         <v>4.1100000000000003</v>
       </c>
     </row>
-    <row r="296" spans="1:51">
+    <row r="296" spans="1:51" hidden="1">
       <c r="A296" s="2" t="s">
         <v>53</v>
       </c>
@@ -12757,7 +12760,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="297" spans="1:51">
+    <row r="297" spans="1:51" hidden="1">
       <c r="A297" s="2" t="s">
         <v>53</v>
       </c>
@@ -12794,7 +12797,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="298" spans="1:51">
+    <row r="298" spans="1:51" hidden="1">
       <c r="A298" t="s">
         <v>53</v>
       </c>
@@ -12828,7 +12831,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="299" spans="1:51">
+    <row r="299" spans="1:51" hidden="1">
       <c r="A299" s="2" t="s">
         <v>53</v>
       </c>
@@ -12862,7 +12865,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="300" spans="1:51">
+    <row r="300" spans="1:51" hidden="1">
       <c r="A300" s="2" t="s">
         <v>53</v>
       </c>
@@ -12899,7 +12902,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="301" spans="1:51">
+    <row r="301" spans="1:51" hidden="1">
       <c r="A301" s="2" t="s">
         <v>53</v>
       </c>
@@ -12939,7 +12942,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="302" spans="1:51">
+    <row r="302" spans="1:51" hidden="1">
       <c r="A302" s="2" t="s">
         <v>53</v>
       </c>
@@ -12985,7 +12988,7 @@
         <v>5.9</v>
       </c>
     </row>
-    <row r="303" spans="1:51">
+    <row r="303" spans="1:51" hidden="1">
       <c r="A303" s="2" t="s">
         <v>53</v>
       </c>
@@ -13028,7 +13031,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="304" spans="1:51">
+    <row r="304" spans="1:51" hidden="1">
       <c r="A304" s="2" t="s">
         <v>53</v>
       </c>
@@ -13065,7 +13068,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="305" spans="1:51">
+    <row r="305" spans="1:51" hidden="1">
       <c r="A305" s="2" t="s">
         <v>53</v>
       </c>
@@ -13102,7 +13105,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="306" spans="1:51">
+    <row r="306" spans="1:51" hidden="1">
       <c r="A306" t="s">
         <v>53</v>
       </c>
@@ -13136,7 +13139,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="307" spans="1:51">
+    <row r="307" spans="1:51" hidden="1">
       <c r="A307" s="2" t="s">
         <v>48</v>
       </c>
@@ -13169,7 +13172,7 @@
         <v>1873</v>
       </c>
     </row>
-    <row r="308" spans="1:51">
+    <row r="308" spans="1:51" hidden="1">
       <c r="A308" s="2" t="s">
         <v>48</v>
       </c>
@@ -13205,7 +13208,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="309" spans="1:51">
+    <row r="309" spans="1:51" hidden="1">
       <c r="A309" s="2" t="s">
         <v>48</v>
       </c>
@@ -13239,7 +13242,7 @@
         <v>1873</v>
       </c>
     </row>
-    <row r="310" spans="1:51">
+    <row r="310" spans="1:51" hidden="1">
       <c r="A310" s="2" t="s">
         <v>48</v>
       </c>
@@ -13276,7 +13279,7 @@
         <v>1873</v>
       </c>
     </row>
-    <row r="311" spans="1:51">
+    <row r="311" spans="1:51" hidden="1">
       <c r="A311" s="2" t="s">
         <v>48</v>
       </c>
@@ -13310,7 +13313,7 @@
         <v>1873</v>
       </c>
     </row>
-    <row r="312" spans="1:51">
+    <row r="312" spans="1:51" hidden="1">
       <c r="A312" s="2" t="s">
         <v>48</v>
       </c>
@@ -13344,7 +13347,7 @@
         <v>1873</v>
       </c>
     </row>
-    <row r="313" spans="1:51">
+    <row r="313" spans="1:51" hidden="1">
       <c r="A313" s="2" t="s">
         <v>48</v>
       </c>
@@ -13378,7 +13381,7 @@
         <v>1873</v>
       </c>
     </row>
-    <row r="314" spans="1:51">
+    <row r="314" spans="1:51" hidden="1">
       <c r="A314" s="2" t="s">
         <v>48</v>
       </c>
@@ -13412,7 +13415,7 @@
         <v>1873</v>
       </c>
     </row>
-    <row r="315" spans="1:51">
+    <row r="315" spans="1:51" hidden="1">
       <c r="A315" s="2" t="s">
         <v>48</v>
       </c>
@@ -13446,7 +13449,7 @@
         <v>1873</v>
       </c>
     </row>
-    <row r="316" spans="1:51">
+    <row r="316" spans="1:51" hidden="1">
       <c r="A316" s="2" t="s">
         <v>48</v>
       </c>
@@ -13489,7 +13492,7 @@
         <v>1873</v>
       </c>
     </row>
-    <row r="317" spans="1:51">
+    <row r="317" spans="1:51" hidden="1">
       <c r="A317" s="2" t="s">
         <v>48</v>
       </c>
@@ -13532,7 +13535,7 @@
         <v>3.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="318" spans="1:51">
+    <row r="318" spans="1:51" hidden="1">
       <c r="A318" s="2" t="s">
         <v>48</v>
       </c>
@@ -13569,7 +13572,7 @@
         <v>1873</v>
       </c>
     </row>
-    <row r="319" spans="1:51">
+    <row r="319" spans="1:51" hidden="1">
       <c r="A319" s="2" t="s">
         <v>48</v>
       </c>
@@ -13603,7 +13606,7 @@
         <v>1873</v>
       </c>
     </row>
-    <row r="320" spans="1:51">
+    <row r="320" spans="1:51" hidden="1">
       <c r="A320" s="2" t="s">
         <v>48</v>
       </c>
@@ -13637,7 +13640,7 @@
         <v>1873</v>
       </c>
     </row>
-    <row r="321" spans="1:51">
+    <row r="321" spans="1:51" hidden="1">
       <c r="A321" s="2" t="s">
         <v>48</v>
       </c>
@@ -13671,7 +13674,7 @@
         <v>1873</v>
       </c>
     </row>
-    <row r="322" spans="1:51">
+    <row r="322" spans="1:51" hidden="1">
       <c r="A322" s="2" t="s">
         <v>48</v>
       </c>
@@ -13711,7 +13714,7 @@
         <v>1873</v>
       </c>
     </row>
-    <row r="323" spans="1:51">
+    <row r="323" spans="1:51" hidden="1">
       <c r="A323" s="2" t="s">
         <v>48</v>
       </c>
@@ -13745,7 +13748,7 @@
         <v>1873</v>
       </c>
     </row>
-    <row r="324" spans="1:51">
+    <row r="324" spans="1:51" hidden="1">
       <c r="A324" s="2" t="s">
         <v>48</v>
       </c>
@@ -13797,7 +13800,7 @@
         <v>7.83</v>
       </c>
     </row>
-    <row r="325" spans="1:51">
+    <row r="325" spans="1:51" hidden="1">
       <c r="A325" s="2" t="s">
         <v>48</v>
       </c>
@@ -13840,7 +13843,7 @@
         <v>1873</v>
       </c>
     </row>
-    <row r="326" spans="1:51">
+    <row r="326" spans="1:51" hidden="1">
       <c r="A326" s="2" t="s">
         <v>48</v>
       </c>
@@ -13874,7 +13877,7 @@
         <v>1873</v>
       </c>
     </row>
-    <row r="327" spans="1:51">
+    <row r="327" spans="1:51" hidden="1">
       <c r="A327" s="2" t="s">
         <v>48</v>
       </c>
@@ -13908,7 +13911,7 @@
         <v>1873</v>
       </c>
     </row>
-    <row r="328" spans="1:51">
+    <row r="328" spans="1:51" hidden="1">
       <c r="A328" s="2" t="s">
         <v>48</v>
       </c>
@@ -13942,7 +13945,7 @@
         <v>1873</v>
       </c>
     </row>
-    <row r="329" spans="1:51">
+    <row r="329" spans="1:51" hidden="1">
       <c r="A329" s="2" t="s">
         <v>48</v>
       </c>
@@ -13976,7 +13979,7 @@
         <v>1873</v>
       </c>
     </row>
-    <row r="330" spans="1:51">
+    <row r="330" spans="1:51" hidden="1">
       <c r="A330" s="2" t="s">
         <v>48</v>
       </c>
@@ -14010,7 +14013,7 @@
         <v>1873</v>
       </c>
     </row>
-    <row r="331" spans="1:51">
+    <row r="331" spans="1:51" hidden="1">
       <c r="A331" s="2" t="s">
         <v>48</v>
       </c>
@@ -14044,7 +14047,7 @@
         <v>1873</v>
       </c>
     </row>
-    <row r="332" spans="1:51">
+    <row r="332" spans="1:51" hidden="1">
       <c r="A332" s="2" t="s">
         <v>48</v>
       </c>
@@ -14078,7 +14081,7 @@
         <v>1873</v>
       </c>
     </row>
-    <row r="333" spans="1:51">
+    <row r="333" spans="1:51" hidden="1">
       <c r="A333" s="2" t="s">
         <v>48</v>
       </c>
@@ -14112,7 +14115,7 @@
         <v>1873</v>
       </c>
     </row>
-    <row r="334" spans="1:51">
+    <row r="334" spans="1:51" hidden="1">
       <c r="A334" s="2" t="s">
         <v>48</v>
       </c>
@@ -14155,7 +14158,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="335" spans="1:51">
+    <row r="335" spans="1:51" hidden="1">
       <c r="A335" s="2" t="s">
         <v>48</v>
       </c>
@@ -14192,7 +14195,7 @@
         <v>1873</v>
       </c>
     </row>
-    <row r="336" spans="1:51">
+    <row r="336" spans="1:51" hidden="1">
       <c r="A336" s="2" t="s">
         <v>48</v>
       </c>
@@ -14268,7 +14271,7 @@
         <v>0.63</v>
       </c>
     </row>
-    <row r="337" spans="1:50">
+    <row r="337" spans="1:50" hidden="1">
       <c r="A337" s="2" t="s">
         <v>48</v>
       </c>
@@ -14302,7 +14305,7 @@
         <v>1873</v>
       </c>
     </row>
-    <row r="338" spans="1:50">
+    <row r="338" spans="1:50" hidden="1">
       <c r="A338" s="2" t="s">
         <v>48</v>
       </c>
@@ -14336,7 +14339,7 @@
         <v>1873</v>
       </c>
     </row>
-    <row r="339" spans="1:50">
+    <row r="339" spans="1:50" hidden="1">
       <c r="A339" s="2" t="s">
         <v>48</v>
       </c>
@@ -14373,7 +14376,7 @@
         <v>1873</v>
       </c>
     </row>
-    <row r="340" spans="1:50">
+    <row r="340" spans="1:50" hidden="1">
       <c r="A340" s="2" t="s">
         <v>48</v>
       </c>
@@ -14410,7 +14413,7 @@
         <v>1873</v>
       </c>
     </row>
-    <row r="341" spans="1:50">
+    <row r="341" spans="1:50" hidden="1">
       <c r="A341" s="2" t="s">
         <v>48</v>
       </c>
@@ -14453,7 +14456,7 @@
         <v>1873</v>
       </c>
     </row>
-    <row r="342" spans="1:50">
+    <row r="342" spans="1:50" hidden="1">
       <c r="A342" s="2" t="s">
         <v>48</v>
       </c>
@@ -14487,7 +14490,7 @@
         <v>1873</v>
       </c>
     </row>
-    <row r="343" spans="1:50">
+    <row r="343" spans="1:50" hidden="1">
       <c r="A343" s="2" t="s">
         <v>48</v>
       </c>
@@ -14527,7 +14530,7 @@
         <v>1873</v>
       </c>
     </row>
-    <row r="344" spans="1:50">
+    <row r="344" spans="1:50" hidden="1">
       <c r="A344" s="2" t="s">
         <v>48</v>
       </c>
@@ -14561,7 +14564,7 @@
         <v>1873</v>
       </c>
     </row>
-    <row r="345" spans="1:50">
+    <row r="345" spans="1:50" hidden="1">
       <c r="A345" s="2" t="s">
         <v>48</v>
       </c>
@@ -14595,7 +14598,7 @@
         <v>1873</v>
       </c>
     </row>
-    <row r="346" spans="1:50">
+    <row r="346" spans="1:50" hidden="1">
       <c r="A346" s="2" t="s">
         <v>48</v>
       </c>
@@ -14659,7 +14662,7 @@
         <v>2.64</v>
       </c>
     </row>
-    <row r="347" spans="1:50">
+    <row r="347" spans="1:50" hidden="1">
       <c r="A347" s="2" t="s">
         <v>51</v>
       </c>
@@ -14693,7 +14696,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="348" spans="1:50">
+    <row r="348" spans="1:50" hidden="1">
       <c r="A348" s="2" t="s">
         <v>51</v>
       </c>
@@ -14730,7 +14733,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="349" spans="1:50">
+    <row r="349" spans="1:50" hidden="1">
       <c r="A349" s="2" t="s">
         <v>51</v>
       </c>
@@ -14767,7 +14770,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="350" spans="1:50">
+    <row r="350" spans="1:50" hidden="1">
       <c r="A350" s="2" t="s">
         <v>51</v>
       </c>
@@ -14804,7 +14807,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="351" spans="1:50">
+    <row r="351" spans="1:50" hidden="1">
       <c r="A351" s="2" t="s">
         <v>51</v>
       </c>
@@ -14838,7 +14841,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="352" spans="1:50">
+    <row r="352" spans="1:50" hidden="1">
       <c r="A352" s="2" t="s">
         <v>51</v>
       </c>
@@ -14872,7 +14875,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="353" spans="1:49">
+    <row r="353" spans="1:49" hidden="1">
       <c r="A353" s="2" t="s">
         <v>51</v>
       </c>
@@ -14906,7 +14909,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="354" spans="1:49">
+    <row r="354" spans="1:49" hidden="1">
       <c r="A354" s="2" t="s">
         <v>51</v>
       </c>
@@ -14943,7 +14946,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="355" spans="1:49">
+    <row r="355" spans="1:49" hidden="1">
       <c r="A355" s="2" t="s">
         <v>51</v>
       </c>
@@ -14989,7 +14992,7 @@
         <v>3.7200000000000004E-2</v>
       </c>
     </row>
-    <row r="356" spans="1:49">
+    <row r="356" spans="1:49" hidden="1">
       <c r="A356" s="2" t="s">
         <v>51</v>
       </c>
@@ -15023,7 +15026,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="357" spans="1:49">
+    <row r="357" spans="1:49" hidden="1">
       <c r="A357" s="2" t="s">
         <v>51</v>
       </c>
@@ -15057,7 +15060,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="358" spans="1:49">
+    <row r="358" spans="1:49" hidden="1">
       <c r="A358" s="2" t="s">
         <v>51</v>
       </c>
@@ -15091,7 +15094,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="359" spans="1:49">
+    <row r="359" spans="1:49" hidden="1">
       <c r="A359" s="2" t="s">
         <v>51</v>
       </c>
@@ -15125,7 +15128,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="360" spans="1:49">
+    <row r="360" spans="1:49" hidden="1">
       <c r="A360" s="2" t="s">
         <v>51</v>
       </c>
@@ -15159,7 +15162,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="361" spans="1:49">
+    <row r="361" spans="1:49" hidden="1">
       <c r="A361" s="2" t="s">
         <v>51</v>
       </c>
@@ -15199,7 +15202,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="362" spans="1:49">
+    <row r="362" spans="1:49" hidden="1">
       <c r="A362" t="s">
         <v>51</v>
       </c>
@@ -15236,7 +15239,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="363" spans="1:49">
+    <row r="363" spans="1:49" hidden="1">
       <c r="A363" s="2" t="s">
         <v>51</v>
       </c>
@@ -15297,7 +15300,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="364" spans="1:49">
+    <row r="364" spans="1:49" hidden="1">
       <c r="A364" s="2" t="s">
         <v>51</v>
       </c>
@@ -15331,7 +15334,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="365" spans="1:49">
+    <row r="365" spans="1:49" hidden="1">
       <c r="A365" s="2" t="s">
         <v>51</v>
       </c>
@@ -15365,7 +15368,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="366" spans="1:49">
+    <row r="366" spans="1:49" hidden="1">
       <c r="A366" s="2" t="s">
         <v>51</v>
       </c>
@@ -15399,7 +15402,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="367" spans="1:49">
+    <row r="367" spans="1:49" hidden="1">
       <c r="A367" s="2" t="s">
         <v>51</v>
       </c>
@@ -15436,7 +15439,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="368" spans="1:49">
+    <row r="368" spans="1:49" hidden="1">
       <c r="A368" s="2" t="s">
         <v>51</v>
       </c>
@@ -15470,7 +15473,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="369" spans="1:51">
+    <row r="369" spans="1:51" hidden="1">
       <c r="A369" s="2" t="s">
         <v>51</v>
       </c>
@@ -15513,7 +15516,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="370" spans="1:51">
+    <row r="370" spans="1:51" hidden="1">
       <c r="A370" s="2" t="s">
         <v>51</v>
       </c>
@@ -15550,7 +15553,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="371" spans="1:51">
+    <row r="371" spans="1:51" hidden="1">
       <c r="A371" s="2" t="s">
         <v>51</v>
       </c>
@@ -15584,7 +15587,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="372" spans="1:51">
+    <row r="372" spans="1:51" hidden="1">
       <c r="A372" s="2" t="s">
         <v>51</v>
       </c>
@@ -15618,7 +15621,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="373" spans="1:51">
+    <row r="373" spans="1:51" hidden="1">
       <c r="A373" s="2" t="s">
         <v>51</v>
       </c>
@@ -15652,7 +15655,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="374" spans="1:51">
+    <row r="374" spans="1:51" hidden="1">
       <c r="A374" s="2" t="s">
         <v>51</v>
       </c>
@@ -15686,7 +15689,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="375" spans="1:51">
+    <row r="375" spans="1:51" hidden="1">
       <c r="A375" s="2" t="s">
         <v>51</v>
       </c>
@@ -15720,7 +15723,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="376" spans="1:51">
+    <row r="376" spans="1:51" hidden="1">
       <c r="A376" s="2" t="s">
         <v>51</v>
       </c>
@@ -15754,7 +15757,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="377" spans="1:51">
+    <row r="377" spans="1:51" hidden="1">
       <c r="A377" s="2" t="s">
         <v>51</v>
       </c>
@@ -15794,7 +15797,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="378" spans="1:51">
+    <row r="378" spans="1:51" hidden="1">
       <c r="A378" s="2" t="s">
         <v>51</v>
       </c>
@@ -15831,7 +15834,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="379" spans="1:51">
+    <row r="379" spans="1:51" hidden="1">
       <c r="A379" s="2" t="s">
         <v>51</v>
       </c>
@@ -15868,7 +15871,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="380" spans="1:51">
+    <row r="380" spans="1:51" hidden="1">
       <c r="A380" s="2" t="s">
         <v>54</v>
       </c>
@@ -15907,7 +15910,7 @@
         <v>54</v>
       </c>
       <c r="B381" s="5">
-        <v>35775</v>
+        <v>35802</v>
       </c>
       <c r="C381" s="5"/>
       <c r="D381" s="6">
@@ -15936,7 +15939,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="382" spans="1:51">
+    <row r="382" spans="1:51" hidden="1">
       <c r="A382" s="2" t="s">
         <v>54</v>
       </c>
@@ -15978,7 +15981,7 @@
         <v>54</v>
       </c>
       <c r="B383" s="5">
-        <v>35803</v>
+        <v>35830</v>
       </c>
       <c r="C383" s="5"/>
       <c r="D383" s="6">
@@ -16007,7 +16010,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="384" spans="1:51">
+    <row r="384" spans="1:51" hidden="1">
       <c r="A384" s="2" t="s">
         <v>54</v>
       </c>
@@ -16052,7 +16055,7 @@
         <v>54</v>
       </c>
       <c r="B385" s="5">
-        <v>35817</v>
+        <v>35844</v>
       </c>
       <c r="C385" s="5"/>
       <c r="D385" s="6">
@@ -16089,7 +16092,7 @@
         <v>54</v>
       </c>
       <c r="B386" s="5">
-        <v>35830</v>
+        <v>35857</v>
       </c>
       <c r="C386" s="5"/>
       <c r="D386" s="6">
@@ -16118,7 +16121,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="387" spans="1:43">
+    <row r="387" spans="1:43" hidden="1">
       <c r="A387" s="2" t="s">
         <v>54</v>
       </c>
@@ -16152,7 +16155,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="388" spans="1:43">
+    <row r="388" spans="1:43" hidden="1">
       <c r="A388" s="2" t="s">
         <v>54</v>
       </c>
@@ -16189,7 +16192,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="389" spans="1:43">
+    <row r="389" spans="1:43" hidden="1">
       <c r="A389" t="s">
         <v>54</v>
       </c>
@@ -16231,7 +16234,7 @@
         <v>54</v>
       </c>
       <c r="B390" s="5">
-        <v>35844</v>
+        <v>35864</v>
       </c>
       <c r="C390" s="5"/>
       <c r="D390" s="6">
@@ -16275,7 +16278,7 @@
         <v>3.39E-2</v>
       </c>
     </row>
-    <row r="391" spans="1:43">
+    <row r="391" spans="1:43" hidden="1">
       <c r="A391" s="2" t="s">
         <v>54</v>
       </c>
@@ -16309,7 +16312,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="392" spans="1:43">
+    <row r="392" spans="1:43" hidden="1">
       <c r="A392" s="2" t="s">
         <v>54</v>
       </c>
@@ -16346,7 +16349,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="393" spans="1:43">
+    <row r="393" spans="1:43" hidden="1">
       <c r="A393" s="2" t="s">
         <v>54</v>
       </c>
@@ -16380,7 +16383,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="394" spans="1:43">
+    <row r="394" spans="1:43" hidden="1">
       <c r="A394" s="2" t="s">
         <v>54</v>
       </c>
@@ -16414,7 +16417,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="395" spans="1:43">
+    <row r="395" spans="1:43" hidden="1">
       <c r="A395" s="2" t="s">
         <v>54</v>
       </c>
@@ -16451,7 +16454,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="396" spans="1:43">
+    <row r="396" spans="1:43" hidden="1">
       <c r="A396" s="2" t="s">
         <v>54</v>
       </c>
@@ -16485,7 +16488,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="397" spans="1:43">
+    <row r="397" spans="1:43" hidden="1">
       <c r="A397" s="2" t="s">
         <v>54</v>
       </c>
@@ -16522,7 +16525,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="398" spans="1:43">
+    <row r="398" spans="1:43" hidden="1">
       <c r="A398" s="2" t="s">
         <v>54</v>
       </c>
@@ -16556,7 +16559,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="399" spans="1:43">
+    <row r="399" spans="1:43" hidden="1">
       <c r="A399" s="2" t="s">
         <v>54</v>
       </c>
@@ -16590,7 +16593,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="400" spans="1:43">
+    <row r="400" spans="1:43" hidden="1">
       <c r="A400" s="2" t="s">
         <v>54</v>
       </c>
@@ -16624,7 +16627,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="401" spans="1:49">
+    <row r="401" spans="1:49" hidden="1">
       <c r="A401" s="2" t="s">
         <v>54</v>
       </c>
@@ -16661,7 +16664,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="402" spans="1:49">
+    <row r="402" spans="1:49" hidden="1">
       <c r="A402" s="2" t="s">
         <v>54</v>
       </c>
@@ -16707,7 +16710,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="403" spans="1:49">
+    <row r="403" spans="1:49" hidden="1">
       <c r="A403" s="2" t="s">
         <v>54</v>
       </c>
@@ -16747,7 +16750,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="404" spans="1:49">
+    <row r="404" spans="1:49" hidden="1">
       <c r="A404" s="2" t="s">
         <v>54</v>
       </c>
@@ -16781,7 +16784,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="405" spans="1:49">
+    <row r="405" spans="1:49" hidden="1">
       <c r="A405" t="s">
         <v>54</v>
       </c>
@@ -16818,7 +16821,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="406" spans="1:49">
+    <row r="406" spans="1:49" hidden="1">
       <c r="A406" t="s">
         <v>54</v>
       </c>
@@ -16855,7 +16858,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="407" spans="1:49">
+    <row r="407" spans="1:49" hidden="1">
       <c r="A407" s="2" t="s">
         <v>54</v>
       </c>
@@ -16895,7 +16898,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="408" spans="1:49">
+    <row r="408" spans="1:49" hidden="1">
       <c r="A408" s="2" t="s">
         <v>54</v>
       </c>
@@ -16929,7 +16932,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="409" spans="1:49">
+    <row r="409" spans="1:49" hidden="1">
       <c r="A409" s="2" t="s">
         <v>49</v>
       </c>
@@ -16962,7 +16965,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="410" spans="1:49">
+    <row r="410" spans="1:49" hidden="1">
       <c r="A410" s="2" t="s">
         <v>49</v>
       </c>
@@ -16999,7 +17002,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="411" spans="1:49">
+    <row r="411" spans="1:49" hidden="1">
       <c r="A411" s="2" t="s">
         <v>49</v>
       </c>
@@ -17036,7 +17039,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="412" spans="1:49">
+    <row r="412" spans="1:49" hidden="1">
       <c r="A412" s="2" t="s">
         <v>49</v>
       </c>
@@ -17073,7 +17076,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="413" spans="1:49">
+    <row r="413" spans="1:49" hidden="1">
       <c r="A413" s="2" t="s">
         <v>49</v>
       </c>
@@ -17107,7 +17110,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="414" spans="1:49">
+    <row r="414" spans="1:49" hidden="1">
       <c r="A414" s="2" t="s">
         <v>49</v>
       </c>
@@ -17141,7 +17144,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="415" spans="1:49">
+    <row r="415" spans="1:49" hidden="1">
       <c r="A415" s="2" t="s">
         <v>49</v>
       </c>
@@ -17175,7 +17178,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="416" spans="1:49">
+    <row r="416" spans="1:49" hidden="1">
       <c r="A416" s="2" t="s">
         <v>49</v>
       </c>
@@ -17209,7 +17212,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="417" spans="1:51">
+    <row r="417" spans="1:51" hidden="1">
       <c r="A417" s="2" t="s">
         <v>49</v>
       </c>
@@ -17243,7 +17246,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="418" spans="1:51">
+    <row r="418" spans="1:51" hidden="1">
       <c r="A418" s="2" t="s">
         <v>49</v>
       </c>
@@ -17277,7 +17280,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="419" spans="1:51">
+    <row r="419" spans="1:51" hidden="1">
       <c r="A419" s="2" t="s">
         <v>49</v>
       </c>
@@ -17311,7 +17314,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="420" spans="1:51">
+    <row r="420" spans="1:51" hidden="1">
       <c r="A420" s="2" t="s">
         <v>49</v>
       </c>
@@ -17345,7 +17348,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="421" spans="1:51">
+    <row r="421" spans="1:51" hidden="1">
       <c r="A421" s="2" t="s">
         <v>49</v>
       </c>
@@ -17388,7 +17391,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="422" spans="1:51">
+    <row r="422" spans="1:51" hidden="1">
       <c r="A422" s="2" t="s">
         <v>49</v>
       </c>
@@ -17437,7 +17440,7 @@
         <v>2.1499999999999998E-2</v>
       </c>
     </row>
-    <row r="423" spans="1:51">
+    <row r="423" spans="1:51" hidden="1">
       <c r="A423" s="2" t="s">
         <v>49</v>
       </c>
@@ -17471,7 +17474,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="424" spans="1:51">
+    <row r="424" spans="1:51" hidden="1">
       <c r="A424" s="2" t="s">
         <v>49</v>
       </c>
@@ -17502,7 +17505,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="425" spans="1:51">
+    <row r="425" spans="1:51" hidden="1">
       <c r="A425" s="2" t="s">
         <v>49</v>
       </c>
@@ -17536,7 +17539,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="426" spans="1:51">
+    <row r="426" spans="1:51" hidden="1">
       <c r="A426" s="2" t="s">
         <v>49</v>
       </c>
@@ -17570,7 +17573,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="427" spans="1:51">
+    <row r="427" spans="1:51" hidden="1">
       <c r="A427" s="2" t="s">
         <v>49</v>
       </c>
@@ -17613,7 +17616,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="428" spans="1:51">
+    <row r="428" spans="1:51" hidden="1">
       <c r="A428" s="2" t="s">
         <v>49</v>
       </c>
@@ -17665,7 +17668,7 @@
         <v>4.62</v>
       </c>
     </row>
-    <row r="429" spans="1:51">
+    <row r="429" spans="1:51" hidden="1">
       <c r="A429" s="2" t="s">
         <v>49</v>
       </c>
@@ -17711,7 +17714,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="430" spans="1:51">
+    <row r="430" spans="1:51" hidden="1">
       <c r="A430" s="2" t="s">
         <v>49</v>
       </c>
@@ -17751,7 +17754,7 @@
         <v>15.4</v>
       </c>
     </row>
-    <row r="431" spans="1:51">
+    <row r="431" spans="1:51" hidden="1">
       <c r="A431" s="2" t="s">
         <v>49</v>
       </c>
@@ -17785,7 +17788,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="432" spans="1:51">
+    <row r="432" spans="1:51" hidden="1">
       <c r="A432" s="2" t="s">
         <v>49</v>
       </c>
@@ -17819,7 +17822,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="433" spans="1:51">
+    <row r="433" spans="1:51" hidden="1">
       <c r="A433" s="2" t="s">
         <v>49</v>
       </c>
@@ -17856,7 +17859,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="434" spans="1:51">
+    <row r="434" spans="1:51" hidden="1">
       <c r="A434" s="2" t="s">
         <v>49</v>
       </c>
@@ -17890,7 +17893,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="435" spans="1:51">
+    <row r="435" spans="1:51" hidden="1">
       <c r="A435" s="2" t="s">
         <v>49</v>
       </c>
@@ -17924,7 +17927,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="436" spans="1:51">
+    <row r="436" spans="1:51" hidden="1">
       <c r="A436" s="2" t="s">
         <v>49</v>
       </c>
@@ -17958,7 +17961,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="437" spans="1:51">
+    <row r="437" spans="1:51" hidden="1">
       <c r="A437" s="2" t="s">
         <v>49</v>
       </c>
@@ -18007,7 +18010,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="438" spans="1:51">
+    <row r="438" spans="1:51" hidden="1">
       <c r="A438" s="2" t="s">
         <v>49</v>
       </c>
@@ -18044,7 +18047,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="439" spans="1:51">
+    <row r="439" spans="1:51" hidden="1">
       <c r="A439" s="2" t="s">
         <v>49</v>
       </c>
@@ -18081,7 +18084,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="440" spans="1:51">
+    <row r="440" spans="1:51" hidden="1">
       <c r="A440" s="2" t="s">
         <v>49</v>
       </c>
@@ -18118,7 +18121,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="441" spans="1:51">
+    <row r="441" spans="1:51" hidden="1">
       <c r="A441" s="2" t="s">
         <v>49</v>
       </c>
@@ -18218,7 +18221,7 @@
         <v>8.9</v>
       </c>
     </row>
-    <row r="442" spans="1:51">
+    <row r="442" spans="1:51" hidden="1">
       <c r="A442" s="2" t="s">
         <v>49</v>
       </c>
@@ -18255,7 +18258,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="443" spans="1:51">
+    <row r="443" spans="1:51" hidden="1">
       <c r="A443" s="2" t="s">
         <v>52</v>
       </c>
@@ -18289,7 +18292,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="444" spans="1:51">
+    <row r="444" spans="1:51" hidden="1">
       <c r="A444" s="2" t="s">
         <v>52</v>
       </c>
@@ -18323,7 +18326,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="445" spans="1:51">
+    <row r="445" spans="1:51" hidden="1">
       <c r="A445" t="s">
         <v>52</v>
       </c>
@@ -18363,7 +18366,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="446" spans="1:51">
+    <row r="446" spans="1:51" hidden="1">
       <c r="A446" s="2" t="s">
         <v>52</v>
       </c>
@@ -18397,7 +18400,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="447" spans="1:51">
+    <row r="447" spans="1:51" hidden="1">
       <c r="A447" s="2" t="s">
         <v>52</v>
       </c>
@@ -18431,7 +18434,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="448" spans="1:51">
+    <row r="448" spans="1:51" hidden="1">
       <c r="A448" s="2" t="s">
         <v>52</v>
       </c>
@@ -18468,7 +18471,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="449" spans="1:49">
+    <row r="449" spans="1:49" hidden="1">
       <c r="A449" s="2" t="s">
         <v>52</v>
       </c>
@@ -18502,7 +18505,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="450" spans="1:49">
+    <row r="450" spans="1:49" hidden="1">
       <c r="A450" s="2" t="s">
         <v>52</v>
       </c>
@@ -18536,7 +18539,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="451" spans="1:49">
+    <row r="451" spans="1:49" hidden="1">
       <c r="A451" s="2" t="s">
         <v>52</v>
       </c>
@@ -18570,7 +18573,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="452" spans="1:49">
+    <row r="452" spans="1:49" hidden="1">
       <c r="A452" s="2" t="s">
         <v>52</v>
       </c>
@@ -18607,7 +18610,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="453" spans="1:49">
+    <row r="453" spans="1:49" hidden="1">
       <c r="A453" s="2" t="s">
         <v>52</v>
       </c>
@@ -18644,7 +18647,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="454" spans="1:49">
+    <row r="454" spans="1:49" hidden="1">
       <c r="A454" s="2" t="s">
         <v>52</v>
       </c>
@@ -18678,7 +18681,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="455" spans="1:49">
+    <row r="455" spans="1:49" hidden="1">
       <c r="A455" s="2" t="s">
         <v>52</v>
       </c>
@@ -18718,7 +18721,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="456" spans="1:49">
+    <row r="456" spans="1:49" hidden="1">
       <c r="A456" s="2" t="s">
         <v>52</v>
       </c>
@@ -18761,7 +18764,7 @@
         <v>2.2400000000000003E-2</v>
       </c>
     </row>
-    <row r="457" spans="1:49">
+    <row r="457" spans="1:49" hidden="1">
       <c r="A457" s="2" t="s">
         <v>52</v>
       </c>
@@ -18795,7 +18798,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="458" spans="1:49">
+    <row r="458" spans="1:49" hidden="1">
       <c r="A458" s="2" t="s">
         <v>52</v>
       </c>
@@ -18829,7 +18832,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="459" spans="1:49">
+    <row r="459" spans="1:49" hidden="1">
       <c r="A459" s="2" t="s">
         <v>52</v>
       </c>
@@ -18863,7 +18866,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="460" spans="1:49">
+    <row r="460" spans="1:49" hidden="1">
       <c r="A460" s="2" t="s">
         <v>52</v>
       </c>
@@ -18903,7 +18906,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="461" spans="1:49">
+    <row r="461" spans="1:49" hidden="1">
       <c r="A461" s="2" t="s">
         <v>52</v>
       </c>
@@ -18937,7 +18940,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="462" spans="1:49">
+    <row r="462" spans="1:49" hidden="1">
       <c r="A462" s="2" t="s">
         <v>52</v>
       </c>
@@ -18992,7 +18995,7 @@
         <v>4.92</v>
       </c>
     </row>
-    <row r="463" spans="1:49">
+    <row r="463" spans="1:49" hidden="1">
       <c r="A463" s="2" t="s">
         <v>52</v>
       </c>
@@ -19032,7 +19035,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="464" spans="1:49">
+    <row r="464" spans="1:49" hidden="1">
       <c r="A464" s="2" t="s">
         <v>52</v>
       </c>
@@ -19066,7 +19069,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="465" spans="1:50">
+    <row r="465" spans="1:50" hidden="1">
       <c r="A465" s="2" t="s">
         <v>52</v>
       </c>
@@ -19103,7 +19106,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="466" spans="1:50">
+    <row r="466" spans="1:50" hidden="1">
       <c r="A466" s="2" t="s">
         <v>52</v>
       </c>
@@ -19140,7 +19143,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="467" spans="1:50">
+    <row r="467" spans="1:50" hidden="1">
       <c r="A467" s="2" t="s">
         <v>52</v>
       </c>
@@ -19177,7 +19180,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="468" spans="1:50">
+    <row r="468" spans="1:50" hidden="1">
       <c r="A468" s="2" t="s">
         <v>52</v>
       </c>
@@ -19226,7 +19229,7 @@
         <v>1.98</v>
       </c>
     </row>
-    <row r="469" spans="1:50">
+    <row r="469" spans="1:50" hidden="1">
       <c r="A469" s="2" t="s">
         <v>55</v>
       </c>
@@ -19328,7 +19331,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="472" spans="1:50">
+    <row r="472" spans="1:50" hidden="1">
       <c r="A472" s="2" t="s">
         <v>55</v>
       </c>
@@ -19362,7 +19365,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="473" spans="1:50">
+    <row r="473" spans="1:50" hidden="1">
       <c r="A473" t="s">
         <v>55</v>
       </c>
@@ -19420,7 +19423,7 @@
         <v>7.05</v>
       </c>
     </row>
-    <row r="474" spans="1:50">
+    <row r="474" spans="1:50" hidden="1">
       <c r="A474" s="2" t="s">
         <v>55</v>
       </c>
@@ -19454,7 +19457,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="475" spans="1:50">
+    <row r="475" spans="1:50" hidden="1">
       <c r="A475" s="2" t="s">
         <v>55</v>
       </c>
@@ -19488,7 +19491,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="476" spans="1:50">
+    <row r="476" spans="1:50" hidden="1">
       <c r="A476" s="2" t="s">
         <v>55</v>
       </c>
@@ -19559,7 +19562,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="478" spans="1:50">
+    <row r="478" spans="1:50" hidden="1">
       <c r="A478" s="2" t="s">
         <v>55</v>
       </c>
@@ -19593,7 +19596,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="479" spans="1:50">
+    <row r="479" spans="1:50" hidden="1">
       <c r="A479" s="2" t="s">
         <v>55</v>
       </c>
@@ -19627,7 +19630,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="480" spans="1:50">
+    <row r="480" spans="1:50" hidden="1">
       <c r="A480" s="2" t="s">
         <v>55</v>
       </c>
@@ -19664,7 +19667,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="481" spans="1:50">
+    <row r="481" spans="1:50" hidden="1">
       <c r="A481" s="2" t="s">
         <v>55</v>
       </c>
@@ -19698,7 +19701,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="482" spans="1:50">
+    <row r="482" spans="1:50" hidden="1">
       <c r="A482" s="2" t="s">
         <v>55</v>
       </c>
@@ -19735,7 +19738,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="483" spans="1:50">
+    <row r="483" spans="1:50" hidden="1">
       <c r="A483" t="s">
         <v>55</v>
       </c>
@@ -19778,7 +19781,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="484" spans="1:50">
+    <row r="484" spans="1:50" hidden="1">
       <c r="A484" s="2" t="s">
         <v>55</v>
       </c>
@@ -19827,7 +19830,7 @@
         <v>2.3799999999999998E-2</v>
       </c>
     </row>
-    <row r="485" spans="1:50">
+    <row r="485" spans="1:50" hidden="1">
       <c r="A485" s="2" t="s">
         <v>55</v>
       </c>
@@ -19861,7 +19864,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="486" spans="1:50">
+    <row r="486" spans="1:50" hidden="1">
       <c r="A486" s="2" t="s">
         <v>55</v>
       </c>
@@ -19895,7 +19898,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="487" spans="1:50">
+    <row r="487" spans="1:50" hidden="1">
       <c r="A487" s="2" t="s">
         <v>55</v>
       </c>
@@ -19929,7 +19932,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="488" spans="1:50">
+    <row r="488" spans="1:50" hidden="1">
       <c r="A488" s="2" t="s">
         <v>55</v>
       </c>
@@ -19969,7 +19972,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="489" spans="1:50">
+    <row r="489" spans="1:50" hidden="1">
       <c r="A489" t="s">
         <v>55</v>
       </c>
@@ -20003,7 +20006,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="490" spans="1:50">
+    <row r="490" spans="1:50" hidden="1">
       <c r="A490" s="2" t="s">
         <v>55</v>
       </c>
@@ -20040,7 +20043,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="491" spans="1:50">
+    <row r="491" spans="1:50" hidden="1">
       <c r="A491" s="2" t="s">
         <v>55</v>
       </c>
@@ -20077,7 +20080,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="492" spans="1:50">
+    <row r="492" spans="1:50" hidden="1">
       <c r="A492" s="2" t="s">
         <v>55</v>
       </c>
@@ -20111,7 +20114,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="493" spans="1:50">
+    <row r="493" spans="1:50" hidden="1">
       <c r="A493" s="2" t="s">
         <v>55</v>
       </c>
@@ -20151,7 +20154,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="494" spans="1:50">
+    <row r="494" spans="1:50" hidden="1">
       <c r="A494" s="2" t="s">
         <v>55</v>
       </c>
@@ -20185,7 +20188,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="495" spans="1:50">
+    <row r="495" spans="1:50" hidden="1">
       <c r="A495" s="2" t="s">
         <v>55</v>
       </c>
@@ -20228,7 +20231,7 @@
         <v>2.78</v>
       </c>
     </row>
-    <row r="496" spans="1:50">
+    <row r="496" spans="1:50" hidden="1">
       <c r="A496" s="2" t="s">
         <v>55</v>
       </c>
@@ -20265,7 +20268,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="497" spans="1:37">
+    <row r="497" spans="1:37" hidden="1">
       <c r="A497" t="s">
         <v>55</v>
       </c>
@@ -20299,7 +20302,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="498" spans="1:37">
+    <row r="498" spans="1:37" hidden="1">
       <c r="A498" t="s">
         <v>55</v>
       </c>
@@ -20333,7 +20336,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="499" spans="1:37">
+    <row r="499" spans="1:37" hidden="1">
       <c r="A499" t="s">
         <v>55</v>
       </c>
@@ -20367,7 +20370,102 @@
         <v>1810</v>
       </c>
     </row>
+    <row r="505" spans="1:37">
+      <c r="H505" s="5"/>
+    </row>
+    <row r="506" spans="1:37">
+      <c r="H506" s="5"/>
+    </row>
+    <row r="507" spans="1:37">
+      <c r="H507" s="5"/>
+    </row>
+    <row r="508" spans="1:37">
+      <c r="H508" s="5"/>
+    </row>
+    <row r="509" spans="1:37">
+      <c r="H509" s="5"/>
+    </row>
+    <row r="510" spans="1:37">
+      <c r="H510" s="5"/>
+    </row>
+    <row r="511" spans="1:37">
+      <c r="H511" s="5"/>
+    </row>
+    <row r="512" spans="1:37">
+      <c r="H512" s="5"/>
+    </row>
+    <row r="513" spans="8:8">
+      <c r="H513" s="5"/>
+    </row>
+    <row r="514" spans="8:8">
+      <c r="H514" s="5"/>
+    </row>
+    <row r="515" spans="8:8">
+      <c r="H515" s="5"/>
+    </row>
+    <row r="516" spans="8:8">
+      <c r="H516" s="5"/>
+    </row>
+    <row r="517" spans="8:8">
+      <c r="H517" s="5"/>
+    </row>
+    <row r="518" spans="8:8">
+      <c r="H518" s="5"/>
+    </row>
+    <row r="519" spans="8:8">
+      <c r="H519" s="5"/>
+    </row>
+    <row r="520" spans="8:8">
+      <c r="H520" s="5"/>
+    </row>
+    <row r="521" spans="8:8">
+      <c r="H521" s="5"/>
+    </row>
+    <row r="522" spans="8:8">
+      <c r="H522" s="5"/>
+    </row>
+    <row r="523" spans="8:8">
+      <c r="H523" s="5"/>
+    </row>
+    <row r="524" spans="8:8">
+      <c r="H524" s="5"/>
+    </row>
+    <row r="525" spans="8:8">
+      <c r="H525" s="5"/>
+    </row>
+    <row r="526" spans="8:8">
+      <c r="H526" s="5"/>
+    </row>
+    <row r="527" spans="8:8">
+      <c r="H527" s="5"/>
+    </row>
+    <row r="528" spans="8:8">
+      <c r="H528" s="5"/>
+    </row>
+    <row r="529" spans="8:8">
+      <c r="H529" s="5"/>
+    </row>
+    <row r="530" spans="8:8">
+      <c r="H530" s="5"/>
+    </row>
+    <row r="531" spans="8:8">
+      <c r="H531" s="5"/>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:AY499" xr:uid="{82957E3C-ACA6-4A6F-B162-5B06AF55FA73}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="exp3SowDec17ROCultivarEmerald"/>
+        <filter val="exp3SowDec30ROCultivarEmerald"/>
+        <filter val="exp3SowDec3ROCultivarEmerald"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="25">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AY499">
     <sortCondition ref="S2:S499"/>
   </sortState>

</xml_diff>

<commit_message>
Some trouble still with Exp 3 TOS differences. Berken calibrated. Waiting for APSIM update with fixed bugs before moving onto TOS experiments.
</commit_message>
<xml_diff>
--- a/Prototypes/Mungbean/Exp3observed.xlsx
+++ b/Prototypes/Mungbean/Exp3observed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pas075\Documents\ApsimX\Prototypes\Mungbean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF9CC480-A1A3-4B12-B537-AAD0347F27A6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1D320BC-CE04-46A5-87FF-5F650007DEA8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8C69385E-AA3F-4CF3-AF00-E1E4599E61EE}"/>
   </bookViews>
@@ -606,7 +606,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C506" sqref="C506"/>
+      <selection pane="bottomLeft" activeCell="B390" sqref="B390"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -614,7 +614,7 @@
     <col min="1" max="1" width="35.7109375" customWidth="1"/>
     <col min="2" max="3" width="19.140625" customWidth="1"/>
     <col min="4" max="5" width="9.42578125" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:51">
@@ -895,34 +895,28 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="5" spans="1:51" hidden="1">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:51">
+      <c r="A5" t="s">
         <v>53</v>
       </c>
       <c r="B5" s="5">
-        <v>35877</v>
+        <v>35816</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="6">
-        <v>109.644263924509</v>
+        <v>48.541169010282097</v>
       </c>
       <c r="E5">
-        <v>1913.03431224823</v>
+        <v>844.70688438415527</v>
+      </c>
+      <c r="Q5">
+        <v>520.38038984621903</v>
       </c>
       <c r="R5">
-        <v>0</v>
+        <v>2.6772934287572898</v>
       </c>
       <c r="S5" s="6">
-        <v>0</v>
-      </c>
-      <c r="T5">
-        <v>298</v>
-      </c>
-      <c r="X5">
-        <v>0.5</v>
-      </c>
-      <c r="Y5">
-        <v>0.32</v>
+        <v>6.5097282791009299</v>
       </c>
       <c r="AF5">
         <v>41</v>
@@ -941,15 +935,6 @@
       </c>
       <c r="AK5">
         <v>1762</v>
-      </c>
-      <c r="AV5">
-        <v>0.63</v>
-      </c>
-      <c r="AW5">
-        <v>0.21</v>
-      </c>
-      <c r="AX5">
-        <v>2.59</v>
       </c>
     </row>
     <row r="6" spans="1:51" hidden="1">
@@ -997,31 +982,23 @@
         <v>1873</v>
       </c>
     </row>
-    <row r="7" spans="1:51" hidden="1">
+    <row r="7" spans="1:51">
       <c r="A7" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B7" s="5">
-        <v>35885</v>
+        <v>35844</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="6">
-        <v>117.682945154019</v>
-      </c>
-      <c r="E7">
-        <v>2050.6658182144165</v>
-      </c>
+        <v>76.852222463001397</v>
+      </c>
+      <c r="E7" s="6"/>
       <c r="R7">
-        <v>0</v>
-      </c>
-      <c r="S7" s="6">
-        <v>0</v>
+        <v>1.7011661078023801</v>
       </c>
       <c r="T7">
-        <v>306</v>
-      </c>
-      <c r="AB7">
-        <v>0</v>
+        <v>320.98560848448199</v>
       </c>
       <c r="AF7">
         <v>41</v>
@@ -1030,25 +1007,22 @@
         <v>45</v>
       </c>
       <c r="AH7">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="AI7">
-        <v>768</v>
+        <v>764</v>
       </c>
       <c r="AJ7">
-        <v>841</v>
+        <v>844</v>
       </c>
       <c r="AK7">
-        <v>1651</v>
-      </c>
-      <c r="AV7">
-        <v>0.54</v>
-      </c>
-      <c r="AW7">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="AX7">
-        <v>2.78</v>
+        <v>1762</v>
+      </c>
+      <c r="AP7">
+        <v>8.199999999999999E-3</v>
+      </c>
+      <c r="AQ7">
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="8" spans="1:51" hidden="1">
@@ -6721,28 +6695,23 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="153" spans="1:51" hidden="1">
-      <c r="A153" t="s">
+    <row r="153" spans="1:51">
+      <c r="A153" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B153" s="5">
-        <v>35816</v>
+        <v>35858</v>
       </c>
       <c r="C153" s="5"/>
       <c r="D153" s="6">
-        <v>48.541169010282097</v>
-      </c>
-      <c r="E153">
-        <v>844.70688438415527</v>
-      </c>
-      <c r="Q153">
-        <v>520.38038984621903</v>
-      </c>
+        <v>91.193633952254601</v>
+      </c>
+      <c r="E153" s="6"/>
       <c r="R153">
-        <v>2.6772934287572898</v>
-      </c>
-      <c r="S153" s="6">
-        <v>6.5097282791009299</v>
+        <v>1.4764526299984699</v>
+      </c>
+      <c r="AC153">
+        <v>5.4807733232930502</v>
       </c>
       <c r="AF153">
         <v>41</v>
@@ -7540,7 +7509,7 @@
         <v>1873</v>
       </c>
     </row>
-    <row r="174" spans="1:51">
+    <row r="174" spans="1:51" hidden="1">
       <c r="A174" s="2" t="s">
         <v>55</v>
       </c>
@@ -8402,113 +8371,47 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="192" spans="1:51" hidden="1">
+    <row r="192" spans="1:51">
       <c r="A192" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B192" s="5">
-        <v>35866</v>
-      </c>
-      <c r="C192" s="5" t="s">
-        <v>45</v>
-      </c>
+        <v>35872</v>
+      </c>
+      <c r="C192" s="5"/>
       <c r="D192" s="6">
-        <v>98.832891246684298</v>
+        <v>104.507135582198</v>
       </c>
       <c r="E192" s="6"/>
-      <c r="F192">
-        <v>123</v>
-      </c>
-      <c r="G192">
-        <f>F192*10</f>
-        <v>1230</v>
-      </c>
-      <c r="H192">
-        <v>0.32355522509913598</v>
-      </c>
-      <c r="J192">
-        <v>0.39381852111033294</v>
-      </c>
-      <c r="K192">
-        <v>0.35788138558432403</v>
-      </c>
-      <c r="L192">
-        <v>0.321987986937252</v>
-      </c>
-      <c r="M192">
-        <v>0.33179233729880997</v>
-      </c>
-      <c r="N192">
-        <v>0.31222737345462998</v>
-      </c>
-      <c r="O192">
-        <v>0.29173664567296398</v>
-      </c>
-      <c r="P192">
-        <v>0.31133805691625799</v>
-      </c>
       <c r="R192">
         <v>0</v>
       </c>
-      <c r="U192">
-        <v>117</v>
-      </c>
-      <c r="V192">
-        <v>12</v>
-      </c>
       <c r="W192">
-        <v>173</v>
-      </c>
-      <c r="AD192">
-        <v>7</v>
-      </c>
-      <c r="AE192">
-        <v>35.6</v>
+        <v>169.23076923076499</v>
+      </c>
+      <c r="X192">
+        <v>0.51519639723657196</v>
+      </c>
+      <c r="Y192">
+        <v>0.35796080644963302</v>
       </c>
       <c r="AF192">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="AG192">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="AH192">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="AI192">
-        <v>787</v>
+        <v>764</v>
       </c>
       <c r="AJ192">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="AK192">
-        <v>1810</v>
-      </c>
-      <c r="AL192">
-        <v>94</v>
-      </c>
-      <c r="AM192">
-        <v>177</v>
-      </c>
-      <c r="AN192">
-        <v>83</v>
-      </c>
-      <c r="AO192">
-        <v>479</v>
-      </c>
-      <c r="AR192">
-        <v>9.6</v>
-      </c>
-      <c r="AS192">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="AT192">
-        <v>0.72</v>
-      </c>
-      <c r="AU192">
-        <v>0.53</v>
-      </c>
-      <c r="AY192">
-        <v>3.1</v>
+        <v>1762</v>
       </c>
     </row>
     <row r="193" spans="1:51" hidden="1">
@@ -8793,77 +8696,34 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="197" spans="1:51" hidden="1">
+    <row r="197" spans="1:51">
       <c r="A197" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B197" s="5">
-        <v>35858</v>
-      </c>
-      <c r="C197" s="5" t="s">
-        <v>45</v>
-      </c>
+        <v>35877</v>
+      </c>
+      <c r="C197" s="5"/>
       <c r="D197" s="6">
-        <v>90.557029177718803</v>
-      </c>
-      <c r="E197" s="6"/>
-      <c r="F197">
-        <v>169</v>
-      </c>
-      <c r="G197">
-        <f>F197*10</f>
-        <v>1690</v>
-      </c>
-      <c r="H197">
-        <v>0.344806101875195</v>
-      </c>
-      <c r="J197">
-        <v>0.39941431692186496</v>
-      </c>
-      <c r="K197">
-        <v>0.36803146531847297</v>
-      </c>
-      <c r="L197">
-        <v>0.32230274429547995</v>
-      </c>
-      <c r="M197">
-        <v>0.328343021788083</v>
-      </c>
-      <c r="N197">
-        <v>0.30730050590900304</v>
-      </c>
-      <c r="O197">
-        <v>0.30456731821104099</v>
-      </c>
-      <c r="P197">
-        <v>0.32016870365446004</v>
+        <v>109.644263924509</v>
+      </c>
+      <c r="E197">
+        <v>1913.03431224823</v>
       </c>
       <c r="R197">
-        <v>2.8742805665381801</v>
-      </c>
-      <c r="U197">
-        <v>56</v>
-      </c>
-      <c r="V197">
-        <v>3</v>
-      </c>
-      <c r="W197">
-        <v>126</v>
+        <v>0</v>
+      </c>
+      <c r="S197" s="6">
+        <v>0</v>
+      </c>
+      <c r="T197">
+        <v>298</v>
       </c>
       <c r="X197">
-        <v>0.30292432965705401</v>
+        <v>0.5</v>
       </c>
       <c r="Y197">
-        <v>0.29910768188711301</v>
-      </c>
-      <c r="AB197">
-        <v>8.1288504883545105</v>
-      </c>
-      <c r="AD197">
-        <v>8.1</v>
-      </c>
-      <c r="AE197">
-        <v>24.1</v>
+        <v>0.32</v>
       </c>
       <c r="AF197">
         <v>41</v>
@@ -8872,40 +8732,25 @@
         <v>45</v>
       </c>
       <c r="AH197">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="AI197">
-        <v>768</v>
+        <v>764</v>
       </c>
       <c r="AJ197">
-        <v>841</v>
+        <v>844</v>
       </c>
       <c r="AK197">
-        <v>1651</v>
-      </c>
-      <c r="AL197">
-        <v>107</v>
-      </c>
-      <c r="AM197">
-        <v>244</v>
-      </c>
-      <c r="AN197">
-        <v>137</v>
-      </c>
-      <c r="AO197">
-        <v>437</v>
-      </c>
-      <c r="AR197">
-        <v>10.9</v>
-      </c>
-      <c r="AS197">
-        <v>6.4</v>
-      </c>
-      <c r="AT197">
-        <v>0.78</v>
-      </c>
-      <c r="AU197">
-        <v>0.59</v>
+        <v>1762</v>
+      </c>
+      <c r="AV197">
+        <v>0.63</v>
+      </c>
+      <c r="AW197">
+        <v>0.21</v>
+      </c>
+      <c r="AX197">
+        <v>2.59</v>
       </c>
     </row>
     <row r="198" spans="1:51" hidden="1">
@@ -11911,7 +11756,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="274" spans="1:51">
+    <row r="274" spans="1:51" hidden="1">
       <c r="A274" s="2" t="s">
         <v>53</v>
       </c>
@@ -11945,7 +11790,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="275" spans="1:51">
+    <row r="275" spans="1:51" hidden="1">
       <c r="A275" s="2" t="s">
         <v>53</v>
       </c>
@@ -12017,7 +11862,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="277" spans="1:51">
+    <row r="277" spans="1:51" hidden="1">
       <c r="A277" s="2" t="s">
         <v>53</v>
       </c>
@@ -12128,7 +11973,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="280" spans="1:51">
+    <row r="280" spans="1:51" hidden="1">
       <c r="A280" s="2" t="s">
         <v>53</v>
       </c>
@@ -12233,7 +12078,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="283" spans="1:51">
+    <row r="283" spans="1:51" hidden="1">
       <c r="A283" s="2" t="s">
         <v>53</v>
       </c>
@@ -12384,23 +12229,26 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="287" spans="1:51" hidden="1">
+    <row r="287" spans="1:51">
       <c r="A287" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B287" s="5">
-        <v>35844</v>
+        <v>35816</v>
       </c>
       <c r="C287" s="5"/>
       <c r="D287" s="6">
-        <v>76.852222463001397</v>
+        <v>48.8549248556387</v>
       </c>
       <c r="E287" s="6"/>
+      <c r="Q287">
+        <v>517.25503532317805</v>
+      </c>
       <c r="R287">
-        <v>1.7011661078023801</v>
+        <v>0.299934938191245</v>
       </c>
       <c r="T287">
-        <v>320.98560848448199</v>
+        <v>14.3813177988122</v>
       </c>
       <c r="AF287">
         <v>41</v>
@@ -12409,22 +12257,16 @@
         <v>45</v>
       </c>
       <c r="AH287">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="AI287">
-        <v>764</v>
+        <v>768</v>
       </c>
       <c r="AJ287">
-        <v>844</v>
+        <v>841</v>
       </c>
       <c r="AK287">
-        <v>1762</v>
-      </c>
-      <c r="AP287">
-        <v>8.199999999999999E-3</v>
-      </c>
-      <c r="AQ287">
-        <v>2.3E-2</v>
+        <v>1651</v>
       </c>
     </row>
     <row r="288" spans="1:51" hidden="1">
@@ -12723,23 +12565,29 @@
         <v>4.1100000000000003</v>
       </c>
     </row>
-    <row r="296" spans="1:51" hidden="1">
+    <row r="296" spans="1:51">
       <c r="A296" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B296" s="5">
-        <v>35858</v>
+        <v>35844</v>
       </c>
       <c r="C296" s="5"/>
       <c r="D296" s="6">
-        <v>91.193633952254601</v>
+        <v>76.689083371717999</v>
       </c>
       <c r="E296" s="6"/>
       <c r="R296">
-        <v>1.4764526299984699</v>
-      </c>
-      <c r="AC296">
-        <v>5.4807733232930502</v>
+        <v>1.9267804414193199</v>
+      </c>
+      <c r="X296">
+        <v>6.5844536392138497E-2</v>
+      </c>
+      <c r="Y296">
+        <v>6.39362125071683E-2</v>
+      </c>
+      <c r="Z296">
+        <v>63.522800552740101</v>
       </c>
       <c r="AF296">
         <v>41</v>
@@ -12748,16 +12596,22 @@
         <v>45</v>
       </c>
       <c r="AH296">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="AI296">
-        <v>764</v>
+        <v>768</v>
       </c>
       <c r="AJ296">
-        <v>844</v>
+        <v>841</v>
       </c>
       <c r="AK296">
-        <v>1762</v>
+        <v>1651</v>
+      </c>
+      <c r="AP296">
+        <v>1.1599999999999999E-2</v>
+      </c>
+      <c r="AQ296">
+        <v>3.39E-2</v>
       </c>
     </row>
     <row r="297" spans="1:51" hidden="1">
@@ -12988,29 +12842,77 @@
         <v>5.9</v>
       </c>
     </row>
-    <row r="303" spans="1:51" hidden="1">
+    <row r="303" spans="1:51">
       <c r="A303" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B303" s="5">
-        <v>35872</v>
-      </c>
-      <c r="C303" s="5"/>
+        <v>35858</v>
+      </c>
+      <c r="C303" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="D303" s="6">
-        <v>104.507135582198</v>
+        <v>90.557029177718803</v>
       </c>
       <c r="E303" s="6"/>
+      <c r="F303">
+        <v>169</v>
+      </c>
+      <c r="G303">
+        <f>F303*10</f>
+        <v>1690</v>
+      </c>
+      <c r="H303">
+        <v>0.344806101875195</v>
+      </c>
+      <c r="J303">
+        <v>0.39941431692186496</v>
+      </c>
+      <c r="K303">
+        <v>0.36803146531847297</v>
+      </c>
+      <c r="L303">
+        <v>0.32230274429547995</v>
+      </c>
+      <c r="M303">
+        <v>0.328343021788083</v>
+      </c>
+      <c r="N303">
+        <v>0.30730050590900304</v>
+      </c>
+      <c r="O303">
+        <v>0.30456731821104099</v>
+      </c>
+      <c r="P303">
+        <v>0.32016870365446004</v>
+      </c>
       <c r="R303">
-        <v>0</v>
+        <v>2.8742805665381801</v>
+      </c>
+      <c r="U303">
+        <v>56</v>
+      </c>
+      <c r="V303">
+        <v>3</v>
       </c>
       <c r="W303">
-        <v>169.23076923076499</v>
+        <v>126</v>
       </c>
       <c r="X303">
-        <v>0.51519639723657196</v>
+        <v>0.30292432965705401</v>
       </c>
       <c r="Y303">
-        <v>0.35796080644963302</v>
+        <v>0.29910768188711301</v>
+      </c>
+      <c r="AB303">
+        <v>8.1288504883545105</v>
+      </c>
+      <c r="AD303">
+        <v>8.1</v>
+      </c>
+      <c r="AE303">
+        <v>24.1</v>
       </c>
       <c r="AF303">
         <v>41</v>
@@ -13019,16 +12921,40 @@
         <v>45</v>
       </c>
       <c r="AH303">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="AI303">
-        <v>764</v>
+        <v>768</v>
       </c>
       <c r="AJ303">
-        <v>844</v>
+        <v>841</v>
       </c>
       <c r="AK303">
-        <v>1762</v>
+        <v>1651</v>
+      </c>
+      <c r="AL303">
+        <v>107</v>
+      </c>
+      <c r="AM303">
+        <v>244</v>
+      </c>
+      <c r="AN303">
+        <v>137</v>
+      </c>
+      <c r="AO303">
+        <v>437</v>
+      </c>
+      <c r="AR303">
+        <v>10.9</v>
+      </c>
+      <c r="AS303">
+        <v>6.4</v>
+      </c>
+      <c r="AT303">
+        <v>0.78</v>
+      </c>
+      <c r="AU303">
+        <v>0.59</v>
       </c>
     </row>
     <row r="304" spans="1:51" hidden="1">
@@ -15905,7 +15831,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="381" spans="1:51">
+    <row r="381" spans="1:51" hidden="1">
       <c r="A381" s="2" t="s">
         <v>54</v>
       </c>
@@ -15976,7 +15902,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="383" spans="1:51">
+    <row r="383" spans="1:51" hidden="1">
       <c r="A383" s="2" t="s">
         <v>54</v>
       </c>
@@ -16010,26 +15936,26 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="384" spans="1:51" hidden="1">
+    <row r="384" spans="1:51">
       <c r="A384" s="2" t="s">
         <v>54</v>
       </c>
       <c r="B384" s="5">
-        <v>35816</v>
+        <v>35872</v>
       </c>
       <c r="C384" s="5"/>
       <c r="D384" s="6">
-        <v>48.8549248556387</v>
+        <v>104.56233421750601</v>
       </c>
       <c r="E384" s="6"/>
-      <c r="Q384">
-        <v>517.25503532317805</v>
-      </c>
       <c r="R384">
-        <v>0.299934938191245</v>
-      </c>
-      <c r="T384">
-        <v>14.3813177988122</v>
+        <v>3.2918772834192298</v>
+      </c>
+      <c r="X384">
+        <v>0.40827087597366601</v>
+      </c>
+      <c r="Y384">
+        <v>0.310828560069494</v>
       </c>
       <c r="AF384">
         <v>41</v>
@@ -16050,7 +15976,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="385" spans="1:43">
+    <row r="385" spans="1:50" hidden="1">
       <c r="A385" s="2" t="s">
         <v>54</v>
       </c>
@@ -16087,7 +16013,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="386" spans="1:43">
+    <row r="386" spans="1:50" hidden="1">
       <c r="A386" s="2" t="s">
         <v>54</v>
       </c>
@@ -16121,7 +16047,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="387" spans="1:43" hidden="1">
+    <row r="387" spans="1:50" hidden="1">
       <c r="A387" s="2" t="s">
         <v>54</v>
       </c>
@@ -16155,7 +16081,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="388" spans="1:43" hidden="1">
+    <row r="388" spans="1:50" hidden="1">
       <c r="A388" s="2" t="s">
         <v>54</v>
       </c>
@@ -16192,7 +16118,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="389" spans="1:43" hidden="1">
+    <row r="389" spans="1:50" hidden="1">
       <c r="A389" t="s">
         <v>54</v>
       </c>
@@ -16229,29 +16155,31 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="390" spans="1:43">
+    <row r="390" spans="1:50">
       <c r="A390" s="2" t="s">
         <v>54</v>
       </c>
       <c r="B390" s="5">
-        <v>35864</v>
+        <v>35911</v>
       </c>
       <c r="C390" s="5"/>
       <c r="D390" s="6">
-        <v>76.689083371717999</v>
-      </c>
-      <c r="E390" s="6"/>
+        <v>117.682945154019</v>
+      </c>
+      <c r="E390">
+        <v>2050.6658182144165</v>
+      </c>
       <c r="R390">
-        <v>1.9267804414193199</v>
-      </c>
-      <c r="X390">
-        <v>6.5844536392138497E-2</v>
-      </c>
-      <c r="Y390">
-        <v>6.39362125071683E-2</v>
-      </c>
-      <c r="Z390">
-        <v>63.522800552740101</v>
+        <v>0</v>
+      </c>
+      <c r="S390" s="6">
+        <v>0</v>
+      </c>
+      <c r="T390">
+        <v>306</v>
+      </c>
+      <c r="AB390">
+        <v>0</v>
       </c>
       <c r="AF390">
         <v>41</v>
@@ -16271,14 +16199,17 @@
       <c r="AK390">
         <v>1651</v>
       </c>
-      <c r="AP390">
-        <v>1.1599999999999999E-2</v>
-      </c>
-      <c r="AQ390">
-        <v>3.39E-2</v>
-      </c>
-    </row>
-    <row r="391" spans="1:43" hidden="1">
+      <c r="AV390">
+        <v>0.54</v>
+      </c>
+      <c r="AW390">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AX390">
+        <v>2.78</v>
+      </c>
+    </row>
+    <row r="391" spans="1:50" hidden="1">
       <c r="A391" s="2" t="s">
         <v>54</v>
       </c>
@@ -16312,7 +16243,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="392" spans="1:43" hidden="1">
+    <row r="392" spans="1:50" hidden="1">
       <c r="A392" s="2" t="s">
         <v>54</v>
       </c>
@@ -16349,7 +16280,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="393" spans="1:43" hidden="1">
+    <row r="393" spans="1:50" hidden="1">
       <c r="A393" s="2" t="s">
         <v>54</v>
       </c>
@@ -16383,7 +16314,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="394" spans="1:43" hidden="1">
+    <row r="394" spans="1:50" hidden="1">
       <c r="A394" s="2" t="s">
         <v>54</v>
       </c>
@@ -16417,7 +16348,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="395" spans="1:43" hidden="1">
+    <row r="395" spans="1:50" hidden="1">
       <c r="A395" s="2" t="s">
         <v>54</v>
       </c>
@@ -16454,7 +16385,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="396" spans="1:43" hidden="1">
+    <row r="396" spans="1:50" hidden="1">
       <c r="A396" s="2" t="s">
         <v>54</v>
       </c>
@@ -16488,7 +16419,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="397" spans="1:43" hidden="1">
+    <row r="397" spans="1:50" hidden="1">
       <c r="A397" s="2" t="s">
         <v>54</v>
       </c>
@@ -16525,7 +16456,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="398" spans="1:43" hidden="1">
+    <row r="398" spans="1:50" hidden="1">
       <c r="A398" s="2" t="s">
         <v>54</v>
       </c>
@@ -16559,7 +16490,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="399" spans="1:43" hidden="1">
+    <row r="399" spans="1:50" hidden="1">
       <c r="A399" s="2" t="s">
         <v>54</v>
       </c>
@@ -16593,7 +16524,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="400" spans="1:43" hidden="1">
+    <row r="400" spans="1:50" hidden="1">
       <c r="A400" s="2" t="s">
         <v>54</v>
       </c>
@@ -16710,44 +16641,62 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="403" spans="1:49" hidden="1">
-      <c r="A403" s="2" t="s">
-        <v>54</v>
+    <row r="403" spans="1:49">
+      <c r="A403" t="s">
+        <v>55</v>
       </c>
       <c r="B403" s="5">
-        <v>35872</v>
+        <v>35816</v>
       </c>
       <c r="C403" s="5"/>
       <c r="D403" s="6">
-        <v>104.56233421750601</v>
+        <v>48.6407417658667</v>
       </c>
       <c r="E403" s="6"/>
+      <c r="Q403">
+        <v>1033.6383885847799</v>
+      </c>
       <c r="R403">
-        <v>3.2918772834192298</v>
+        <v>3.88403983784593</v>
+      </c>
+      <c r="T403">
+        <v>323.18831342654801</v>
+      </c>
+      <c r="U403">
+        <v>142</v>
+      </c>
+      <c r="V403">
+        <v>185</v>
       </c>
       <c r="X403">
-        <v>0.40827087597366601</v>
+        <v>1.5951271639239099E-2</v>
       </c>
       <c r="Y403">
-        <v>0.310828560069494</v>
+        <v>1.39747809360974E-2</v>
       </c>
       <c r="AF403">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="AG403">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="AH403">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="AI403">
-        <v>768</v>
+        <v>787</v>
       </c>
       <c r="AJ403">
-        <v>841</v>
+        <v>846</v>
       </c>
       <c r="AK403">
-        <v>1651</v>
+        <v>1810</v>
+      </c>
+      <c r="AV403">
+        <v>1.65</v>
+      </c>
+      <c r="AW403">
+        <v>7.05</v>
       </c>
     </row>
     <row r="404" spans="1:49" hidden="1">
@@ -19263,7 +19212,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="470" spans="1:50">
+    <row r="470" spans="1:50" hidden="1">
       <c r="A470" s="2" t="s">
         <v>55</v>
       </c>
@@ -19297,7 +19246,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="471" spans="1:50">
+    <row r="471" spans="1:50" hidden="1">
       <c r="A471" s="2" t="s">
         <v>55</v>
       </c>
@@ -19365,38 +19314,29 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="473" spans="1:50" hidden="1">
-      <c r="A473" t="s">
+    <row r="473" spans="1:50">
+      <c r="A473" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B473" s="5">
-        <v>35816</v>
+        <v>35844</v>
       </c>
       <c r="C473" s="5"/>
       <c r="D473" s="6">
-        <v>48.6407417658667</v>
+        <v>76.612066438067998</v>
       </c>
       <c r="E473" s="6"/>
-      <c r="Q473">
-        <v>1033.6383885847799</v>
-      </c>
       <c r="R473">
-        <v>3.88403983784593</v>
+        <v>1.02112006406083</v>
       </c>
       <c r="T473">
-        <v>323.18831342654801</v>
-      </c>
-      <c r="U473">
-        <v>142</v>
-      </c>
-      <c r="V473">
-        <v>185</v>
+        <v>277.70653545614402</v>
       </c>
       <c r="X473">
-        <v>1.5951271639239099E-2</v>
+        <v>0.22649198546697999</v>
       </c>
       <c r="Y473">
-        <v>1.39747809360974E-2</v>
+        <v>0.16600042744176099</v>
       </c>
       <c r="AF473">
         <v>44</v>
@@ -19416,11 +19356,11 @@
       <c r="AK473">
         <v>1810</v>
       </c>
-      <c r="AV473">
-        <v>1.65</v>
-      </c>
-      <c r="AW473">
-        <v>7.05</v>
+      <c r="AP473">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="AQ473">
+        <v>2.3799999999999998E-2</v>
       </c>
     </row>
     <row r="474" spans="1:50" hidden="1">
@@ -19525,7 +19465,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="477" spans="1:50">
+    <row r="477" spans="1:50" hidden="1">
       <c r="A477" s="2" t="s">
         <v>55</v>
       </c>
@@ -19667,7 +19607,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="481" spans="1:50" hidden="1">
+    <row r="481" spans="1:51" hidden="1">
       <c r="A481" s="2" t="s">
         <v>55</v>
       </c>
@@ -19701,7 +19641,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="482" spans="1:50" hidden="1">
+    <row r="482" spans="1:51" hidden="1">
       <c r="A482" s="2" t="s">
         <v>55</v>
       </c>
@@ -19738,7 +19678,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="483" spans="1:50" hidden="1">
+    <row r="483" spans="1:51" hidden="1">
       <c r="A483" t="s">
         <v>55</v>
       </c>
@@ -19781,29 +19721,20 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="484" spans="1:50" hidden="1">
+    <row r="484" spans="1:51">
       <c r="A484" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B484" s="5">
-        <v>35844</v>
+        <v>35858</v>
       </c>
       <c r="C484" s="5"/>
       <c r="D484" s="6">
-        <v>76.612066438067998</v>
+        <v>90.875331564986695</v>
       </c>
       <c r="E484" s="6"/>
       <c r="R484">
-        <v>1.02112006406083</v>
-      </c>
-      <c r="T484">
-        <v>277.70653545614402</v>
-      </c>
-      <c r="X484">
-        <v>0.22649198546697999</v>
-      </c>
-      <c r="Y484">
-        <v>0.16600042744176099</v>
+        <v>1.02442320204191</v>
       </c>
       <c r="AF484">
         <v>44</v>
@@ -19823,14 +19754,8 @@
       <c r="AK484">
         <v>1810</v>
       </c>
-      <c r="AP484">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="AQ484">
-        <v>2.3799999999999998E-2</v>
-      </c>
-    </row>
-    <row r="485" spans="1:50" hidden="1">
+    </row>
+    <row r="485" spans="1:51" hidden="1">
       <c r="A485" s="2" t="s">
         <v>55</v>
       </c>
@@ -19864,7 +19789,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="486" spans="1:50" hidden="1">
+    <row r="486" spans="1:51" hidden="1">
       <c r="A486" s="2" t="s">
         <v>55</v>
       </c>
@@ -19898,7 +19823,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="487" spans="1:50" hidden="1">
+    <row r="487" spans="1:51" hidden="1">
       <c r="A487" s="2" t="s">
         <v>55</v>
       </c>
@@ -19932,7 +19857,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="488" spans="1:50" hidden="1">
+    <row r="488" spans="1:51" hidden="1">
       <c r="A488" s="2" t="s">
         <v>55</v>
       </c>
@@ -19972,7 +19897,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="489" spans="1:50" hidden="1">
+    <row r="489" spans="1:51" hidden="1">
       <c r="A489" t="s">
         <v>55</v>
       </c>
@@ -20006,7 +19931,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="490" spans="1:50" hidden="1">
+    <row r="490" spans="1:51" hidden="1">
       <c r="A490" s="2" t="s">
         <v>55</v>
       </c>
@@ -20043,7 +19968,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="491" spans="1:50" hidden="1">
+    <row r="491" spans="1:51" hidden="1">
       <c r="A491" s="2" t="s">
         <v>55</v>
       </c>
@@ -20080,20 +20005,68 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="492" spans="1:50" hidden="1">
+    <row r="492" spans="1:51">
       <c r="A492" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B492" s="5">
-        <v>35858</v>
-      </c>
-      <c r="C492" s="5"/>
+        <v>35866</v>
+      </c>
+      <c r="C492" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="D492" s="6">
-        <v>90.875331564986695</v>
+        <v>98.832891246684298</v>
       </c>
       <c r="E492" s="6"/>
+      <c r="F492">
+        <v>123</v>
+      </c>
+      <c r="G492">
+        <f>F492*10</f>
+        <v>1230</v>
+      </c>
+      <c r="H492">
+        <v>0.32355522509913598</v>
+      </c>
+      <c r="J492">
+        <v>0.39381852111033294</v>
+      </c>
+      <c r="K492">
+        <v>0.35788138558432403</v>
+      </c>
+      <c r="L492">
+        <v>0.321987986937252</v>
+      </c>
+      <c r="M492">
+        <v>0.33179233729880997</v>
+      </c>
+      <c r="N492">
+        <v>0.31222737345462998</v>
+      </c>
+      <c r="O492">
+        <v>0.29173664567296398</v>
+      </c>
+      <c r="P492">
+        <v>0.31133805691625799</v>
+      </c>
       <c r="R492">
-        <v>1.02442320204191</v>
+        <v>0</v>
+      </c>
+      <c r="U492">
+        <v>117</v>
+      </c>
+      <c r="V492">
+        <v>12</v>
+      </c>
+      <c r="W492">
+        <v>173</v>
+      </c>
+      <c r="AD492">
+        <v>7</v>
+      </c>
+      <c r="AE492">
+        <v>35.6</v>
       </c>
       <c r="AF492">
         <v>44</v>
@@ -20113,8 +20086,35 @@
       <c r="AK492">
         <v>1810</v>
       </c>
-    </row>
-    <row r="493" spans="1:50" hidden="1">
+      <c r="AL492">
+        <v>94</v>
+      </c>
+      <c r="AM492">
+        <v>177</v>
+      </c>
+      <c r="AN492">
+        <v>83</v>
+      </c>
+      <c r="AO492">
+        <v>479</v>
+      </c>
+      <c r="AR492">
+        <v>9.6</v>
+      </c>
+      <c r="AS492">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="AT492">
+        <v>0.72</v>
+      </c>
+      <c r="AU492">
+        <v>0.53</v>
+      </c>
+      <c r="AY492">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="493" spans="1:51" hidden="1">
       <c r="A493" s="2" t="s">
         <v>55</v>
       </c>
@@ -20154,7 +20154,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="494" spans="1:50" hidden="1">
+    <row r="494" spans="1:51" hidden="1">
       <c r="A494" s="2" t="s">
         <v>55</v>
       </c>
@@ -20188,7 +20188,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="495" spans="1:50" hidden="1">
+    <row r="495" spans="1:51" hidden="1">
       <c r="A495" s="2" t="s">
         <v>55</v>
       </c>
@@ -20231,7 +20231,7 @@
         <v>2.78</v>
       </c>
     </row>
-    <row r="496" spans="1:50" hidden="1">
+    <row r="496" spans="1:51" hidden="1">
       <c r="A496" s="2" t="s">
         <v>55</v>
       </c>
@@ -20370,6 +20370,9 @@
         <v>1810</v>
       </c>
     </row>
+    <row r="503" spans="1:37">
+      <c r="H503" s="5"/>
+    </row>
     <row r="505" spans="1:37">
       <c r="H505" s="5"/>
     </row>
@@ -20452,7 +20455,7 @@
       <c r="H531" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AY499" xr:uid="{82957E3C-ACA6-4A6F-B162-5B06AF55FA73}">
+  <autoFilter ref="A1:AY499" xr:uid="{02D4A4B4-9E0C-40E1-812B-A8B29B5ABB76}">
     <filterColumn colId="0">
       <filters>
         <filter val="exp3SowDec17ROCultivarEmerald"/>
@@ -20460,11 +20463,15 @@
         <filter val="exp3SowDec3ROCultivarEmerald"/>
       </filters>
     </filterColumn>
-    <filterColumn colId="25">
+    <filterColumn colId="17">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
       </customFilters>
     </filterColumn>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:AY492">
+      <sortCondition ref="A2:A499"/>
+      <sortCondition ref="D2:D499"/>
+    </sortState>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AY499">
     <sortCondition ref="S2:S499"/>

</xml_diff>

<commit_message>
Thomas Exp done (at least unless Neil has any tips). Jade in TOS is starting to look good (mainly in exp 2)
</commit_message>
<xml_diff>
--- a/Prototypes/Mungbean/Exp3observed.xlsx
+++ b/Prototypes/Mungbean/Exp3observed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pas075\Documents\ApsimX\Prototypes\Mungbean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1D320BC-CE04-46A5-87FF-5F650007DEA8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DFCB21B-B3BC-4DF8-B9DC-8DF7A08C9754}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8C69385E-AA3F-4CF3-AF00-E1E4599E61EE}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8C69385E-AA3F-4CF3-AF00-E1E4599E61EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="1" r:id="rId1"/>
@@ -606,7 +606,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B390" sqref="B390"/>
+      <selection pane="bottomLeft" activeCell="E500" sqref="E500"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -895,7 +895,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="5" spans="1:51">
+    <row r="5" spans="1:51" hidden="1">
       <c r="A5" t="s">
         <v>53</v>
       </c>
@@ -982,7 +982,7 @@
         <v>1873</v>
       </c>
     </row>
-    <row r="7" spans="1:51">
+    <row r="7" spans="1:51" hidden="1">
       <c r="A7" s="2" t="s">
         <v>53</v>
       </c>
@@ -1526,12 +1526,12 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="21" spans="1:47" hidden="1">
+    <row r="21" spans="1:47">
       <c r="A21" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B21" s="5">
-        <v>35863</v>
+        <v>35877</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>45</v>
@@ -3281,12 +3281,12 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="66" spans="1:47" hidden="1">
+    <row r="66" spans="1:47">
       <c r="A66" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B66" s="5">
-        <v>35863</v>
+        <v>35877</v>
       </c>
       <c r="C66" s="5" t="s">
         <v>45</v>
@@ -6695,7 +6695,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="153" spans="1:51">
+    <row r="153" spans="1:51" hidden="1">
       <c r="A153" s="2" t="s">
         <v>53</v>
       </c>
@@ -8013,7 +8013,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="187" spans="1:51" hidden="1">
+    <row r="187" spans="1:51">
       <c r="A187" t="s">
         <v>52</v>
       </c>
@@ -8371,7 +8371,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="192" spans="1:51">
+    <row r="192" spans="1:51" hidden="1">
       <c r="A192" s="2" t="s">
         <v>53</v>
       </c>
@@ -8532,12 +8532,12 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="195" spans="1:51" hidden="1">
+    <row r="195" spans="1:51">
       <c r="A195" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B195" s="5">
-        <v>35858</v>
+        <v>35885</v>
       </c>
       <c r="C195" s="5" t="s">
         <v>45</v>
@@ -8696,7 +8696,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="197" spans="1:51">
+    <row r="197" spans="1:51" hidden="1">
       <c r="A197" s="2" t="s">
         <v>53</v>
       </c>
@@ -10173,12 +10173,12 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="233" spans="1:50" hidden="1">
+    <row r="233" spans="1:50">
       <c r="A233" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B233" s="5">
-        <v>35871</v>
+        <v>35885</v>
       </c>
       <c r="C233" s="5" t="s">
         <v>45</v>
@@ -12229,7 +12229,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="287" spans="1:51">
+    <row r="287" spans="1:51" hidden="1">
       <c r="A287" s="2" t="s">
         <v>54</v>
       </c>
@@ -12565,7 +12565,7 @@
         <v>4.1100000000000003</v>
       </c>
     </row>
-    <row r="296" spans="1:51">
+    <row r="296" spans="1:51" hidden="1">
       <c r="A296" s="2" t="s">
         <v>54</v>
       </c>
@@ -12847,7 +12847,7 @@
         <v>54</v>
       </c>
       <c r="B303" s="5">
-        <v>35858</v>
+        <v>35885</v>
       </c>
       <c r="C303" s="5" t="s">
         <v>45</v>
@@ -14121,12 +14121,12 @@
         <v>1873</v>
       </c>
     </row>
-    <row r="336" spans="1:51" hidden="1">
+    <row r="336" spans="1:51">
       <c r="A336" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B336" s="5">
-        <v>35872</v>
+        <v>35899</v>
       </c>
       <c r="C336" s="5" t="s">
         <v>45</v>
@@ -15936,7 +15936,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="384" spans="1:51">
+    <row r="384" spans="1:51" hidden="1">
       <c r="A384" s="2" t="s">
         <v>54</v>
       </c>
@@ -16155,7 +16155,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="390" spans="1:50">
+    <row r="390" spans="1:50" hidden="1">
       <c r="A390" s="2" t="s">
         <v>54</v>
       </c>
@@ -16641,7 +16641,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="403" spans="1:49">
+    <row r="403" spans="1:49" hidden="1">
       <c r="A403" t="s">
         <v>55</v>
       </c>
@@ -18070,7 +18070,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="441" spans="1:51" hidden="1">
+    <row r="441" spans="1:51">
       <c r="A441" s="2" t="s">
         <v>49</v>
       </c>
@@ -19314,7 +19314,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="473" spans="1:50">
+    <row r="473" spans="1:50" hidden="1">
       <c r="A473" s="2" t="s">
         <v>55</v>
       </c>
@@ -19721,7 +19721,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="484" spans="1:51">
+    <row r="484" spans="1:51" hidden="1">
       <c r="A484" s="2" t="s">
         <v>55</v>
       </c>
@@ -20455,23 +20455,12 @@
       <c r="H531" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AY499" xr:uid="{02D4A4B4-9E0C-40E1-812B-A8B29B5ABB76}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="exp3SowDec17ROCultivarEmerald"/>
-        <filter val="exp3SowDec30ROCultivarEmerald"/>
-        <filter val="exp3SowDec3ROCultivarEmerald"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="17">
+  <autoFilter ref="A1:AY499" xr:uid="{1600DBA9-BC42-4CBE-895C-5637B5C9DC9F}">
+    <filterColumn colId="2">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
       </customFilters>
     </filterColumn>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:AY492">
-      <sortCondition ref="A2:A499"/>
-      <sortCondition ref="D2:D499"/>
-    </sortState>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AY499">
     <sortCondition ref="S2:S499"/>

</xml_diff>